<commit_message>
Good work on AL formater
</commit_message>
<xml_diff>
--- a/Sample Tables/Sample Crosstab.xlsx
+++ b/Sample Tables/Sample Crosstab.xlsx
@@ -17,7 +17,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="938" uniqueCount="266">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="897" uniqueCount="261">
   <si>
     <t>Analysis</t>
   </si>
@@ -799,30 +799,14 @@
     <t>SGS Engage --- Sample Crosstab</t>
   </si>
   <si>
-    <t>Sample Comments</t>
-  </si>
-  <si>
-    <t>Client Sample Id</t>
-  </si>
-  <si>
-    <t>Lab Sample Id</t>
-  </si>
-  <si>
-    <t>Comments</t>
-  </si>
-  <si>
-    <t>8260C - Surrogate recoveries for toluene-d8 (121%), and 4-bromofluorobenzene (157%) do not meet QC criteria due to matrix interference
-AK101 - Surrogate recovery for 4-bromofluorobenzene ( 19000 %) does not meet QC criteria due to matrix interference.</t>
-  </si>
-  <si>
-    <t>8270D SIM - The PAH LOQs are elevated due to sample dilution (5X). The sample was diluted due to the dark color of the extract.</t>
+    <t>Action Level</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <fonts count="8" x14ac:knownFonts="1">
+  <fonts count="6" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <name val="Calibri"/>
@@ -830,41 +814,35 @@
     <font>
       <sz val="10"/>
       <name val="Arial"/>
+      <family val="2"/>
     </font>
     <font>
       <sz val="10"/>
       <color rgb="FFFFFFFF"/>
       <name val="Arial"/>
+      <family val="2"/>
     </font>
     <font>
       <b/>
       <sz val="10"/>
       <name val="Arial"/>
+      <family val="2"/>
     </font>
     <font>
       <b/>
       <sz val="10"/>
       <color rgb="FFFFFFFF"/>
       <name val="Arial"/>
+      <family val="2"/>
     </font>
     <font>
       <sz val="12"/>
       <color indexed="12"/>
       <name val="Arial"/>
-    </font>
-    <font>
-      <b/>
-      <sz val="10"/>
-      <color rgb="FF000000"/>
-      <name val="Arial"/>
-    </font>
-    <font>
-      <sz val="10"/>
-      <color rgb="FF000000"/>
-      <name val="Arial"/>
+      <family val="2"/>
     </font>
   </fonts>
-  <fills count="5">
+  <fills count="4">
     <fill>
       <patternFill patternType="none"/>
     </fill>
@@ -883,14 +861,8 @@
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor rgb="FFFFFFFF"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
   </fills>
-  <borders count="3">
+  <borders count="4">
     <border>
       <left/>
       <right/>
@@ -932,6 +904,21 @@
         <color indexed="0"/>
       </diagonal>
     </border>
+    <border>
+      <left style="thin">
+        <color indexed="64"/>
+      </left>
+      <right style="thin">
+        <color indexed="64"/>
+      </right>
+      <top style="thin">
+        <color indexed="64"/>
+      </top>
+      <bottom style="thin">
+        <color indexed="64"/>
+      </bottom>
+      <diagonal/>
+    </border>
   </borders>
   <cellStyleXfs count="3">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
@@ -942,7 +929,7 @@
       <alignment horizontal="center" vertical="center"/>
     </xf>
   </cellStyleXfs>
-  <cellXfs count="13">
+  <cellXfs count="9">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="1" xfId="1">
       <alignment horizontal="center" vertical="center"/>
@@ -959,25 +946,13 @@
     <xf numFmtId="0" fontId="1" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="4" fillId="2" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="7" fillId="4" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="7" fillId="4" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    <xf numFmtId="0" fontId="4" fillId="2" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="5" fillId="3" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="6" fillId="4" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="2" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
   </cellXfs>
@@ -1328,166 +1303,167 @@
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <sheetPr codeName="Sheet1"/>
-  <dimension ref="A1:S54"/>
+  <dimension ref="A1:T49"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
       <pane ySplit="7" topLeftCell="A8" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" sqref="A1:F1"/>
+      <selection pane="bottomLeft" activeCell="C48" sqref="C48"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="9.140625" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
     <col min="1" max="1" width="17.140625" customWidth="1"/>
     <col min="2" max="2" width="25.85546875" customWidth="1"/>
-    <col min="3" max="3" width="25.7109375" customWidth="1"/>
-    <col min="4" max="19" width="21" customWidth="1"/>
+    <col min="3" max="4" width="25.7109375" customWidth="1"/>
+    <col min="5" max="20" width="21" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:19" ht="38.1" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A1" s="10" t="s">
+    <row r="1" spans="1:20" ht="38.1" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A1" s="8" t="s">
         <v>259</v>
       </c>
-      <c r="B1" s="10" t="s">
+      <c r="B1" s="8" t="s">
         <v>259</v>
       </c>
-      <c r="C1" s="10" t="s">
+      <c r="C1" s="8" t="s">
         <v>259</v>
       </c>
-      <c r="D1" s="10" t="s">
+      <c r="D1" s="8"/>
+      <c r="E1" s="8" t="s">
         <v>259</v>
       </c>
-      <c r="E1" s="10" t="s">
+      <c r="F1" s="8" t="s">
         <v>259</v>
       </c>
-      <c r="F1" s="10" t="s">
+      <c r="G1" s="8" t="s">
         <v>259</v>
       </c>
     </row>
-    <row r="2" spans="1:19" x14ac:dyDescent="0.25">
-      <c r="A2" s="9" t="s">
+    <row r="2" spans="1:20" x14ac:dyDescent="0.25">
+      <c r="A2" s="7" t="s">
         <v>217</v>
       </c>
-      <c r="B2" s="9" t="s">
+      <c r="B2" s="7" t="s">
         <v>217</v>
       </c>
       <c r="C2" s="4" t="s">
         <v>219</v>
       </c>
-      <c r="D2" s="5" t="s">
+      <c r="D2" s="4"/>
+      <c r="E2" s="5" t="s">
         <v>224</v>
       </c>
-      <c r="E2" s="5" t="s">
+      <c r="F2" s="5" t="s">
         <v>228</v>
       </c>
-      <c r="F2" s="5" t="s">
+      <c r="G2" s="5" t="s">
         <v>230</v>
       </c>
-      <c r="G2" s="5" t="s">
+      <c r="H2" s="5" t="s">
         <v>232</v>
       </c>
-      <c r="H2" s="5" t="s">
+      <c r="I2" s="5" t="s">
         <v>234</v>
       </c>
-      <c r="I2" s="5" t="s">
+      <c r="J2" s="5" t="s">
         <v>236</v>
       </c>
-      <c r="J2" s="5" t="s">
+      <c r="K2" s="5" t="s">
         <v>238</v>
       </c>
-      <c r="K2" s="5" t="s">
+      <c r="L2" s="5" t="s">
         <v>240</v>
       </c>
-      <c r="L2" s="5" t="s">
+      <c r="M2" s="5" t="s">
         <v>242</v>
       </c>
-      <c r="M2" s="5" t="s">
+      <c r="N2" s="5" t="s">
         <v>244</v>
       </c>
-      <c r="N2" s="5" t="s">
+      <c r="O2" s="5" t="s">
         <v>246</v>
       </c>
-      <c r="O2" s="5" t="s">
+      <c r="P2" s="5" t="s">
         <v>248</v>
       </c>
-      <c r="P2" s="5" t="s">
+      <c r="Q2" s="5" t="s">
         <v>250</v>
       </c>
-      <c r="Q2" s="5" t="s">
+      <c r="R2" s="5" t="s">
         <v>252</v>
       </c>
-      <c r="R2" s="5" t="s">
+      <c r="S2" s="5" t="s">
         <v>254</v>
       </c>
-      <c r="S2" s="5" t="s">
+      <c r="T2" s="5" t="s">
         <v>256</v>
       </c>
     </row>
-    <row r="3" spans="1:19" x14ac:dyDescent="0.25">
-      <c r="A3" s="9" t="s">
+    <row r="3" spans="1:20" x14ac:dyDescent="0.25">
+      <c r="A3" s="7" t="s">
         <v>218</v>
       </c>
-      <c r="B3" s="9" t="s">
+      <c r="B3" s="7" t="s">
         <v>218</v>
       </c>
       <c r="C3" s="4" t="s">
         <v>220</v>
       </c>
-      <c r="D3" s="5" t="s">
+      <c r="D3" s="4"/>
+      <c r="E3" s="5" t="s">
         <v>3</v>
       </c>
-      <c r="E3" s="5" t="s">
+      <c r="F3" s="5" t="s">
         <v>4</v>
       </c>
-      <c r="F3" s="5" t="s">
+      <c r="G3" s="5" t="s">
         <v>5</v>
       </c>
-      <c r="G3" s="5" t="s">
+      <c r="H3" s="5" t="s">
         <v>6</v>
       </c>
-      <c r="H3" s="5" t="s">
+      <c r="I3" s="5" t="s">
         <v>7</v>
       </c>
-      <c r="I3" s="5" t="s">
+      <c r="J3" s="5" t="s">
         <v>8</v>
       </c>
-      <c r="J3" s="5" t="s">
+      <c r="K3" s="5" t="s">
         <v>9</v>
       </c>
-      <c r="K3" s="5" t="s">
+      <c r="L3" s="5" t="s">
         <v>10</v>
       </c>
-      <c r="L3" s="5" t="s">
+      <c r="M3" s="5" t="s">
         <v>11</v>
       </c>
-      <c r="M3" s="5" t="s">
+      <c r="N3" s="5" t="s">
         <v>12</v>
       </c>
-      <c r="N3" s="5" t="s">
+      <c r="O3" s="5" t="s">
         <v>13</v>
       </c>
-      <c r="O3" s="5" t="s">
+      <c r="P3" s="5" t="s">
         <v>14</v>
       </c>
-      <c r="P3" s="5" t="s">
+      <c r="Q3" s="5" t="s">
         <v>15</v>
       </c>
-      <c r="Q3" s="5" t="s">
+      <c r="R3" s="5" t="s">
         <v>16</v>
       </c>
-      <c r="R3" s="5" t="s">
+      <c r="S3" s="5" t="s">
         <v>17</v>
       </c>
-      <c r="S3" s="5" t="s">
+      <c r="T3" s="5" t="s">
         <v>18</v>
       </c>
     </row>
-    <row r="4" spans="1:19" x14ac:dyDescent="0.25">
+    <row r="4" spans="1:20" x14ac:dyDescent="0.25">
       <c r="C4" s="4" t="s">
         <v>221</v>
       </c>
-      <c r="D4" s="5" t="s">
-        <v>225</v>
-      </c>
+      <c r="D4" s="4"/>
       <c r="E4" s="5" t="s">
         <v>225</v>
       </c>
@@ -1533,14 +1509,15 @@
       <c r="S4" s="5" t="s">
         <v>225</v>
       </c>
-    </row>
-    <row r="5" spans="1:19" x14ac:dyDescent="0.25">
+      <c r="T4" s="5" t="s">
+        <v>225</v>
+      </c>
+    </row>
+    <row r="5" spans="1:20" x14ac:dyDescent="0.25">
       <c r="C5" s="4" t="s">
         <v>222</v>
       </c>
-      <c r="D5" s="5" t="s">
-        <v>226</v>
-      </c>
+      <c r="D5" s="4"/>
       <c r="E5" s="5" t="s">
         <v>226</v>
       </c>
@@ -1584,63 +1561,67 @@
         <v>226</v>
       </c>
       <c r="S5" s="5" t="s">
+        <v>226</v>
+      </c>
+      <c r="T5" s="5" t="s">
         <v>257</v>
       </c>
     </row>
-    <row r="6" spans="1:19" x14ac:dyDescent="0.25">
+    <row r="6" spans="1:20" x14ac:dyDescent="0.25">
       <c r="C6" s="4" t="s">
         <v>223</v>
       </c>
-      <c r="D6" s="5" t="s">
+      <c r="D6" s="4"/>
+      <c r="E6" s="5" t="s">
         <v>227</v>
       </c>
-      <c r="E6" s="5" t="s">
+      <c r="F6" s="5" t="s">
         <v>229</v>
       </c>
-      <c r="F6" s="5" t="s">
+      <c r="G6" s="5" t="s">
         <v>231</v>
       </c>
-      <c r="G6" s="5" t="s">
+      <c r="H6" s="5" t="s">
         <v>233</v>
       </c>
-      <c r="H6" s="5" t="s">
+      <c r="I6" s="5" t="s">
         <v>235</v>
       </c>
-      <c r="I6" s="5" t="s">
+      <c r="J6" s="5" t="s">
         <v>237</v>
       </c>
-      <c r="J6" s="5" t="s">
+      <c r="K6" s="5" t="s">
         <v>239</v>
       </c>
-      <c r="K6" s="5" t="s">
+      <c r="L6" s="5" t="s">
         <v>241</v>
       </c>
-      <c r="L6" s="5" t="s">
+      <c r="M6" s="5" t="s">
         <v>243</v>
       </c>
-      <c r="M6" s="5" t="s">
+      <c r="N6" s="5" t="s">
         <v>245</v>
       </c>
-      <c r="N6" s="5" t="s">
+      <c r="O6" s="5" t="s">
         <v>247</v>
       </c>
-      <c r="O6" s="5" t="s">
+      <c r="P6" s="5" t="s">
         <v>249</v>
       </c>
-      <c r="P6" s="5" t="s">
+      <c r="Q6" s="5" t="s">
         <v>251</v>
       </c>
-      <c r="Q6" s="5" t="s">
+      <c r="R6" s="5" t="s">
         <v>253</v>
       </c>
-      <c r="R6" s="5" t="s">
+      <c r="S6" s="5" t="s">
         <v>255</v>
       </c>
-      <c r="S6" s="5" t="s">
+      <c r="T6" s="5" t="s">
         <v>258</v>
       </c>
     </row>
-    <row r="7" spans="1:19" x14ac:dyDescent="0.25">
+    <row r="7" spans="1:20" x14ac:dyDescent="0.25">
       <c r="A7" s="3" t="s">
         <v>0</v>
       </c>
@@ -1650,7 +1631,9 @@
       <c r="C7" s="3" t="s">
         <v>2</v>
       </c>
-      <c r="D7" s="2"/>
+      <c r="D7" s="6" t="s">
+        <v>260</v>
+      </c>
       <c r="E7" s="2"/>
       <c r="F7" s="2"/>
       <c r="G7" s="2"/>
@@ -1666,8 +1649,9 @@
       <c r="Q7" s="2"/>
       <c r="R7" s="2"/>
       <c r="S7" s="2"/>
-    </row>
-    <row r="8" spans="1:19" x14ac:dyDescent="0.25">
+      <c r="T7" s="2"/>
+    </row>
+    <row r="8" spans="1:20" x14ac:dyDescent="0.25">
       <c r="A8" s="1" t="s">
         <v>19</v>
       </c>
@@ -1677,15 +1661,13 @@
       <c r="C8" s="1" t="s">
         <v>21</v>
       </c>
-      <c r="D8" s="1" t="s">
-        <v>22</v>
-      </c>
+      <c r="D8" s="1"/>
       <c r="E8" s="1" t="s">
+        <v>22</v>
+      </c>
+      <c r="F8" s="1" t="s">
         <v>23</v>
       </c>
-      <c r="F8" s="1" t="s">
-        <v>22</v>
-      </c>
       <c r="G8" s="1" t="s">
         <v>22</v>
       </c>
@@ -1702,11 +1684,11 @@
         <v>22</v>
       </c>
       <c r="L8" s="1" t="s">
+        <v>22</v>
+      </c>
+      <c r="M8" s="1" t="s">
         <v>24</v>
       </c>
-      <c r="M8" s="1" t="s">
-        <v>22</v>
-      </c>
       <c r="N8" s="1" t="s">
         <v>22</v>
       </c>
@@ -1725,8 +1707,11 @@
       <c r="S8" s="1" t="s">
         <v>22</v>
       </c>
-    </row>
-    <row r="9" spans="1:19" x14ac:dyDescent="0.25">
+      <c r="T8" s="1" t="s">
+        <v>22</v>
+      </c>
+    </row>
+    <row r="9" spans="1:20" x14ac:dyDescent="0.25">
       <c r="A9" s="1" t="s">
         <v>19</v>
       </c>
@@ -1736,15 +1721,13 @@
       <c r="C9" s="1" t="s">
         <v>21</v>
       </c>
-      <c r="D9" s="1" t="s">
-        <v>22</v>
-      </c>
+      <c r="D9" s="1"/>
       <c r="E9" s="1" t="s">
+        <v>22</v>
+      </c>
+      <c r="F9" s="1" t="s">
         <v>23</v>
       </c>
-      <c r="F9" s="1" t="s">
-        <v>22</v>
-      </c>
       <c r="G9" s="1" t="s">
         <v>22</v>
       </c>
@@ -1761,11 +1744,11 @@
         <v>22</v>
       </c>
       <c r="L9" s="1" t="s">
+        <v>22</v>
+      </c>
+      <c r="M9" s="1" t="s">
         <v>26</v>
       </c>
-      <c r="M9" s="1" t="s">
-        <v>22</v>
-      </c>
       <c r="N9" s="1" t="s">
         <v>22</v>
       </c>
@@ -1784,8 +1767,11 @@
       <c r="S9" s="1" t="s">
         <v>22</v>
       </c>
-    </row>
-    <row r="10" spans="1:19" x14ac:dyDescent="0.25">
+      <c r="T9" s="1" t="s">
+        <v>22</v>
+      </c>
+    </row>
+    <row r="10" spans="1:20" x14ac:dyDescent="0.25">
       <c r="A10" s="1" t="s">
         <v>19</v>
       </c>
@@ -1795,15 +1781,13 @@
       <c r="C10" s="1" t="s">
         <v>21</v>
       </c>
-      <c r="D10" s="1" t="s">
-        <v>22</v>
-      </c>
+      <c r="D10" s="1"/>
       <c r="E10" s="1" t="s">
+        <v>22</v>
+      </c>
+      <c r="F10" s="1" t="s">
         <v>23</v>
       </c>
-      <c r="F10" s="1" t="s">
-        <v>22</v>
-      </c>
       <c r="G10" s="1" t="s">
         <v>22</v>
       </c>
@@ -1820,11 +1804,11 @@
         <v>22</v>
       </c>
       <c r="L10" s="1" t="s">
+        <v>22</v>
+      </c>
+      <c r="M10" s="1" t="s">
         <v>28</v>
       </c>
-      <c r="M10" s="1" t="s">
-        <v>22</v>
-      </c>
       <c r="N10" s="1" t="s">
         <v>22</v>
       </c>
@@ -1843,8 +1827,11 @@
       <c r="S10" s="1" t="s">
         <v>22</v>
       </c>
-    </row>
-    <row r="11" spans="1:19" x14ac:dyDescent="0.25">
+      <c r="T10" s="1" t="s">
+        <v>22</v>
+      </c>
+    </row>
+    <row r="11" spans="1:20" x14ac:dyDescent="0.25">
       <c r="A11" s="1" t="s">
         <v>19</v>
       </c>
@@ -1854,15 +1841,13 @@
       <c r="C11" s="1" t="s">
         <v>21</v>
       </c>
-      <c r="D11" s="1" t="s">
-        <v>22</v>
-      </c>
+      <c r="D11" s="1"/>
       <c r="E11" s="1" t="s">
+        <v>22</v>
+      </c>
+      <c r="F11" s="1" t="s">
         <v>23</v>
       </c>
-      <c r="F11" s="1" t="s">
-        <v>22</v>
-      </c>
       <c r="G11" s="1" t="s">
         <v>22</v>
       </c>
@@ -1879,11 +1864,11 @@
         <v>22</v>
       </c>
       <c r="L11" s="1" t="s">
+        <v>22</v>
+      </c>
+      <c r="M11" s="1" t="s">
         <v>30</v>
       </c>
-      <c r="M11" s="1" t="s">
-        <v>22</v>
-      </c>
       <c r="N11" s="1" t="s">
         <v>22</v>
       </c>
@@ -1902,8 +1887,11 @@
       <c r="S11" s="1" t="s">
         <v>22</v>
       </c>
-    </row>
-    <row r="12" spans="1:19" x14ac:dyDescent="0.25">
+      <c r="T11" s="1" t="s">
+        <v>22</v>
+      </c>
+    </row>
+    <row r="12" spans="1:20" x14ac:dyDescent="0.25">
       <c r="A12" s="1" t="s">
         <v>19</v>
       </c>
@@ -1913,15 +1901,13 @@
       <c r="C12" s="1" t="s">
         <v>21</v>
       </c>
-      <c r="D12" s="1" t="s">
-        <v>22</v>
-      </c>
+      <c r="D12" s="1"/>
       <c r="E12" s="1" t="s">
+        <v>22</v>
+      </c>
+      <c r="F12" s="1" t="s">
         <v>23</v>
       </c>
-      <c r="F12" s="1" t="s">
-        <v>22</v>
-      </c>
       <c r="G12" s="1" t="s">
         <v>22</v>
       </c>
@@ -1938,11 +1924,11 @@
         <v>22</v>
       </c>
       <c r="L12" s="1" t="s">
+        <v>22</v>
+      </c>
+      <c r="M12" s="1" t="s">
         <v>30</v>
       </c>
-      <c r="M12" s="1" t="s">
-        <v>22</v>
-      </c>
       <c r="N12" s="1" t="s">
         <v>22</v>
       </c>
@@ -1961,8 +1947,11 @@
       <c r="S12" s="1" t="s">
         <v>22</v>
       </c>
-    </row>
-    <row r="13" spans="1:19" x14ac:dyDescent="0.25">
+      <c r="T12" s="1" t="s">
+        <v>22</v>
+      </c>
+    </row>
+    <row r="13" spans="1:20" x14ac:dyDescent="0.25">
       <c r="A13" s="1" t="s">
         <v>19</v>
       </c>
@@ -1972,15 +1961,13 @@
       <c r="C13" s="1" t="s">
         <v>21</v>
       </c>
-      <c r="D13" s="1" t="s">
-        <v>22</v>
-      </c>
+      <c r="D13" s="1"/>
       <c r="E13" s="1" t="s">
+        <v>22</v>
+      </c>
+      <c r="F13" s="1" t="s">
         <v>23</v>
       </c>
-      <c r="F13" s="1" t="s">
-        <v>22</v>
-      </c>
       <c r="G13" s="1" t="s">
         <v>22</v>
       </c>
@@ -1997,11 +1984,11 @@
         <v>22</v>
       </c>
       <c r="L13" s="1" t="s">
+        <v>22</v>
+      </c>
+      <c r="M13" s="1" t="s">
         <v>30</v>
       </c>
-      <c r="M13" s="1" t="s">
-        <v>22</v>
-      </c>
       <c r="N13" s="1" t="s">
         <v>22</v>
       </c>
@@ -2020,8 +2007,11 @@
       <c r="S13" s="1" t="s">
         <v>22</v>
       </c>
-    </row>
-    <row r="14" spans="1:19" x14ac:dyDescent="0.25">
+      <c r="T13" s="1" t="s">
+        <v>22</v>
+      </c>
+    </row>
+    <row r="14" spans="1:20" x14ac:dyDescent="0.25">
       <c r="A14" s="1" t="s">
         <v>19</v>
       </c>
@@ -2031,15 +2021,13 @@
       <c r="C14" s="1" t="s">
         <v>21</v>
       </c>
-      <c r="D14" s="1" t="s">
-        <v>22</v>
-      </c>
+      <c r="D14" s="1"/>
       <c r="E14" s="1" t="s">
+        <v>22</v>
+      </c>
+      <c r="F14" s="1" t="s">
         <v>23</v>
       </c>
-      <c r="F14" s="1" t="s">
-        <v>22</v>
-      </c>
       <c r="G14" s="1" t="s">
         <v>22</v>
       </c>
@@ -2056,11 +2044,11 @@
         <v>22</v>
       </c>
       <c r="L14" s="1" t="s">
+        <v>22</v>
+      </c>
+      <c r="M14" s="1" t="s">
         <v>30</v>
       </c>
-      <c r="M14" s="1" t="s">
-        <v>22</v>
-      </c>
       <c r="N14" s="1" t="s">
         <v>22</v>
       </c>
@@ -2079,8 +2067,11 @@
       <c r="S14" s="1" t="s">
         <v>22</v>
       </c>
-    </row>
-    <row r="15" spans="1:19" x14ac:dyDescent="0.25">
+      <c r="T14" s="1" t="s">
+        <v>22</v>
+      </c>
+    </row>
+    <row r="15" spans="1:20" x14ac:dyDescent="0.25">
       <c r="A15" s="1" t="s">
         <v>19</v>
       </c>
@@ -2090,15 +2081,13 @@
       <c r="C15" s="1" t="s">
         <v>21</v>
       </c>
-      <c r="D15" s="1" t="s">
-        <v>22</v>
-      </c>
+      <c r="D15" s="1"/>
       <c r="E15" s="1" t="s">
+        <v>22</v>
+      </c>
+      <c r="F15" s="1" t="s">
         <v>23</v>
       </c>
-      <c r="F15" s="1" t="s">
-        <v>22</v>
-      </c>
       <c r="G15" s="1" t="s">
         <v>22</v>
       </c>
@@ -2115,11 +2104,11 @@
         <v>22</v>
       </c>
       <c r="L15" s="1" t="s">
+        <v>22</v>
+      </c>
+      <c r="M15" s="1" t="s">
         <v>30</v>
       </c>
-      <c r="M15" s="1" t="s">
-        <v>22</v>
-      </c>
       <c r="N15" s="1" t="s">
         <v>22</v>
       </c>
@@ -2138,8 +2127,11 @@
       <c r="S15" s="1" t="s">
         <v>22</v>
       </c>
-    </row>
-    <row r="16" spans="1:19" x14ac:dyDescent="0.25">
+      <c r="T15" s="1" t="s">
+        <v>22</v>
+      </c>
+    </row>
+    <row r="16" spans="1:20" x14ac:dyDescent="0.25">
       <c r="A16" s="1" t="s">
         <v>19</v>
       </c>
@@ -2149,15 +2141,13 @@
       <c r="C16" s="1" t="s">
         <v>21</v>
       </c>
-      <c r="D16" s="1" t="s">
-        <v>22</v>
-      </c>
+      <c r="D16" s="1"/>
       <c r="E16" s="1" t="s">
+        <v>22</v>
+      </c>
+      <c r="F16" s="1" t="s">
         <v>23</v>
       </c>
-      <c r="F16" s="1" t="s">
-        <v>22</v>
-      </c>
       <c r="G16" s="1" t="s">
         <v>22</v>
       </c>
@@ -2174,11 +2164,11 @@
         <v>22</v>
       </c>
       <c r="L16" s="1" t="s">
+        <v>22</v>
+      </c>
+      <c r="M16" s="1" t="s">
         <v>30</v>
       </c>
-      <c r="M16" s="1" t="s">
-        <v>22</v>
-      </c>
       <c r="N16" s="1" t="s">
         <v>22</v>
       </c>
@@ -2197,8 +2187,11 @@
       <c r="S16" s="1" t="s">
         <v>22</v>
       </c>
-    </row>
-    <row r="17" spans="1:19" x14ac:dyDescent="0.25">
+      <c r="T16" s="1" t="s">
+        <v>22</v>
+      </c>
+    </row>
+    <row r="17" spans="1:20" x14ac:dyDescent="0.25">
       <c r="A17" s="1" t="s">
         <v>19</v>
       </c>
@@ -2208,15 +2201,13 @@
       <c r="C17" s="1" t="s">
         <v>21</v>
       </c>
-      <c r="D17" s="1" t="s">
-        <v>22</v>
-      </c>
+      <c r="D17" s="1"/>
       <c r="E17" s="1" t="s">
+        <v>22</v>
+      </c>
+      <c r="F17" s="1" t="s">
         <v>23</v>
       </c>
-      <c r="F17" s="1" t="s">
-        <v>22</v>
-      </c>
       <c r="G17" s="1" t="s">
         <v>22</v>
       </c>
@@ -2233,11 +2224,11 @@
         <v>22</v>
       </c>
       <c r="L17" s="1" t="s">
+        <v>22</v>
+      </c>
+      <c r="M17" s="1" t="s">
         <v>30</v>
       </c>
-      <c r="M17" s="1" t="s">
-        <v>22</v>
-      </c>
       <c r="N17" s="1" t="s">
         <v>22</v>
       </c>
@@ -2256,8 +2247,11 @@
       <c r="S17" s="1" t="s">
         <v>22</v>
       </c>
-    </row>
-    <row r="18" spans="1:19" x14ac:dyDescent="0.25">
+      <c r="T17" s="1" t="s">
+        <v>22</v>
+      </c>
+    </row>
+    <row r="18" spans="1:20" x14ac:dyDescent="0.25">
       <c r="A18" s="1" t="s">
         <v>19</v>
       </c>
@@ -2267,15 +2261,13 @@
       <c r="C18" s="1" t="s">
         <v>21</v>
       </c>
-      <c r="D18" s="1" t="s">
-        <v>22</v>
-      </c>
+      <c r="D18" s="1"/>
       <c r="E18" s="1" t="s">
+        <v>22</v>
+      </c>
+      <c r="F18" s="1" t="s">
         <v>23</v>
       </c>
-      <c r="F18" s="1" t="s">
-        <v>22</v>
-      </c>
       <c r="G18" s="1" t="s">
         <v>22</v>
       </c>
@@ -2292,11 +2284,11 @@
         <v>22</v>
       </c>
       <c r="L18" s="1" t="s">
+        <v>22</v>
+      </c>
+      <c r="M18" s="1" t="s">
         <v>30</v>
       </c>
-      <c r="M18" s="1" t="s">
-        <v>22</v>
-      </c>
       <c r="N18" s="1" t="s">
         <v>22</v>
       </c>
@@ -2315,8 +2307,11 @@
       <c r="S18" s="1" t="s">
         <v>22</v>
       </c>
-    </row>
-    <row r="19" spans="1:19" x14ac:dyDescent="0.25">
+      <c r="T18" s="1" t="s">
+        <v>22</v>
+      </c>
+    </row>
+    <row r="19" spans="1:20" x14ac:dyDescent="0.25">
       <c r="A19" s="1" t="s">
         <v>19</v>
       </c>
@@ -2326,15 +2321,13 @@
       <c r="C19" s="1" t="s">
         <v>21</v>
       </c>
-      <c r="D19" s="1" t="s">
-        <v>22</v>
-      </c>
+      <c r="D19" s="1"/>
       <c r="E19" s="1" t="s">
+        <v>22</v>
+      </c>
+      <c r="F19" s="1" t="s">
         <v>23</v>
       </c>
-      <c r="F19" s="1" t="s">
-        <v>22</v>
-      </c>
       <c r="G19" s="1" t="s">
         <v>22</v>
       </c>
@@ -2351,11 +2344,11 @@
         <v>22</v>
       </c>
       <c r="L19" s="1" t="s">
+        <v>22</v>
+      </c>
+      <c r="M19" s="1" t="s">
         <v>30</v>
       </c>
-      <c r="M19" s="1" t="s">
-        <v>22</v>
-      </c>
       <c r="N19" s="1" t="s">
         <v>22</v>
       </c>
@@ -2374,8 +2367,11 @@
       <c r="S19" s="1" t="s">
         <v>22</v>
       </c>
-    </row>
-    <row r="20" spans="1:19" x14ac:dyDescent="0.25">
+      <c r="T19" s="1" t="s">
+        <v>22</v>
+      </c>
+    </row>
+    <row r="20" spans="1:20" x14ac:dyDescent="0.25">
       <c r="A20" s="1" t="s">
         <v>19</v>
       </c>
@@ -2385,15 +2381,13 @@
       <c r="C20" s="1" t="s">
         <v>21</v>
       </c>
-      <c r="D20" s="1" t="s">
-        <v>22</v>
-      </c>
+      <c r="D20" s="1"/>
       <c r="E20" s="1" t="s">
+        <v>22</v>
+      </c>
+      <c r="F20" s="1" t="s">
         <v>23</v>
       </c>
-      <c r="F20" s="1" t="s">
-        <v>22</v>
-      </c>
       <c r="G20" s="1" t="s">
         <v>22</v>
       </c>
@@ -2410,11 +2404,11 @@
         <v>22</v>
       </c>
       <c r="L20" s="1" t="s">
+        <v>22</v>
+      </c>
+      <c r="M20" s="1" t="s">
         <v>30</v>
       </c>
-      <c r="M20" s="1" t="s">
-        <v>22</v>
-      </c>
       <c r="N20" s="1" t="s">
         <v>22</v>
       </c>
@@ -2433,8 +2427,11 @@
       <c r="S20" s="1" t="s">
         <v>22</v>
       </c>
-    </row>
-    <row r="21" spans="1:19" x14ac:dyDescent="0.25">
+      <c r="T20" s="1" t="s">
+        <v>22</v>
+      </c>
+    </row>
+    <row r="21" spans="1:20" x14ac:dyDescent="0.25">
       <c r="A21" s="1" t="s">
         <v>19</v>
       </c>
@@ -2444,15 +2441,13 @@
       <c r="C21" s="1" t="s">
         <v>21</v>
       </c>
-      <c r="D21" s="1" t="s">
-        <v>22</v>
-      </c>
+      <c r="D21" s="1"/>
       <c r="E21" s="1" t="s">
+        <v>22</v>
+      </c>
+      <c r="F21" s="1" t="s">
         <v>23</v>
       </c>
-      <c r="F21" s="1" t="s">
-        <v>22</v>
-      </c>
       <c r="G21" s="1" t="s">
         <v>22</v>
       </c>
@@ -2469,11 +2464,11 @@
         <v>22</v>
       </c>
       <c r="L21" s="1" t="s">
+        <v>22</v>
+      </c>
+      <c r="M21" s="1" t="s">
         <v>41</v>
       </c>
-      <c r="M21" s="1" t="s">
-        <v>22</v>
-      </c>
       <c r="N21" s="1" t="s">
         <v>22</v>
       </c>
@@ -2492,8 +2487,11 @@
       <c r="S21" s="1" t="s">
         <v>22</v>
       </c>
-    </row>
-    <row r="22" spans="1:19" x14ac:dyDescent="0.25">
+      <c r="T21" s="1" t="s">
+        <v>22</v>
+      </c>
+    </row>
+    <row r="22" spans="1:20" x14ac:dyDescent="0.25">
       <c r="A22" s="1" t="s">
         <v>19</v>
       </c>
@@ -2503,15 +2501,13 @@
       <c r="C22" s="1" t="s">
         <v>21</v>
       </c>
-      <c r="D22" s="1" t="s">
-        <v>22</v>
-      </c>
+      <c r="D22" s="1"/>
       <c r="E22" s="1" t="s">
+        <v>22</v>
+      </c>
+      <c r="F22" s="1" t="s">
         <v>23</v>
       </c>
-      <c r="F22" s="1" t="s">
-        <v>22</v>
-      </c>
       <c r="G22" s="1" t="s">
         <v>22</v>
       </c>
@@ -2528,11 +2524,11 @@
         <v>22</v>
       </c>
       <c r="L22" s="1" t="s">
+        <v>22</v>
+      </c>
+      <c r="M22" s="1" t="s">
         <v>30</v>
       </c>
-      <c r="M22" s="1" t="s">
-        <v>22</v>
-      </c>
       <c r="N22" s="1" t="s">
         <v>22</v>
       </c>
@@ -2551,8 +2547,11 @@
       <c r="S22" s="1" t="s">
         <v>22</v>
       </c>
-    </row>
-    <row r="23" spans="1:19" x14ac:dyDescent="0.25">
+      <c r="T22" s="1" t="s">
+        <v>22</v>
+      </c>
+    </row>
+    <row r="23" spans="1:20" x14ac:dyDescent="0.25">
       <c r="A23" s="1" t="s">
         <v>19</v>
       </c>
@@ -2562,15 +2561,13 @@
       <c r="C23" s="1" t="s">
         <v>21</v>
       </c>
-      <c r="D23" s="1" t="s">
-        <v>22</v>
-      </c>
+      <c r="D23" s="1"/>
       <c r="E23" s="1" t="s">
+        <v>22</v>
+      </c>
+      <c r="F23" s="1" t="s">
         <v>44</v>
       </c>
-      <c r="F23" s="1" t="s">
-        <v>22</v>
-      </c>
       <c r="G23" s="1" t="s">
         <v>22</v>
       </c>
@@ -2587,11 +2584,11 @@
         <v>22</v>
       </c>
       <c r="L23" s="1" t="s">
+        <v>22</v>
+      </c>
+      <c r="M23" s="1" t="s">
         <v>45</v>
       </c>
-      <c r="M23" s="1" t="s">
-        <v>22</v>
-      </c>
       <c r="N23" s="1" t="s">
         <v>22</v>
       </c>
@@ -2610,8 +2607,11 @@
       <c r="S23" s="1" t="s">
         <v>22</v>
       </c>
-    </row>
-    <row r="24" spans="1:19" x14ac:dyDescent="0.25">
+      <c r="T23" s="1" t="s">
+        <v>22</v>
+      </c>
+    </row>
+    <row r="24" spans="1:20" x14ac:dyDescent="0.25">
       <c r="A24" s="1" t="s">
         <v>19</v>
       </c>
@@ -2621,15 +2621,13 @@
       <c r="C24" s="1" t="s">
         <v>21</v>
       </c>
-      <c r="D24" s="1" t="s">
-        <v>22</v>
-      </c>
+      <c r="D24" s="1"/>
       <c r="E24" s="1" t="s">
+        <v>22</v>
+      </c>
+      <c r="F24" s="1" t="s">
         <v>23</v>
       </c>
-      <c r="F24" s="1" t="s">
-        <v>22</v>
-      </c>
       <c r="G24" s="1" t="s">
         <v>22</v>
       </c>
@@ -2646,11 +2644,11 @@
         <v>22</v>
       </c>
       <c r="L24" s="1" t="s">
+        <v>22</v>
+      </c>
+      <c r="M24" s="1" t="s">
         <v>47</v>
       </c>
-      <c r="M24" s="1" t="s">
-        <v>22</v>
-      </c>
       <c r="N24" s="1" t="s">
         <v>22</v>
       </c>
@@ -2669,8 +2667,11 @@
       <c r="S24" s="1" t="s">
         <v>22</v>
       </c>
-    </row>
-    <row r="25" spans="1:19" x14ac:dyDescent="0.25">
+      <c r="T24" s="1" t="s">
+        <v>22</v>
+      </c>
+    </row>
+    <row r="25" spans="1:20" x14ac:dyDescent="0.25">
       <c r="A25" s="1" t="s">
         <v>19</v>
       </c>
@@ -2680,15 +2681,13 @@
       <c r="C25" s="1" t="s">
         <v>21</v>
       </c>
-      <c r="D25" s="1" t="s">
-        <v>22</v>
-      </c>
+      <c r="D25" s="1"/>
       <c r="E25" s="1" t="s">
+        <v>22</v>
+      </c>
+      <c r="F25" s="1" t="s">
         <v>23</v>
       </c>
-      <c r="F25" s="1" t="s">
-        <v>22</v>
-      </c>
       <c r="G25" s="1" t="s">
         <v>22</v>
       </c>
@@ -2705,11 +2704,11 @@
         <v>22</v>
       </c>
       <c r="L25" s="1" t="s">
+        <v>22</v>
+      </c>
+      <c r="M25" s="1" t="s">
         <v>30</v>
       </c>
-      <c r="M25" s="1" t="s">
-        <v>22</v>
-      </c>
       <c r="N25" s="1" t="s">
         <v>22</v>
       </c>
@@ -2728,8 +2727,11 @@
       <c r="S25" s="1" t="s">
         <v>22</v>
       </c>
-    </row>
-    <row r="26" spans="1:19" x14ac:dyDescent="0.25">
+      <c r="T25" s="1" t="s">
+        <v>22</v>
+      </c>
+    </row>
+    <row r="26" spans="1:20" x14ac:dyDescent="0.25">
       <c r="A26" s="1" t="s">
         <v>49</v>
       </c>
@@ -2739,42 +2741,40 @@
       <c r="C26" s="1" t="s">
         <v>51</v>
       </c>
-      <c r="D26" s="1" t="s">
+      <c r="D26" s="1"/>
+      <c r="E26" s="1" t="s">
         <v>52</v>
       </c>
-      <c r="E26" s="1" t="s">
+      <c r="F26" s="1" t="s">
         <v>53</v>
       </c>
-      <c r="F26" s="1" t="s">
+      <c r="G26" s="1" t="s">
         <v>54</v>
       </c>
-      <c r="G26" s="1" t="s">
+      <c r="H26" s="1" t="s">
         <v>55</v>
       </c>
-      <c r="H26" s="1" t="s">
+      <c r="I26" s="1" t="s">
         <v>56</v>
       </c>
-      <c r="I26" s="1" t="s">
+      <c r="J26" s="1" t="s">
         <v>57</v>
       </c>
-      <c r="J26" s="1" t="s">
+      <c r="K26" s="1" t="s">
         <v>58</v>
       </c>
-      <c r="K26" s="1" t="s">
+      <c r="L26" s="1" t="s">
         <v>59</v>
       </c>
-      <c r="L26" s="1" t="s">
+      <c r="M26" s="1" t="s">
         <v>60</v>
       </c>
-      <c r="M26" s="1" t="s">
+      <c r="N26" s="1" t="s">
         <v>61</v>
       </c>
-      <c r="N26" s="1" t="s">
+      <c r="O26" s="1" t="s">
         <v>62</v>
       </c>
-      <c r="O26" s="1" t="s">
-        <v>22</v>
-      </c>
       <c r="P26" s="1" t="s">
         <v>22</v>
       </c>
@@ -2782,13 +2782,16 @@
         <v>22</v>
       </c>
       <c r="R26" s="1" t="s">
+        <v>22</v>
+      </c>
+      <c r="S26" s="1" t="s">
         <v>63</v>
       </c>
-      <c r="S26" s="1" t="s">
+      <c r="T26" s="1" t="s">
         <v>64</v>
       </c>
     </row>
-    <row r="27" spans="1:19" x14ac:dyDescent="0.25">
+    <row r="27" spans="1:20" x14ac:dyDescent="0.25">
       <c r="A27" s="1" t="s">
         <v>65</v>
       </c>
@@ -2798,9 +2801,7 @@
       <c r="C27" s="1" t="s">
         <v>21</v>
       </c>
-      <c r="D27" s="1" t="s">
-        <v>22</v>
-      </c>
+      <c r="D27" s="1"/>
       <c r="E27" s="1" t="s">
         <v>22</v>
       </c>
@@ -2832,22 +2833,25 @@
         <v>22</v>
       </c>
       <c r="O27" s="1" t="s">
+        <v>22</v>
+      </c>
+      <c r="P27" s="1" t="s">
         <v>67</v>
       </c>
-      <c r="P27" s="1" t="s">
+      <c r="Q27" s="1" t="s">
         <v>68</v>
       </c>
-      <c r="Q27" s="1" t="s">
+      <c r="R27" s="1" t="s">
         <v>69</v>
       </c>
-      <c r="R27" s="1" t="s">
-        <v>22</v>
-      </c>
       <c r="S27" s="1" t="s">
         <v>22</v>
       </c>
-    </row>
-    <row r="28" spans="1:19" x14ac:dyDescent="0.25">
+      <c r="T27" s="1" t="s">
+        <v>22</v>
+      </c>
+    </row>
+    <row r="28" spans="1:20" x14ac:dyDescent="0.25">
       <c r="A28" s="1" t="s">
         <v>65</v>
       </c>
@@ -2857,9 +2861,7 @@
       <c r="C28" s="1" t="s">
         <v>21</v>
       </c>
-      <c r="D28" s="1" t="s">
-        <v>22</v>
-      </c>
+      <c r="D28" s="1"/>
       <c r="E28" s="1" t="s">
         <v>22</v>
       </c>
@@ -2891,22 +2893,25 @@
         <v>22</v>
       </c>
       <c r="O28" s="1" t="s">
+        <v>22</v>
+      </c>
+      <c r="P28" s="1" t="s">
         <v>71</v>
       </c>
-      <c r="P28" s="1" t="s">
+      <c r="Q28" s="1" t="s">
         <v>72</v>
       </c>
-      <c r="Q28" s="1" t="s">
+      <c r="R28" s="1" t="s">
         <v>73</v>
       </c>
-      <c r="R28" s="1" t="s">
-        <v>22</v>
-      </c>
       <c r="S28" s="1" t="s">
         <v>22</v>
       </c>
-    </row>
-    <row r="29" spans="1:19" x14ac:dyDescent="0.25">
+      <c r="T28" s="1" t="s">
+        <v>22</v>
+      </c>
+    </row>
+    <row r="29" spans="1:20" x14ac:dyDescent="0.25">
       <c r="A29" s="1" t="s">
         <v>65</v>
       </c>
@@ -2916,9 +2921,7 @@
       <c r="C29" s="1" t="s">
         <v>51</v>
       </c>
-      <c r="D29" s="1" t="s">
-        <v>22</v>
-      </c>
+      <c r="D29" s="1"/>
       <c r="E29" s="1" t="s">
         <v>22</v>
       </c>
@@ -2950,22 +2953,25 @@
         <v>22</v>
       </c>
       <c r="O29" s="1" t="s">
+        <v>22</v>
+      </c>
+      <c r="P29" s="1" t="s">
         <v>74</v>
       </c>
-      <c r="P29" s="1" t="s">
+      <c r="Q29" s="1" t="s">
         <v>75</v>
       </c>
-      <c r="Q29" s="1" t="s">
+      <c r="R29" s="1" t="s">
         <v>76</v>
       </c>
-      <c r="R29" s="1" t="s">
-        <v>22</v>
-      </c>
       <c r="S29" s="1" t="s">
         <v>22</v>
       </c>
-    </row>
-    <row r="30" spans="1:19" x14ac:dyDescent="0.25">
+      <c r="T29" s="1" t="s">
+        <v>22</v>
+      </c>
+    </row>
+    <row r="30" spans="1:20" x14ac:dyDescent="0.25">
       <c r="A30" s="1" t="s">
         <v>65</v>
       </c>
@@ -2975,9 +2981,7 @@
       <c r="C30" s="1" t="s">
         <v>21</v>
       </c>
-      <c r="D30" s="1" t="s">
-        <v>22</v>
-      </c>
+      <c r="D30" s="1"/>
       <c r="E30" s="1" t="s">
         <v>22</v>
       </c>
@@ -3009,22 +3013,25 @@
         <v>22</v>
       </c>
       <c r="O30" s="1" t="s">
+        <v>22</v>
+      </c>
+      <c r="P30" s="1" t="s">
         <v>78</v>
       </c>
-      <c r="P30" s="1" t="s">
+      <c r="Q30" s="1" t="s">
         <v>79</v>
       </c>
-      <c r="Q30" s="1" t="s">
+      <c r="R30" s="1" t="s">
         <v>80</v>
       </c>
-      <c r="R30" s="1" t="s">
-        <v>22</v>
-      </c>
       <c r="S30" s="1" t="s">
         <v>22</v>
       </c>
-    </row>
-    <row r="31" spans="1:19" x14ac:dyDescent="0.25">
+      <c r="T30" s="1" t="s">
+        <v>22</v>
+      </c>
+    </row>
+    <row r="31" spans="1:20" x14ac:dyDescent="0.25">
       <c r="A31" s="1" t="s">
         <v>65</v>
       </c>
@@ -3034,9 +3041,7 @@
       <c r="C31" s="1" t="s">
         <v>21</v>
       </c>
-      <c r="D31" s="1" t="s">
-        <v>22</v>
-      </c>
+      <c r="D31" s="1"/>
       <c r="E31" s="1" t="s">
         <v>22</v>
       </c>
@@ -3068,22 +3073,25 @@
         <v>22</v>
       </c>
       <c r="O31" s="1" t="s">
+        <v>22</v>
+      </c>
+      <c r="P31" s="1" t="s">
         <v>71</v>
       </c>
-      <c r="P31" s="1" t="s">
+      <c r="Q31" s="1" t="s">
         <v>82</v>
       </c>
-      <c r="Q31" s="1" t="s">
+      <c r="R31" s="1" t="s">
         <v>73</v>
       </c>
-      <c r="R31" s="1" t="s">
-        <v>22</v>
-      </c>
       <c r="S31" s="1" t="s">
         <v>22</v>
       </c>
-    </row>
-    <row r="32" spans="1:19" x14ac:dyDescent="0.25">
+      <c r="T31" s="1" t="s">
+        <v>22</v>
+      </c>
+    </row>
+    <row r="32" spans="1:20" x14ac:dyDescent="0.25">
       <c r="A32" s="1" t="s">
         <v>65</v>
       </c>
@@ -3093,9 +3101,7 @@
       <c r="C32" s="1" t="s">
         <v>21</v>
       </c>
-      <c r="D32" s="1" t="s">
-        <v>22</v>
-      </c>
+      <c r="D32" s="1"/>
       <c r="E32" s="1" t="s">
         <v>22</v>
       </c>
@@ -3127,22 +3133,25 @@
         <v>22</v>
       </c>
       <c r="O32" s="1" t="s">
+        <v>22</v>
+      </c>
+      <c r="P32" s="1" t="s">
         <v>71</v>
       </c>
-      <c r="P32" s="1" t="s">
+      <c r="Q32" s="1" t="s">
         <v>84</v>
       </c>
-      <c r="Q32" s="1" t="s">
+      <c r="R32" s="1" t="s">
         <v>73</v>
       </c>
-      <c r="R32" s="1" t="s">
-        <v>22</v>
-      </c>
       <c r="S32" s="1" t="s">
         <v>22</v>
       </c>
-    </row>
-    <row r="33" spans="1:19" x14ac:dyDescent="0.25">
+      <c r="T32" s="1" t="s">
+        <v>22</v>
+      </c>
+    </row>
+    <row r="33" spans="1:20" x14ac:dyDescent="0.25">
       <c r="A33" s="1" t="s">
         <v>85</v>
       </c>
@@ -3152,56 +3161,57 @@
       <c r="C33" s="1" t="s">
         <v>51</v>
       </c>
-      <c r="D33" s="1" t="s">
+      <c r="D33" s="1"/>
+      <c r="E33" s="1" t="s">
         <v>87</v>
       </c>
-      <c r="E33" s="1" t="s">
+      <c r="F33" s="1" t="s">
         <v>88</v>
       </c>
-      <c r="F33" s="1" t="s">
+      <c r="G33" s="1" t="s">
         <v>89</v>
       </c>
-      <c r="G33" s="1" t="s">
+      <c r="H33" s="1" t="s">
         <v>90</v>
       </c>
-      <c r="H33" s="1" t="s">
+      <c r="I33" s="1" t="s">
         <v>91</v>
       </c>
-      <c r="I33" s="1" t="s">
+      <c r="J33" s="1" t="s">
         <v>92</v>
       </c>
-      <c r="J33" s="1" t="s">
+      <c r="K33" s="1" t="s">
         <v>93</v>
       </c>
-      <c r="K33" s="1" t="s">
+      <c r="L33" s="1" t="s">
         <v>94</v>
       </c>
-      <c r="L33" s="1" t="s">
+      <c r="M33" s="1" t="s">
         <v>95</v>
       </c>
-      <c r="M33" s="1" t="s">
+      <c r="N33" s="1" t="s">
         <v>87</v>
       </c>
-      <c r="N33" s="1" t="s">
+      <c r="O33" s="1" t="s">
         <v>96</v>
       </c>
-      <c r="O33" s="1" t="s">
+      <c r="P33" s="1" t="s">
         <v>93</v>
-      </c>
-      <c r="P33" s="1" t="s">
-        <v>97</v>
       </c>
       <c r="Q33" s="1" t="s">
         <v>97</v>
       </c>
       <c r="R33" s="1" t="s">
+        <v>97</v>
+      </c>
+      <c r="S33" s="1" t="s">
         <v>93</v>
       </c>
-      <c r="S33" s="1" t="s">
-        <v>22</v>
-      </c>
-    </row>
-    <row r="34" spans="1:19" x14ac:dyDescent="0.25">
+      <c r="T33" s="1" t="s">
+        <v>22</v>
+      </c>
+    </row>
+    <row r="34" spans="1:20" x14ac:dyDescent="0.25">
       <c r="A34" s="1" t="s">
         <v>98</v>
       </c>
@@ -3211,56 +3221,57 @@
       <c r="C34" s="1" t="s">
         <v>100</v>
       </c>
-      <c r="D34" s="1" t="s">
+      <c r="D34" s="1"/>
+      <c r="E34" s="1" t="s">
         <v>101</v>
       </c>
-      <c r="E34" s="1" t="s">
+      <c r="F34" s="1" t="s">
         <v>102</v>
       </c>
-      <c r="F34" s="1" t="s">
+      <c r="G34" s="1" t="s">
         <v>103</v>
-      </c>
-      <c r="G34" s="1" t="s">
-        <v>104</v>
       </c>
       <c r="H34" s="1" t="s">
         <v>104</v>
       </c>
       <c r="I34" s="1" t="s">
+        <v>104</v>
+      </c>
+      <c r="J34" s="1" t="s">
         <v>105</v>
       </c>
-      <c r="J34" s="1" t="s">
+      <c r="K34" s="1" t="s">
         <v>106</v>
       </c>
-      <c r="K34" s="1" t="s">
+      <c r="L34" s="1" t="s">
         <v>107</v>
       </c>
-      <c r="L34" s="1" t="s">
+      <c r="M34" s="1" t="s">
         <v>108</v>
       </c>
-      <c r="M34" s="1" t="s">
+      <c r="N34" s="1" t="s">
         <v>109</v>
       </c>
-      <c r="N34" s="1" t="s">
+      <c r="O34" s="1" t="s">
         <v>110</v>
       </c>
-      <c r="O34" s="1" t="s">
+      <c r="P34" s="1" t="s">
         <v>104</v>
       </c>
-      <c r="P34" s="1" t="s">
+      <c r="Q34" s="1" t="s">
         <v>111</v>
       </c>
-      <c r="Q34" s="1" t="s">
+      <c r="R34" s="1" t="s">
         <v>106</v>
       </c>
-      <c r="R34" s="1" t="s">
+      <c r="S34" s="1" t="s">
         <v>112</v>
       </c>
-      <c r="S34" s="1" t="s">
-        <v>22</v>
-      </c>
-    </row>
-    <row r="35" spans="1:19" x14ac:dyDescent="0.25">
+      <c r="T34" s="1" t="s">
+        <v>22</v>
+      </c>
+    </row>
+    <row r="35" spans="1:20" x14ac:dyDescent="0.25">
       <c r="A35" s="1" t="s">
         <v>113</v>
       </c>
@@ -3270,42 +3281,40 @@
       <c r="C35" s="1" t="s">
         <v>21</v>
       </c>
-      <c r="D35" s="1" t="s">
+      <c r="D35" s="1"/>
+      <c r="E35" s="1" t="s">
         <v>115</v>
       </c>
-      <c r="E35" s="1" t="s">
+      <c r="F35" s="1" t="s">
         <v>116</v>
       </c>
-      <c r="F35" s="1" t="s">
+      <c r="G35" s="1" t="s">
         <v>117</v>
       </c>
-      <c r="G35" s="1" t="s">
+      <c r="H35" s="1" t="s">
         <v>118</v>
       </c>
-      <c r="H35" s="1" t="s">
+      <c r="I35" s="1" t="s">
         <v>119</v>
       </c>
-      <c r="I35" s="1" t="s">
+      <c r="J35" s="1" t="s">
         <v>120</v>
       </c>
-      <c r="J35" s="1" t="s">
+      <c r="K35" s="1" t="s">
         <v>121</v>
       </c>
-      <c r="K35" s="1" t="s">
+      <c r="L35" s="1" t="s">
         <v>122</v>
       </c>
-      <c r="L35" s="1" t="s">
+      <c r="M35" s="1" t="s">
         <v>123</v>
       </c>
-      <c r="M35" s="1" t="s">
+      <c r="N35" s="1" t="s">
         <v>124</v>
       </c>
-      <c r="N35" s="1" t="s">
+      <c r="O35" s="1" t="s">
         <v>125</v>
       </c>
-      <c r="O35" s="1" t="s">
-        <v>22</v>
-      </c>
       <c r="P35" s="1" t="s">
         <v>22</v>
       </c>
@@ -3313,13 +3322,16 @@
         <v>22</v>
       </c>
       <c r="R35" s="1" t="s">
+        <v>22</v>
+      </c>
+      <c r="S35" s="1" t="s">
         <v>126</v>
       </c>
-      <c r="S35" s="1" t="s">
+      <c r="T35" s="1" t="s">
         <v>127</v>
       </c>
     </row>
-    <row r="36" spans="1:19" x14ac:dyDescent="0.25">
+    <row r="36" spans="1:20" x14ac:dyDescent="0.25">
       <c r="A36" s="1" t="s">
         <v>113</v>
       </c>
@@ -3329,42 +3341,40 @@
       <c r="C36" s="1" t="s">
         <v>21</v>
       </c>
-      <c r="D36" s="1" t="s">
+      <c r="D36" s="1"/>
+      <c r="E36" s="1" t="s">
         <v>129</v>
       </c>
-      <c r="E36" s="1" t="s">
+      <c r="F36" s="1" t="s">
         <v>130</v>
       </c>
-      <c r="F36" s="1" t="s">
+      <c r="G36" s="1" t="s">
         <v>131</v>
       </c>
-      <c r="G36" s="1" t="s">
+      <c r="H36" s="1" t="s">
         <v>132</v>
       </c>
-      <c r="H36" s="1" t="s">
+      <c r="I36" s="1" t="s">
         <v>133</v>
       </c>
-      <c r="I36" s="1" t="s">
+      <c r="J36" s="1" t="s">
         <v>134</v>
       </c>
-      <c r="J36" s="1" t="s">
+      <c r="K36" s="1" t="s">
         <v>135</v>
       </c>
-      <c r="K36" s="1" t="s">
+      <c r="L36" s="1" t="s">
         <v>136</v>
       </c>
-      <c r="L36" s="1" t="s">
+      <c r="M36" s="1" t="s">
         <v>137</v>
       </c>
-      <c r="M36" s="1" t="s">
+      <c r="N36" s="1" t="s">
         <v>138</v>
       </c>
-      <c r="N36" s="1" t="s">
+      <c r="O36" s="1" t="s">
         <v>139</v>
       </c>
-      <c r="O36" s="1" t="s">
-        <v>22</v>
-      </c>
       <c r="P36" s="1" t="s">
         <v>22</v>
       </c>
@@ -3372,13 +3382,16 @@
         <v>22</v>
       </c>
       <c r="R36" s="1" t="s">
+        <v>22</v>
+      </c>
+      <c r="S36" s="1" t="s">
         <v>140</v>
       </c>
-      <c r="S36" s="1" t="s">
+      <c r="T36" s="1" t="s">
         <v>141</v>
       </c>
     </row>
-    <row r="37" spans="1:19" x14ac:dyDescent="0.25">
+    <row r="37" spans="1:20" x14ac:dyDescent="0.25">
       <c r="A37" s="1" t="s">
         <v>113</v>
       </c>
@@ -3388,42 +3401,40 @@
       <c r="C37" s="1" t="s">
         <v>21</v>
       </c>
-      <c r="D37" s="1" t="s">
+      <c r="D37" s="1"/>
+      <c r="E37" s="1" t="s">
         <v>129</v>
       </c>
-      <c r="E37" s="1" t="s">
+      <c r="F37" s="1" t="s">
         <v>130</v>
       </c>
-      <c r="F37" s="1" t="s">
+      <c r="G37" s="1" t="s">
         <v>131</v>
       </c>
-      <c r="G37" s="1" t="s">
+      <c r="H37" s="1" t="s">
         <v>132</v>
       </c>
-      <c r="H37" s="1" t="s">
+      <c r="I37" s="1" t="s">
         <v>133</v>
       </c>
-      <c r="I37" s="1" t="s">
+      <c r="J37" s="1" t="s">
         <v>134</v>
       </c>
-      <c r="J37" s="1" t="s">
+      <c r="K37" s="1" t="s">
         <v>135</v>
       </c>
-      <c r="K37" s="1" t="s">
+      <c r="L37" s="1" t="s">
         <v>136</v>
       </c>
-      <c r="L37" s="1" t="s">
+      <c r="M37" s="1" t="s">
         <v>137</v>
       </c>
-      <c r="M37" s="1" t="s">
+      <c r="N37" s="1" t="s">
         <v>138</v>
       </c>
-      <c r="N37" s="1" t="s">
+      <c r="O37" s="1" t="s">
         <v>143</v>
       </c>
-      <c r="O37" s="1" t="s">
-        <v>22</v>
-      </c>
       <c r="P37" s="1" t="s">
         <v>22</v>
       </c>
@@ -3431,13 +3442,16 @@
         <v>22</v>
       </c>
       <c r="R37" s="1" t="s">
+        <v>22</v>
+      </c>
+      <c r="S37" s="1" t="s">
         <v>140</v>
       </c>
-      <c r="S37" s="1" t="s">
+      <c r="T37" s="1" t="s">
         <v>141</v>
       </c>
     </row>
-    <row r="38" spans="1:19" x14ac:dyDescent="0.25">
+    <row r="38" spans="1:20" x14ac:dyDescent="0.25">
       <c r="A38" s="1" t="s">
         <v>113</v>
       </c>
@@ -3447,42 +3461,40 @@
       <c r="C38" s="1" t="s">
         <v>21</v>
       </c>
-      <c r="D38" s="1" t="s">
+      <c r="D38" s="1"/>
+      <c r="E38" s="1" t="s">
         <v>145</v>
       </c>
-      <c r="E38" s="1" t="s">
+      <c r="F38" s="1" t="s">
         <v>146</v>
       </c>
-      <c r="F38" s="1" t="s">
+      <c r="G38" s="1" t="s">
         <v>147</v>
       </c>
-      <c r="G38" s="1" t="s">
+      <c r="H38" s="1" t="s">
         <v>148</v>
       </c>
-      <c r="H38" s="1" t="s">
+      <c r="I38" s="1" t="s">
         <v>149</v>
       </c>
-      <c r="I38" s="1" t="s">
+      <c r="J38" s="1" t="s">
         <v>150</v>
       </c>
-      <c r="J38" s="1" t="s">
+      <c r="K38" s="1" t="s">
         <v>151</v>
       </c>
-      <c r="K38" s="1" t="s">
+      <c r="L38" s="1" t="s">
         <v>152</v>
       </c>
-      <c r="L38" s="1" t="s">
+      <c r="M38" s="1" t="s">
         <v>153</v>
       </c>
-      <c r="M38" s="1" t="s">
+      <c r="N38" s="1" t="s">
         <v>154</v>
       </c>
-      <c r="N38" s="1" t="s">
+      <c r="O38" s="1" t="s">
         <v>155</v>
       </c>
-      <c r="O38" s="1" t="s">
-        <v>22</v>
-      </c>
       <c r="P38" s="1" t="s">
         <v>22</v>
       </c>
@@ -3490,13 +3502,16 @@
         <v>22</v>
       </c>
       <c r="R38" s="1" t="s">
+        <v>22</v>
+      </c>
+      <c r="S38" s="1" t="s">
         <v>156</v>
       </c>
-      <c r="S38" s="1" t="s">
+      <c r="T38" s="1" t="s">
         <v>157</v>
       </c>
     </row>
-    <row r="39" spans="1:19" x14ac:dyDescent="0.25">
+    <row r="39" spans="1:20" x14ac:dyDescent="0.25">
       <c r="A39" s="1" t="s">
         <v>113</v>
       </c>
@@ -3506,42 +3521,40 @@
       <c r="C39" s="1" t="s">
         <v>21</v>
       </c>
-      <c r="D39" s="1" t="s">
+      <c r="D39" s="1"/>
+      <c r="E39" s="1" t="s">
         <v>158</v>
       </c>
-      <c r="E39" s="1" t="s">
+      <c r="F39" s="1" t="s">
         <v>159</v>
       </c>
-      <c r="F39" s="1" t="s">
+      <c r="G39" s="1" t="s">
         <v>160</v>
       </c>
-      <c r="G39" s="1" t="s">
+      <c r="H39" s="1" t="s">
         <v>161</v>
       </c>
-      <c r="H39" s="1" t="s">
+      <c r="I39" s="1" t="s">
         <v>162</v>
       </c>
-      <c r="I39" s="1" t="s">
+      <c r="J39" s="1" t="s">
         <v>163</v>
       </c>
-      <c r="J39" s="1" t="s">
+      <c r="K39" s="1" t="s">
         <v>164</v>
       </c>
-      <c r="K39" s="1" t="s">
+      <c r="L39" s="1" t="s">
         <v>165</v>
       </c>
-      <c r="L39" s="1" t="s">
+      <c r="M39" s="1" t="s">
         <v>166</v>
       </c>
-      <c r="M39" s="1" t="s">
+      <c r="N39" s="1" t="s">
         <v>167</v>
       </c>
-      <c r="N39" s="1" t="s">
+      <c r="O39" s="1" t="s">
         <v>168</v>
       </c>
-      <c r="O39" s="1" t="s">
-        <v>22</v>
-      </c>
       <c r="P39" s="1" t="s">
         <v>22</v>
       </c>
@@ -3549,13 +3562,16 @@
         <v>22</v>
       </c>
       <c r="R39" s="1" t="s">
+        <v>22</v>
+      </c>
+      <c r="S39" s="1" t="s">
         <v>169</v>
       </c>
-      <c r="S39" s="1" t="s">
+      <c r="T39" s="1" t="s">
         <v>156</v>
       </c>
     </row>
-    <row r="40" spans="1:19" x14ac:dyDescent="0.25">
+    <row r="40" spans="1:20" x14ac:dyDescent="0.25">
       <c r="A40" s="1" t="s">
         <v>113</v>
       </c>
@@ -3565,42 +3581,40 @@
       <c r="C40" s="1" t="s">
         <v>21</v>
       </c>
-      <c r="D40" s="1" t="s">
+      <c r="D40" s="1"/>
+      <c r="E40" s="1" t="s">
         <v>145</v>
       </c>
-      <c r="E40" s="1" t="s">
+      <c r="F40" s="1" t="s">
         <v>170</v>
       </c>
-      <c r="F40" s="1" t="s">
+      <c r="G40" s="1" t="s">
         <v>147</v>
       </c>
-      <c r="G40" s="1" t="s">
+      <c r="H40" s="1" t="s">
         <v>171</v>
       </c>
-      <c r="H40" s="1" t="s">
+      <c r="I40" s="1" t="s">
         <v>149</v>
       </c>
-      <c r="I40" s="1" t="s">
+      <c r="J40" s="1" t="s">
         <v>150</v>
       </c>
-      <c r="J40" s="1" t="s">
+      <c r="K40" s="1" t="s">
         <v>151</v>
       </c>
-      <c r="K40" s="1" t="s">
+      <c r="L40" s="1" t="s">
         <v>172</v>
       </c>
-      <c r="L40" s="1" t="s">
+      <c r="M40" s="1" t="s">
         <v>173</v>
       </c>
-      <c r="M40" s="1" t="s">
+      <c r="N40" s="1" t="s">
         <v>174</v>
       </c>
-      <c r="N40" s="1" t="s">
+      <c r="O40" s="1" t="s">
         <v>175</v>
       </c>
-      <c r="O40" s="1" t="s">
-        <v>22</v>
-      </c>
       <c r="P40" s="1" t="s">
         <v>22</v>
       </c>
@@ -3608,13 +3622,16 @@
         <v>22</v>
       </c>
       <c r="R40" s="1" t="s">
+        <v>22</v>
+      </c>
+      <c r="S40" s="1" t="s">
         <v>156</v>
       </c>
-      <c r="S40" s="1" t="s">
+      <c r="T40" s="1" t="s">
         <v>157</v>
       </c>
     </row>
-    <row r="41" spans="1:19" x14ac:dyDescent="0.25">
+    <row r="41" spans="1:20" x14ac:dyDescent="0.25">
       <c r="A41" s="1" t="s">
         <v>113</v>
       </c>
@@ -3624,42 +3641,40 @@
       <c r="C41" s="1" t="s">
         <v>21</v>
       </c>
-      <c r="D41" s="1" t="s">
+      <c r="D41" s="1"/>
+      <c r="E41" s="1" t="s">
         <v>145</v>
       </c>
-      <c r="E41" s="1" t="s">
+      <c r="F41" s="1" t="s">
         <v>170</v>
       </c>
-      <c r="F41" s="1" t="s">
+      <c r="G41" s="1" t="s">
         <v>147</v>
       </c>
-      <c r="G41" s="1" t="s">
+      <c r="H41" s="1" t="s">
         <v>171</v>
       </c>
-      <c r="H41" s="1" t="s">
+      <c r="I41" s="1" t="s">
         <v>149</v>
       </c>
-      <c r="I41" s="1" t="s">
+      <c r="J41" s="1" t="s">
         <v>150</v>
       </c>
-      <c r="J41" s="1" t="s">
+      <c r="K41" s="1" t="s">
         <v>151</v>
       </c>
-      <c r="K41" s="1" t="s">
+      <c r="L41" s="1" t="s">
         <v>172</v>
       </c>
-      <c r="L41" s="1" t="s">
+      <c r="M41" s="1" t="s">
         <v>177</v>
       </c>
-      <c r="M41" s="1" t="s">
+      <c r="N41" s="1" t="s">
         <v>145</v>
       </c>
-      <c r="N41" s="1" t="s">
+      <c r="O41" s="1" t="s">
         <v>178</v>
       </c>
-      <c r="O41" s="1" t="s">
-        <v>22</v>
-      </c>
       <c r="P41" s="1" t="s">
         <v>22</v>
       </c>
@@ -3667,13 +3682,16 @@
         <v>22</v>
       </c>
       <c r="R41" s="1" t="s">
+        <v>22</v>
+      </c>
+      <c r="S41" s="1" t="s">
         <v>156</v>
       </c>
-      <c r="S41" s="1" t="s">
+      <c r="T41" s="1" t="s">
         <v>157</v>
       </c>
     </row>
-    <row r="42" spans="1:19" x14ac:dyDescent="0.25">
+    <row r="42" spans="1:20" x14ac:dyDescent="0.25">
       <c r="A42" s="1" t="s">
         <v>113</v>
       </c>
@@ -3683,42 +3701,40 @@
       <c r="C42" s="1" t="s">
         <v>21</v>
       </c>
-      <c r="D42" s="1" t="s">
+      <c r="D42" s="1"/>
+      <c r="E42" s="1" t="s">
         <v>180</v>
       </c>
-      <c r="E42" s="1" t="s">
+      <c r="F42" s="1" t="s">
         <v>181</v>
       </c>
-      <c r="F42" s="1" t="s">
+      <c r="G42" s="1" t="s">
         <v>182</v>
       </c>
-      <c r="G42" s="1" t="s">
+      <c r="H42" s="1" t="s">
         <v>183</v>
       </c>
-      <c r="H42" s="1" t="s">
+      <c r="I42" s="1" t="s">
         <v>137</v>
       </c>
-      <c r="I42" s="1" t="s">
+      <c r="J42" s="1" t="s">
         <v>184</v>
       </c>
-      <c r="J42" s="1" t="s">
+      <c r="K42" s="1" t="s">
         <v>185</v>
       </c>
-      <c r="K42" s="1" t="s">
+      <c r="L42" s="1" t="s">
         <v>186</v>
       </c>
-      <c r="L42" s="1" t="s">
+      <c r="M42" s="1" t="s">
         <v>187</v>
       </c>
-      <c r="M42" s="1" t="s">
+      <c r="N42" s="1" t="s">
         <v>188</v>
       </c>
-      <c r="N42" s="1" t="s">
+      <c r="O42" s="1" t="s">
         <v>189</v>
       </c>
-      <c r="O42" s="1" t="s">
-        <v>22</v>
-      </c>
       <c r="P42" s="1" t="s">
         <v>22</v>
       </c>
@@ -3726,13 +3742,16 @@
         <v>22</v>
       </c>
       <c r="R42" s="1" t="s">
+        <v>22</v>
+      </c>
+      <c r="S42" s="1" t="s">
         <v>190</v>
       </c>
-      <c r="S42" s="1" t="s">
+      <c r="T42" s="1" t="s">
         <v>191</v>
       </c>
     </row>
-    <row r="43" spans="1:19" x14ac:dyDescent="0.25">
+    <row r="43" spans="1:20" x14ac:dyDescent="0.25">
       <c r="A43" s="1" t="s">
         <v>113</v>
       </c>
@@ -3742,42 +3761,40 @@
       <c r="C43" s="1" t="s">
         <v>21</v>
       </c>
-      <c r="D43" s="1" t="s">
+      <c r="D43" s="1"/>
+      <c r="E43" s="1" t="s">
         <v>145</v>
       </c>
-      <c r="E43" s="1" t="s">
+      <c r="F43" s="1" t="s">
         <v>192</v>
       </c>
-      <c r="F43" s="1" t="s">
+      <c r="G43" s="1" t="s">
         <v>147</v>
       </c>
-      <c r="G43" s="1" t="s">
+      <c r="H43" s="1" t="s">
         <v>193</v>
       </c>
-      <c r="H43" s="1" t="s">
+      <c r="I43" s="1" t="s">
         <v>149</v>
       </c>
-      <c r="I43" s="1" t="s">
+      <c r="J43" s="1" t="s">
         <v>150</v>
       </c>
-      <c r="J43" s="1" t="s">
+      <c r="K43" s="1" t="s">
         <v>151</v>
       </c>
-      <c r="K43" s="1" t="s">
+      <c r="L43" s="1" t="s">
         <v>172</v>
       </c>
-      <c r="L43" s="1" t="s">
+      <c r="M43" s="1" t="s">
         <v>194</v>
       </c>
-      <c r="M43" s="1" t="s">
+      <c r="N43" s="1" t="s">
         <v>145</v>
       </c>
-      <c r="N43" s="1" t="s">
+      <c r="O43" s="1" t="s">
         <v>195</v>
       </c>
-      <c r="O43" s="1" t="s">
-        <v>22</v>
-      </c>
       <c r="P43" s="1" t="s">
         <v>22</v>
       </c>
@@ -3785,13 +3802,16 @@
         <v>22</v>
       </c>
       <c r="R43" s="1" t="s">
+        <v>22</v>
+      </c>
+      <c r="S43" s="1" t="s">
         <v>156</v>
       </c>
-      <c r="S43" s="1" t="s">
+      <c r="T43" s="1" t="s">
         <v>157</v>
       </c>
     </row>
-    <row r="44" spans="1:19" x14ac:dyDescent="0.25">
+    <row r="44" spans="1:20" x14ac:dyDescent="0.25">
       <c r="A44" s="1" t="s">
         <v>113</v>
       </c>
@@ -3801,42 +3821,40 @@
       <c r="C44" s="1" t="s">
         <v>21</v>
       </c>
-      <c r="D44" s="1" t="s">
+      <c r="D44" s="1"/>
+      <c r="E44" s="1" t="s">
         <v>115</v>
       </c>
-      <c r="E44" s="1" t="s">
+      <c r="F44" s="1" t="s">
         <v>196</v>
       </c>
-      <c r="F44" s="1" t="s">
+      <c r="G44" s="1" t="s">
         <v>117</v>
       </c>
-      <c r="G44" s="1" t="s">
+      <c r="H44" s="1" t="s">
         <v>197</v>
       </c>
-      <c r="H44" s="1" t="s">
+      <c r="I44" s="1" t="s">
         <v>119</v>
       </c>
-      <c r="I44" s="1" t="s">
+      <c r="J44" s="1" t="s">
         <v>120</v>
       </c>
-      <c r="J44" s="1" t="s">
+      <c r="K44" s="1" t="s">
         <v>121</v>
       </c>
-      <c r="K44" s="1" t="s">
+      <c r="L44" s="1" t="s">
         <v>198</v>
       </c>
-      <c r="L44" s="1" t="s">
+      <c r="M44" s="1" t="s">
         <v>199</v>
       </c>
-      <c r="M44" s="1" t="s">
+      <c r="N44" s="1" t="s">
         <v>200</v>
       </c>
-      <c r="N44" s="1" t="s">
+      <c r="O44" s="1" t="s">
         <v>201</v>
       </c>
-      <c r="O44" s="1" t="s">
-        <v>22</v>
-      </c>
       <c r="P44" s="1" t="s">
         <v>22</v>
       </c>
@@ -3844,13 +3862,16 @@
         <v>22</v>
       </c>
       <c r="R44" s="1" t="s">
+        <v>22</v>
+      </c>
+      <c r="S44" s="1" t="s">
         <v>126</v>
       </c>
-      <c r="S44" s="1" t="s">
+      <c r="T44" s="1" t="s">
         <v>127</v>
       </c>
     </row>
-    <row r="45" spans="1:19" x14ac:dyDescent="0.25">
+    <row r="45" spans="1:20" x14ac:dyDescent="0.25">
       <c r="A45" s="1" t="s">
         <v>113</v>
       </c>
@@ -3860,42 +3881,40 @@
       <c r="C45" s="1" t="s">
         <v>21</v>
       </c>
-      <c r="D45" s="1" t="s">
+      <c r="D45" s="1"/>
+      <c r="E45" s="1" t="s">
         <v>145</v>
       </c>
-      <c r="E45" s="1" t="s">
+      <c r="F45" s="1" t="s">
         <v>202</v>
       </c>
-      <c r="F45" s="1" t="s">
+      <c r="G45" s="1" t="s">
         <v>147</v>
       </c>
-      <c r="G45" s="1" t="s">
+      <c r="H45" s="1" t="s">
         <v>171</v>
       </c>
-      <c r="H45" s="1" t="s">
+      <c r="I45" s="1" t="s">
         <v>149</v>
       </c>
-      <c r="I45" s="1" t="s">
+      <c r="J45" s="1" t="s">
         <v>150</v>
       </c>
-      <c r="J45" s="1" t="s">
+      <c r="K45" s="1" t="s">
         <v>151</v>
       </c>
-      <c r="K45" s="1" t="s">
+      <c r="L45" s="1" t="s">
         <v>143</v>
       </c>
-      <c r="L45" s="1" t="s">
+      <c r="M45" s="1" t="s">
         <v>203</v>
       </c>
-      <c r="M45" s="1" t="s">
+      <c r="N45" s="1" t="s">
         <v>204</v>
       </c>
-      <c r="N45" s="1" t="s">
+      <c r="O45" s="1" t="s">
         <v>205</v>
       </c>
-      <c r="O45" s="1" t="s">
-        <v>22</v>
-      </c>
       <c r="P45" s="1" t="s">
         <v>22</v>
       </c>
@@ -3903,13 +3922,16 @@
         <v>22</v>
       </c>
       <c r="R45" s="1" t="s">
+        <v>22</v>
+      </c>
+      <c r="S45" s="1" t="s">
         <v>156</v>
       </c>
-      <c r="S45" s="1" t="s">
+      <c r="T45" s="1" t="s">
         <v>157</v>
       </c>
     </row>
-    <row r="46" spans="1:19" x14ac:dyDescent="0.25">
+    <row r="46" spans="1:20" x14ac:dyDescent="0.25">
       <c r="A46" s="1" t="s">
         <v>113</v>
       </c>
@@ -3919,42 +3941,40 @@
       <c r="C46" s="1" t="s">
         <v>21</v>
       </c>
-      <c r="D46" s="1" t="s">
+      <c r="D46" s="1"/>
+      <c r="E46" s="1" t="s">
         <v>145</v>
       </c>
-      <c r="E46" s="1" t="s">
+      <c r="F46" s="1" t="s">
         <v>170</v>
       </c>
-      <c r="F46" s="1" t="s">
+      <c r="G46" s="1" t="s">
         <v>147</v>
       </c>
-      <c r="G46" s="1" t="s">
+      <c r="H46" s="1" t="s">
         <v>171</v>
       </c>
-      <c r="H46" s="1" t="s">
+      <c r="I46" s="1" t="s">
         <v>149</v>
       </c>
-      <c r="I46" s="1" t="s">
+      <c r="J46" s="1" t="s">
         <v>150</v>
       </c>
-      <c r="J46" s="1" t="s">
+      <c r="K46" s="1" t="s">
         <v>151</v>
       </c>
-      <c r="K46" s="1" t="s">
+      <c r="L46" s="1" t="s">
         <v>172</v>
       </c>
-      <c r="L46" s="1" t="s">
+      <c r="M46" s="1" t="s">
         <v>207</v>
       </c>
-      <c r="M46" s="1" t="s">
+      <c r="N46" s="1" t="s">
         <v>145</v>
       </c>
-      <c r="N46" s="1" t="s">
+      <c r="O46" s="1" t="s">
         <v>208</v>
       </c>
-      <c r="O46" s="1" t="s">
-        <v>22</v>
-      </c>
       <c r="P46" s="1" t="s">
         <v>22</v>
       </c>
@@ -3962,13 +3982,16 @@
         <v>22</v>
       </c>
       <c r="R46" s="1" t="s">
+        <v>22</v>
+      </c>
+      <c r="S46" s="1" t="s">
         <v>156</v>
       </c>
-      <c r="S46" s="1" t="s">
+      <c r="T46" s="1" t="s">
         <v>157</v>
       </c>
     </row>
-    <row r="47" spans="1:19" x14ac:dyDescent="0.25">
+    <row r="47" spans="1:20" x14ac:dyDescent="0.25">
       <c r="A47" s="1" t="s">
         <v>113</v>
       </c>
@@ -3978,42 +4001,40 @@
       <c r="C47" s="1" t="s">
         <v>21</v>
       </c>
-      <c r="D47" s="1" t="s">
+      <c r="D47" s="1"/>
+      <c r="E47" s="1" t="s">
         <v>145</v>
       </c>
-      <c r="E47" s="1" t="s">
+      <c r="F47" s="1" t="s">
         <v>209</v>
       </c>
-      <c r="F47" s="1" t="s">
+      <c r="G47" s="1" t="s">
         <v>147</v>
       </c>
-      <c r="G47" s="1" t="s">
+      <c r="H47" s="1" t="s">
         <v>171</v>
       </c>
-      <c r="H47" s="1" t="s">
+      <c r="I47" s="1" t="s">
         <v>149</v>
       </c>
-      <c r="I47" s="1" t="s">
+      <c r="J47" s="1" t="s">
         <v>150</v>
       </c>
-      <c r="J47" s="1" t="s">
+      <c r="K47" s="1" t="s">
         <v>151</v>
       </c>
-      <c r="K47" s="1" t="s">
+      <c r="L47" s="1" t="s">
         <v>210</v>
       </c>
-      <c r="L47" s="1" t="s">
+      <c r="M47" s="1" t="s">
         <v>211</v>
       </c>
-      <c r="M47" s="1" t="s">
+      <c r="N47" s="1" t="s">
         <v>212</v>
       </c>
-      <c r="N47" s="1" t="s">
+      <c r="O47" s="1" t="s">
         <v>213</v>
       </c>
-      <c r="O47" s="1" t="s">
-        <v>22</v>
-      </c>
       <c r="P47" s="1" t="s">
         <v>22</v>
       </c>
@@ -4021,13 +4042,16 @@
         <v>22</v>
       </c>
       <c r="R47" s="1" t="s">
+        <v>22</v>
+      </c>
+      <c r="S47" s="1" t="s">
         <v>156</v>
       </c>
-      <c r="S47" s="1" t="s">
+      <c r="T47" s="1" t="s">
         <v>157</v>
       </c>
     </row>
-    <row r="48" spans="1:19" x14ac:dyDescent="0.25">
+    <row r="48" spans="1:20" x14ac:dyDescent="0.25">
       <c r="A48" s="1" t="s">
         <v>113</v>
       </c>
@@ -4037,42 +4061,40 @@
       <c r="C48" s="1" t="s">
         <v>21</v>
       </c>
-      <c r="D48" s="1" t="s">
+      <c r="D48" s="1"/>
+      <c r="E48" s="1" t="s">
         <v>145</v>
       </c>
-      <c r="E48" s="1" t="s">
+      <c r="F48" s="1" t="s">
         <v>170</v>
       </c>
-      <c r="F48" s="1" t="s">
+      <c r="G48" s="1" t="s">
         <v>147</v>
       </c>
-      <c r="G48" s="1" t="s">
+      <c r="H48" s="1" t="s">
         <v>171</v>
       </c>
-      <c r="H48" s="1" t="s">
+      <c r="I48" s="1" t="s">
         <v>149</v>
       </c>
-      <c r="I48" s="1" t="s">
+      <c r="J48" s="1" t="s">
         <v>150</v>
       </c>
-      <c r="J48" s="1" t="s">
+      <c r="K48" s="1" t="s">
         <v>151</v>
       </c>
-      <c r="K48" s="1" t="s">
+      <c r="L48" s="1" t="s">
         <v>172</v>
       </c>
-      <c r="L48" s="1" t="s">
+      <c r="M48" s="1" t="s">
         <v>215</v>
       </c>
-      <c r="M48" s="1" t="s">
+      <c r="N48" s="1" t="s">
         <v>145</v>
       </c>
-      <c r="N48" s="1" t="s">
+      <c r="O48" s="1" t="s">
         <v>208</v>
       </c>
-      <c r="O48" s="1" t="s">
-        <v>22</v>
-      </c>
       <c r="P48" s="1" t="s">
         <v>22</v>
       </c>
@@ -4080,13 +4102,16 @@
         <v>22</v>
       </c>
       <c r="R48" s="1" t="s">
+        <v>22</v>
+      </c>
+      <c r="S48" s="1" t="s">
         <v>156</v>
       </c>
-      <c r="S48" s="1" t="s">
+      <c r="T48" s="1" t="s">
         <v>157</v>
       </c>
     </row>
-    <row r="49" spans="1:19" x14ac:dyDescent="0.25">
+    <row r="49" spans="1:20" x14ac:dyDescent="0.25">
       <c r="A49" s="1" t="s">
         <v>113</v>
       </c>
@@ -4096,42 +4121,40 @@
       <c r="C49" s="1" t="s">
         <v>21</v>
       </c>
-      <c r="D49" s="1" t="s">
+      <c r="D49" s="1"/>
+      <c r="E49" s="1" t="s">
         <v>145</v>
       </c>
-      <c r="E49" s="1" t="s">
+      <c r="F49" s="1" t="s">
         <v>170</v>
       </c>
-      <c r="F49" s="1" t="s">
+      <c r="G49" s="1" t="s">
         <v>147</v>
       </c>
-      <c r="G49" s="1" t="s">
+      <c r="H49" s="1" t="s">
         <v>171</v>
       </c>
-      <c r="H49" s="1" t="s">
+      <c r="I49" s="1" t="s">
         <v>149</v>
       </c>
-      <c r="I49" s="1" t="s">
+      <c r="J49" s="1" t="s">
         <v>150</v>
       </c>
-      <c r="J49" s="1" t="s">
+      <c r="K49" s="1" t="s">
         <v>151</v>
       </c>
-      <c r="K49" s="1" t="s">
+      <c r="L49" s="1" t="s">
         <v>172</v>
       </c>
-      <c r="L49" s="1" t="s">
+      <c r="M49" s="1" t="s">
         <v>207</v>
       </c>
-      <c r="M49" s="1" t="s">
+      <c r="N49" s="1" t="s">
         <v>145</v>
       </c>
-      <c r="N49" s="1" t="s">
+      <c r="O49" s="1" t="s">
         <v>208</v>
       </c>
-      <c r="O49" s="1" t="s">
-        <v>22</v>
-      </c>
       <c r="P49" s="1" t="s">
         <v>22</v>
       </c>
@@ -4139,156 +4162,21 @@
         <v>22</v>
       </c>
       <c r="R49" s="1" t="s">
+        <v>22</v>
+      </c>
+      <c r="S49" s="1" t="s">
         <v>156</v>
       </c>
-      <c r="S49" s="1" t="s">
+      <c r="T49" s="1" t="s">
         <v>157</v>
-      </c>
-    </row>
-    <row r="51" spans="1:19" x14ac:dyDescent="0.25">
-      <c r="A51" s="11" t="s">
-        <v>260</v>
-      </c>
-      <c r="B51" s="11" t="s">
-        <v>260</v>
-      </c>
-      <c r="C51" s="11" t="s">
-        <v>260</v>
-      </c>
-    </row>
-    <row r="52" spans="1:19" x14ac:dyDescent="0.25">
-      <c r="A52" s="6" t="s">
-        <v>261</v>
-      </c>
-      <c r="B52" s="6" t="s">
-        <v>262</v>
-      </c>
-      <c r="C52" s="12" t="s">
-        <v>263</v>
-      </c>
-      <c r="D52" s="12" t="s">
-        <v>263</v>
-      </c>
-      <c r="E52" s="12" t="s">
-        <v>263</v>
-      </c>
-      <c r="F52" s="12" t="s">
-        <v>263</v>
-      </c>
-      <c r="G52" s="12" t="s">
-        <v>263</v>
-      </c>
-      <c r="H52" s="12" t="s">
-        <v>263</v>
-      </c>
-      <c r="I52" s="12" t="s">
-        <v>263</v>
-      </c>
-      <c r="J52" s="12" t="s">
-        <v>263</v>
-      </c>
-      <c r="K52" s="12" t="s">
-        <v>263</v>
-      </c>
-      <c r="L52" s="12" t="s">
-        <v>263</v>
-      </c>
-      <c r="M52" s="12" t="s">
-        <v>263</v>
-      </c>
-    </row>
-    <row r="53" spans="1:19" x14ac:dyDescent="0.25">
-      <c r="A53" s="7" t="s">
-        <v>242</v>
-      </c>
-      <c r="B53" s="7" t="s">
-        <v>11</v>
-      </c>
-      <c r="C53" s="8" t="s">
-        <v>264</v>
-      </c>
-      <c r="D53" s="8" t="s">
-        <v>264</v>
-      </c>
-      <c r="E53" s="8" t="s">
-        <v>264</v>
-      </c>
-      <c r="F53" s="8" t="s">
-        <v>264</v>
-      </c>
-      <c r="G53" s="8" t="s">
-        <v>264</v>
-      </c>
-      <c r="H53" s="8" t="s">
-        <v>264</v>
-      </c>
-      <c r="I53" s="8" t="s">
-        <v>264</v>
-      </c>
-      <c r="J53" s="8" t="s">
-        <v>264</v>
-      </c>
-      <c r="K53" s="8" t="s">
-        <v>264</v>
-      </c>
-      <c r="L53" s="8" t="s">
-        <v>264</v>
-      </c>
-      <c r="M53" s="8" t="s">
-        <v>264</v>
-      </c>
-    </row>
-    <row r="54" spans="1:19" x14ac:dyDescent="0.25">
-      <c r="A54" s="7" t="s">
-        <v>228</v>
-      </c>
-      <c r="B54" s="7" t="s">
-        <v>4</v>
-      </c>
-      <c r="C54" s="8" t="s">
-        <v>265</v>
-      </c>
-      <c r="D54" s="8" t="s">
-        <v>265</v>
-      </c>
-      <c r="E54" s="8" t="s">
-        <v>265</v>
-      </c>
-      <c r="F54" s="8" t="s">
-        <v>265</v>
-      </c>
-      <c r="G54" s="8" t="s">
-        <v>265</v>
-      </c>
-      <c r="H54" s="8" t="s">
-        <v>265</v>
-      </c>
-      <c r="I54" s="8" t="s">
-        <v>265</v>
-      </c>
-      <c r="J54" s="8" t="s">
-        <v>265</v>
-      </c>
-      <c r="K54" s="8" t="s">
-        <v>265</v>
-      </c>
-      <c r="L54" s="8" t="s">
-        <v>265</v>
-      </c>
-      <c r="M54" s="8" t="s">
-        <v>265</v>
       </c>
     </row>
   </sheetData>
   <autoFilter ref="A7:C49"/>
-  <mergeCells count="7">
-    <mergeCell ref="C53:M53"/>
-    <mergeCell ref="C54:M54"/>
+  <mergeCells count="3">
     <mergeCell ref="A2:B2"/>
     <mergeCell ref="A3:B3"/>
-    <mergeCell ref="A1:F1"/>
-    <mergeCell ref="A51:C51"/>
-    <mergeCell ref="C52:M52"/>
+    <mergeCell ref="A1:G1"/>
   </mergeCells>
   <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
   <drawing r:id="rId1"/>

</xml_diff>

<commit_message>
done with Add AL to column
</commit_message>
<xml_diff>
--- a/Sample Tables/Sample Crosstab.xlsx
+++ b/Sample Tables/Sample Crosstab.xlsx
@@ -17,7 +17,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="897" uniqueCount="261">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="896" uniqueCount="260">
   <si>
     <t>Analysis</t>
   </si>
@@ -797,9 +797,6 @@
   </si>
   <si>
     <t>SGS Engage --- Sample Crosstab</t>
-  </si>
-  <si>
-    <t>Action Level</t>
   </si>
 </sst>
 </file>
@@ -862,7 +859,7 @@
       </patternFill>
     </fill>
   </fills>
-  <borders count="4">
+  <borders count="3">
     <border>
       <left/>
       <right/>
@@ -904,21 +901,6 @@
         <color indexed="0"/>
       </diagonal>
     </border>
-    <border>
-      <left style="thin">
-        <color indexed="64"/>
-      </left>
-      <right style="thin">
-        <color indexed="64"/>
-      </right>
-      <top style="thin">
-        <color indexed="64"/>
-      </top>
-      <bottom style="thin">
-        <color indexed="64"/>
-      </bottom>
-      <diagonal/>
-    </border>
   </borders>
   <cellStyleXfs count="3">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
@@ -929,7 +911,7 @@
       <alignment horizontal="center" vertical="center"/>
     </xf>
   </cellStyleXfs>
-  <cellXfs count="9">
+  <cellXfs count="8">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="1" xfId="1">
       <alignment horizontal="center" vertical="center"/>
@@ -944,9 +926,6 @@
       <alignment horizontal="right" vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="2" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
@@ -1303,167 +1282,166 @@
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <sheetPr codeName="Sheet1"/>
-  <dimension ref="A1:T49"/>
+  <dimension ref="A1:S49"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
       <pane ySplit="7" topLeftCell="A8" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="C48" sqref="C48"/>
+      <selection pane="bottomLeft" activeCell="E14" sqref="E14"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="9.140625" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
     <col min="1" max="1" width="17.140625" customWidth="1"/>
     <col min="2" max="2" width="25.85546875" customWidth="1"/>
-    <col min="3" max="4" width="25.7109375" customWidth="1"/>
-    <col min="5" max="20" width="21" customWidth="1"/>
+    <col min="3" max="3" width="25.7109375" customWidth="1"/>
+    <col min="4" max="19" width="21" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:20" ht="38.1" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A1" s="8" t="s">
+    <row r="1" spans="1:19" ht="38.1" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A1" s="7" t="s">
         <v>259</v>
       </c>
-      <c r="B1" s="8" t="s">
+      <c r="B1" s="7" t="s">
         <v>259</v>
       </c>
-      <c r="C1" s="8" t="s">
+      <c r="C1" s="7" t="s">
         <v>259</v>
       </c>
-      <c r="D1" s="8"/>
-      <c r="E1" s="8" t="s">
+      <c r="D1" s="7" t="s">
         <v>259</v>
       </c>
-      <c r="F1" s="8" t="s">
+      <c r="E1" s="7" t="s">
         <v>259</v>
       </c>
-      <c r="G1" s="8" t="s">
+      <c r="F1" s="7" t="s">
         <v>259</v>
       </c>
     </row>
-    <row r="2" spans="1:20" x14ac:dyDescent="0.25">
-      <c r="A2" s="7" t="s">
+    <row r="2" spans="1:19" x14ac:dyDescent="0.25">
+      <c r="A2" s="6" t="s">
         <v>217</v>
       </c>
-      <c r="B2" s="7" t="s">
+      <c r="B2" s="6" t="s">
         <v>217</v>
       </c>
       <c r="C2" s="4" t="s">
         <v>219</v>
       </c>
-      <c r="D2" s="4"/>
+      <c r="D2" s="5" t="s">
+        <v>224</v>
+      </c>
       <c r="E2" s="5" t="s">
-        <v>224</v>
+        <v>228</v>
       </c>
       <c r="F2" s="5" t="s">
-        <v>228</v>
+        <v>230</v>
       </c>
       <c r="G2" s="5" t="s">
-        <v>230</v>
+        <v>232</v>
       </c>
       <c r="H2" s="5" t="s">
-        <v>232</v>
+        <v>234</v>
       </c>
       <c r="I2" s="5" t="s">
-        <v>234</v>
+        <v>236</v>
       </c>
       <c r="J2" s="5" t="s">
-        <v>236</v>
+        <v>238</v>
       </c>
       <c r="K2" s="5" t="s">
-        <v>238</v>
+        <v>240</v>
       </c>
       <c r="L2" s="5" t="s">
-        <v>240</v>
+        <v>242</v>
       </c>
       <c r="M2" s="5" t="s">
-        <v>242</v>
+        <v>244</v>
       </c>
       <c r="N2" s="5" t="s">
-        <v>244</v>
+        <v>246</v>
       </c>
       <c r="O2" s="5" t="s">
-        <v>246</v>
+        <v>248</v>
       </c>
       <c r="P2" s="5" t="s">
-        <v>248</v>
+        <v>250</v>
       </c>
       <c r="Q2" s="5" t="s">
-        <v>250</v>
+        <v>252</v>
       </c>
       <c r="R2" s="5" t="s">
-        <v>252</v>
+        <v>254</v>
       </c>
       <c r="S2" s="5" t="s">
-        <v>254</v>
-      </c>
-      <c r="T2" s="5" t="s">
         <v>256</v>
       </c>
     </row>
-    <row r="3" spans="1:20" x14ac:dyDescent="0.25">
-      <c r="A3" s="7" t="s">
+    <row r="3" spans="1:19" x14ac:dyDescent="0.25">
+      <c r="A3" s="6" t="s">
         <v>218</v>
       </c>
-      <c r="B3" s="7" t="s">
+      <c r="B3" s="6" t="s">
         <v>218</v>
       </c>
       <c r="C3" s="4" t="s">
         <v>220</v>
       </c>
-      <c r="D3" s="4"/>
+      <c r="D3" s="5" t="s">
+        <v>3</v>
+      </c>
       <c r="E3" s="5" t="s">
-        <v>3</v>
+        <v>4</v>
       </c>
       <c r="F3" s="5" t="s">
-        <v>4</v>
+        <v>5</v>
       </c>
       <c r="G3" s="5" t="s">
-        <v>5</v>
+        <v>6</v>
       </c>
       <c r="H3" s="5" t="s">
-        <v>6</v>
+        <v>7</v>
       </c>
       <c r="I3" s="5" t="s">
-        <v>7</v>
+        <v>8</v>
       </c>
       <c r="J3" s="5" t="s">
-        <v>8</v>
+        <v>9</v>
       </c>
       <c r="K3" s="5" t="s">
-        <v>9</v>
+        <v>10</v>
       </c>
       <c r="L3" s="5" t="s">
-        <v>10</v>
+        <v>11</v>
       </c>
       <c r="M3" s="5" t="s">
-        <v>11</v>
+        <v>12</v>
       </c>
       <c r="N3" s="5" t="s">
-        <v>12</v>
+        <v>13</v>
       </c>
       <c r="O3" s="5" t="s">
-        <v>13</v>
+        <v>14</v>
       </c>
       <c r="P3" s="5" t="s">
-        <v>14</v>
+        <v>15</v>
       </c>
       <c r="Q3" s="5" t="s">
-        <v>15</v>
+        <v>16</v>
       </c>
       <c r="R3" s="5" t="s">
-        <v>16</v>
+        <v>17</v>
       </c>
       <c r="S3" s="5" t="s">
-        <v>17</v>
-      </c>
-      <c r="T3" s="5" t="s">
         <v>18</v>
       </c>
     </row>
-    <row r="4" spans="1:20" x14ac:dyDescent="0.25">
+    <row r="4" spans="1:19" x14ac:dyDescent="0.25">
       <c r="C4" s="4" t="s">
         <v>221</v>
       </c>
-      <c r="D4" s="4"/>
+      <c r="D4" s="5" t="s">
+        <v>225</v>
+      </c>
       <c r="E4" s="5" t="s">
         <v>225</v>
       </c>
@@ -1509,15 +1487,14 @@
       <c r="S4" s="5" t="s">
         <v>225</v>
       </c>
-      <c r="T4" s="5" t="s">
-        <v>225</v>
-      </c>
-    </row>
-    <row r="5" spans="1:20" x14ac:dyDescent="0.25">
+    </row>
+    <row r="5" spans="1:19" x14ac:dyDescent="0.25">
       <c r="C5" s="4" t="s">
         <v>222</v>
       </c>
-      <c r="D5" s="4"/>
+      <c r="D5" s="5" t="s">
+        <v>226</v>
+      </c>
       <c r="E5" s="5" t="s">
         <v>226</v>
       </c>
@@ -1561,67 +1538,63 @@
         <v>226</v>
       </c>
       <c r="S5" s="5" t="s">
-        <v>226</v>
-      </c>
-      <c r="T5" s="5" t="s">
         <v>257</v>
       </c>
     </row>
-    <row r="6" spans="1:20" x14ac:dyDescent="0.25">
+    <row r="6" spans="1:19" x14ac:dyDescent="0.25">
       <c r="C6" s="4" t="s">
         <v>223</v>
       </c>
-      <c r="D6" s="4"/>
+      <c r="D6" s="5" t="s">
+        <v>227</v>
+      </c>
       <c r="E6" s="5" t="s">
-        <v>227</v>
+        <v>229</v>
       </c>
       <c r="F6" s="5" t="s">
-        <v>229</v>
+        <v>231</v>
       </c>
       <c r="G6" s="5" t="s">
-        <v>231</v>
+        <v>233</v>
       </c>
       <c r="H6" s="5" t="s">
-        <v>233</v>
+        <v>235</v>
       </c>
       <c r="I6" s="5" t="s">
-        <v>235</v>
+        <v>237</v>
       </c>
       <c r="J6" s="5" t="s">
-        <v>237</v>
+        <v>239</v>
       </c>
       <c r="K6" s="5" t="s">
-        <v>239</v>
+        <v>241</v>
       </c>
       <c r="L6" s="5" t="s">
-        <v>241</v>
+        <v>243</v>
       </c>
       <c r="M6" s="5" t="s">
-        <v>243</v>
+        <v>245</v>
       </c>
       <c r="N6" s="5" t="s">
-        <v>245</v>
+        <v>247</v>
       </c>
       <c r="O6" s="5" t="s">
-        <v>247</v>
+        <v>249</v>
       </c>
       <c r="P6" s="5" t="s">
-        <v>249</v>
+        <v>251</v>
       </c>
       <c r="Q6" s="5" t="s">
-        <v>251</v>
+        <v>253</v>
       </c>
       <c r="R6" s="5" t="s">
-        <v>253</v>
+        <v>255</v>
       </c>
       <c r="S6" s="5" t="s">
-        <v>255</v>
-      </c>
-      <c r="T6" s="5" t="s">
         <v>258</v>
       </c>
     </row>
-    <row r="7" spans="1:20" x14ac:dyDescent="0.25">
+    <row r="7" spans="1:19" x14ac:dyDescent="0.25">
       <c r="A7" s="3" t="s">
         <v>0</v>
       </c>
@@ -1631,9 +1604,7 @@
       <c r="C7" s="3" t="s">
         <v>2</v>
       </c>
-      <c r="D7" s="6" t="s">
-        <v>260</v>
-      </c>
+      <c r="D7" s="2"/>
       <c r="E7" s="2"/>
       <c r="F7" s="2"/>
       <c r="G7" s="2"/>
@@ -1649,9 +1620,8 @@
       <c r="Q7" s="2"/>
       <c r="R7" s="2"/>
       <c r="S7" s="2"/>
-      <c r="T7" s="2"/>
-    </row>
-    <row r="8" spans="1:20" x14ac:dyDescent="0.25">
+    </row>
+    <row r="8" spans="1:19" x14ac:dyDescent="0.25">
       <c r="A8" s="1" t="s">
         <v>19</v>
       </c>
@@ -1661,12 +1631,14 @@
       <c r="C8" s="1" t="s">
         <v>21</v>
       </c>
-      <c r="D8" s="1"/>
+      <c r="D8" s="1" t="s">
+        <v>22</v>
+      </c>
       <c r="E8" s="1" t="s">
-        <v>22</v>
+        <v>23</v>
       </c>
       <c r="F8" s="1" t="s">
-        <v>23</v>
+        <v>22</v>
       </c>
       <c r="G8" s="1" t="s">
         <v>22</v>
@@ -1684,10 +1656,10 @@
         <v>22</v>
       </c>
       <c r="L8" s="1" t="s">
-        <v>22</v>
+        <v>24</v>
       </c>
       <c r="M8" s="1" t="s">
-        <v>24</v>
+        <v>22</v>
       </c>
       <c r="N8" s="1" t="s">
         <v>22</v>
@@ -1707,11 +1679,8 @@
       <c r="S8" s="1" t="s">
         <v>22</v>
       </c>
-      <c r="T8" s="1" t="s">
-        <v>22</v>
-      </c>
-    </row>
-    <row r="9" spans="1:20" x14ac:dyDescent="0.25">
+    </row>
+    <row r="9" spans="1:19" x14ac:dyDescent="0.25">
       <c r="A9" s="1" t="s">
         <v>19</v>
       </c>
@@ -1721,12 +1690,14 @@
       <c r="C9" s="1" t="s">
         <v>21</v>
       </c>
-      <c r="D9" s="1"/>
+      <c r="D9" s="1" t="s">
+        <v>22</v>
+      </c>
       <c r="E9" s="1" t="s">
-        <v>22</v>
+        <v>23</v>
       </c>
       <c r="F9" s="1" t="s">
-        <v>23</v>
+        <v>22</v>
       </c>
       <c r="G9" s="1" t="s">
         <v>22</v>
@@ -1744,10 +1715,10 @@
         <v>22</v>
       </c>
       <c r="L9" s="1" t="s">
-        <v>22</v>
+        <v>26</v>
       </c>
       <c r="M9" s="1" t="s">
-        <v>26</v>
+        <v>22</v>
       </c>
       <c r="N9" s="1" t="s">
         <v>22</v>
@@ -1767,11 +1738,8 @@
       <c r="S9" s="1" t="s">
         <v>22</v>
       </c>
-      <c r="T9" s="1" t="s">
-        <v>22</v>
-      </c>
-    </row>
-    <row r="10" spans="1:20" x14ac:dyDescent="0.25">
+    </row>
+    <row r="10" spans="1:19" x14ac:dyDescent="0.25">
       <c r="A10" s="1" t="s">
         <v>19</v>
       </c>
@@ -1781,12 +1749,14 @@
       <c r="C10" s="1" t="s">
         <v>21</v>
       </c>
-      <c r="D10" s="1"/>
+      <c r="D10" s="1" t="s">
+        <v>22</v>
+      </c>
       <c r="E10" s="1" t="s">
-        <v>22</v>
+        <v>23</v>
       </c>
       <c r="F10" s="1" t="s">
-        <v>23</v>
+        <v>22</v>
       </c>
       <c r="G10" s="1" t="s">
         <v>22</v>
@@ -1804,10 +1774,10 @@
         <v>22</v>
       </c>
       <c r="L10" s="1" t="s">
-        <v>22</v>
+        <v>28</v>
       </c>
       <c r="M10" s="1" t="s">
-        <v>28</v>
+        <v>22</v>
       </c>
       <c r="N10" s="1" t="s">
         <v>22</v>
@@ -1827,11 +1797,8 @@
       <c r="S10" s="1" t="s">
         <v>22</v>
       </c>
-      <c r="T10" s="1" t="s">
-        <v>22</v>
-      </c>
-    </row>
-    <row r="11" spans="1:20" x14ac:dyDescent="0.25">
+    </row>
+    <row r="11" spans="1:19" x14ac:dyDescent="0.25">
       <c r="A11" s="1" t="s">
         <v>19</v>
       </c>
@@ -1841,12 +1808,14 @@
       <c r="C11" s="1" t="s">
         <v>21</v>
       </c>
-      <c r="D11" s="1"/>
+      <c r="D11" s="1" t="s">
+        <v>22</v>
+      </c>
       <c r="E11" s="1" t="s">
-        <v>22</v>
+        <v>23</v>
       </c>
       <c r="F11" s="1" t="s">
-        <v>23</v>
+        <v>22</v>
       </c>
       <c r="G11" s="1" t="s">
         <v>22</v>
@@ -1864,10 +1833,10 @@
         <v>22</v>
       </c>
       <c r="L11" s="1" t="s">
-        <v>22</v>
+        <v>30</v>
       </c>
       <c r="M11" s="1" t="s">
-        <v>30</v>
+        <v>22</v>
       </c>
       <c r="N11" s="1" t="s">
         <v>22</v>
@@ -1887,11 +1856,8 @@
       <c r="S11" s="1" t="s">
         <v>22</v>
       </c>
-      <c r="T11" s="1" t="s">
-        <v>22</v>
-      </c>
-    </row>
-    <row r="12" spans="1:20" x14ac:dyDescent="0.25">
+    </row>
+    <row r="12" spans="1:19" x14ac:dyDescent="0.25">
       <c r="A12" s="1" t="s">
         <v>19</v>
       </c>
@@ -1901,12 +1867,14 @@
       <c r="C12" s="1" t="s">
         <v>21</v>
       </c>
-      <c r="D12" s="1"/>
+      <c r="D12" s="1" t="s">
+        <v>22</v>
+      </c>
       <c r="E12" s="1" t="s">
-        <v>22</v>
+        <v>23</v>
       </c>
       <c r="F12" s="1" t="s">
-        <v>23</v>
+        <v>22</v>
       </c>
       <c r="G12" s="1" t="s">
         <v>22</v>
@@ -1924,10 +1892,10 @@
         <v>22</v>
       </c>
       <c r="L12" s="1" t="s">
-        <v>22</v>
+        <v>30</v>
       </c>
       <c r="M12" s="1" t="s">
-        <v>30</v>
+        <v>22</v>
       </c>
       <c r="N12" s="1" t="s">
         <v>22</v>
@@ -1947,11 +1915,8 @@
       <c r="S12" s="1" t="s">
         <v>22</v>
       </c>
-      <c r="T12" s="1" t="s">
-        <v>22</v>
-      </c>
-    </row>
-    <row r="13" spans="1:20" x14ac:dyDescent="0.25">
+    </row>
+    <row r="13" spans="1:19" x14ac:dyDescent="0.25">
       <c r="A13" s="1" t="s">
         <v>19</v>
       </c>
@@ -1961,12 +1926,14 @@
       <c r="C13" s="1" t="s">
         <v>21</v>
       </c>
-      <c r="D13" s="1"/>
+      <c r="D13" s="1" t="s">
+        <v>22</v>
+      </c>
       <c r="E13" s="1" t="s">
-        <v>22</v>
+        <v>23</v>
       </c>
       <c r="F13" s="1" t="s">
-        <v>23</v>
+        <v>22</v>
       </c>
       <c r="G13" s="1" t="s">
         <v>22</v>
@@ -1984,10 +1951,10 @@
         <v>22</v>
       </c>
       <c r="L13" s="1" t="s">
-        <v>22</v>
+        <v>30</v>
       </c>
       <c r="M13" s="1" t="s">
-        <v>30</v>
+        <v>22</v>
       </c>
       <c r="N13" s="1" t="s">
         <v>22</v>
@@ -2007,11 +1974,8 @@
       <c r="S13" s="1" t="s">
         <v>22</v>
       </c>
-      <c r="T13" s="1" t="s">
-        <v>22</v>
-      </c>
-    </row>
-    <row r="14" spans="1:20" x14ac:dyDescent="0.25">
+    </row>
+    <row r="14" spans="1:19" x14ac:dyDescent="0.25">
       <c r="A14" s="1" t="s">
         <v>19</v>
       </c>
@@ -2021,12 +1985,14 @@
       <c r="C14" s="1" t="s">
         <v>21</v>
       </c>
-      <c r="D14" s="1"/>
+      <c r="D14" s="1" t="s">
+        <v>22</v>
+      </c>
       <c r="E14" s="1" t="s">
-        <v>22</v>
+        <v>23</v>
       </c>
       <c r="F14" s="1" t="s">
-        <v>23</v>
+        <v>22</v>
       </c>
       <c r="G14" s="1" t="s">
         <v>22</v>
@@ -2044,10 +2010,10 @@
         <v>22</v>
       </c>
       <c r="L14" s="1" t="s">
-        <v>22</v>
+        <v>30</v>
       </c>
       <c r="M14" s="1" t="s">
-        <v>30</v>
+        <v>22</v>
       </c>
       <c r="N14" s="1" t="s">
         <v>22</v>
@@ -2067,11 +2033,8 @@
       <c r="S14" s="1" t="s">
         <v>22</v>
       </c>
-      <c r="T14" s="1" t="s">
-        <v>22</v>
-      </c>
-    </row>
-    <row r="15" spans="1:20" x14ac:dyDescent="0.25">
+    </row>
+    <row r="15" spans="1:19" x14ac:dyDescent="0.25">
       <c r="A15" s="1" t="s">
         <v>19</v>
       </c>
@@ -2081,12 +2044,14 @@
       <c r="C15" s="1" t="s">
         <v>21</v>
       </c>
-      <c r="D15" s="1"/>
+      <c r="D15" s="1" t="s">
+        <v>22</v>
+      </c>
       <c r="E15" s="1" t="s">
-        <v>22</v>
+        <v>23</v>
       </c>
       <c r="F15" s="1" t="s">
-        <v>23</v>
+        <v>22</v>
       </c>
       <c r="G15" s="1" t="s">
         <v>22</v>
@@ -2104,10 +2069,10 @@
         <v>22</v>
       </c>
       <c r="L15" s="1" t="s">
-        <v>22</v>
+        <v>30</v>
       </c>
       <c r="M15" s="1" t="s">
-        <v>30</v>
+        <v>22</v>
       </c>
       <c r="N15" s="1" t="s">
         <v>22</v>
@@ -2127,11 +2092,8 @@
       <c r="S15" s="1" t="s">
         <v>22</v>
       </c>
-      <c r="T15" s="1" t="s">
-        <v>22</v>
-      </c>
-    </row>
-    <row r="16" spans="1:20" x14ac:dyDescent="0.25">
+    </row>
+    <row r="16" spans="1:19" x14ac:dyDescent="0.25">
       <c r="A16" s="1" t="s">
         <v>19</v>
       </c>
@@ -2141,12 +2103,14 @@
       <c r="C16" s="1" t="s">
         <v>21</v>
       </c>
-      <c r="D16" s="1"/>
+      <c r="D16" s="1" t="s">
+        <v>22</v>
+      </c>
       <c r="E16" s="1" t="s">
-        <v>22</v>
+        <v>23</v>
       </c>
       <c r="F16" s="1" t="s">
-        <v>23</v>
+        <v>22</v>
       </c>
       <c r="G16" s="1" t="s">
         <v>22</v>
@@ -2164,10 +2128,10 @@
         <v>22</v>
       </c>
       <c r="L16" s="1" t="s">
-        <v>22</v>
+        <v>30</v>
       </c>
       <c r="M16" s="1" t="s">
-        <v>30</v>
+        <v>22</v>
       </c>
       <c r="N16" s="1" t="s">
         <v>22</v>
@@ -2187,11 +2151,8 @@
       <c r="S16" s="1" t="s">
         <v>22</v>
       </c>
-      <c r="T16" s="1" t="s">
-        <v>22</v>
-      </c>
-    </row>
-    <row r="17" spans="1:20" x14ac:dyDescent="0.25">
+    </row>
+    <row r="17" spans="1:19" x14ac:dyDescent="0.25">
       <c r="A17" s="1" t="s">
         <v>19</v>
       </c>
@@ -2201,12 +2162,14 @@
       <c r="C17" s="1" t="s">
         <v>21</v>
       </c>
-      <c r="D17" s="1"/>
+      <c r="D17" s="1" t="s">
+        <v>22</v>
+      </c>
       <c r="E17" s="1" t="s">
-        <v>22</v>
+        <v>23</v>
       </c>
       <c r="F17" s="1" t="s">
-        <v>23</v>
+        <v>22</v>
       </c>
       <c r="G17" s="1" t="s">
         <v>22</v>
@@ -2224,10 +2187,10 @@
         <v>22</v>
       </c>
       <c r="L17" s="1" t="s">
-        <v>22</v>
+        <v>30</v>
       </c>
       <c r="M17" s="1" t="s">
-        <v>30</v>
+        <v>22</v>
       </c>
       <c r="N17" s="1" t="s">
         <v>22</v>
@@ -2247,11 +2210,8 @@
       <c r="S17" s="1" t="s">
         <v>22</v>
       </c>
-      <c r="T17" s="1" t="s">
-        <v>22</v>
-      </c>
-    </row>
-    <row r="18" spans="1:20" x14ac:dyDescent="0.25">
+    </row>
+    <row r="18" spans="1:19" x14ac:dyDescent="0.25">
       <c r="A18" s="1" t="s">
         <v>19</v>
       </c>
@@ -2261,12 +2221,14 @@
       <c r="C18" s="1" t="s">
         <v>21</v>
       </c>
-      <c r="D18" s="1"/>
+      <c r="D18" s="1" t="s">
+        <v>22</v>
+      </c>
       <c r="E18" s="1" t="s">
-        <v>22</v>
+        <v>23</v>
       </c>
       <c r="F18" s="1" t="s">
-        <v>23</v>
+        <v>22</v>
       </c>
       <c r="G18" s="1" t="s">
         <v>22</v>
@@ -2284,10 +2246,10 @@
         <v>22</v>
       </c>
       <c r="L18" s="1" t="s">
-        <v>22</v>
+        <v>30</v>
       </c>
       <c r="M18" s="1" t="s">
-        <v>30</v>
+        <v>22</v>
       </c>
       <c r="N18" s="1" t="s">
         <v>22</v>
@@ -2307,11 +2269,8 @@
       <c r="S18" s="1" t="s">
         <v>22</v>
       </c>
-      <c r="T18" s="1" t="s">
-        <v>22</v>
-      </c>
-    </row>
-    <row r="19" spans="1:20" x14ac:dyDescent="0.25">
+    </row>
+    <row r="19" spans="1:19" x14ac:dyDescent="0.25">
       <c r="A19" s="1" t="s">
         <v>19</v>
       </c>
@@ -2321,12 +2280,14 @@
       <c r="C19" s="1" t="s">
         <v>21</v>
       </c>
-      <c r="D19" s="1"/>
+      <c r="D19" s="1" t="s">
+        <v>22</v>
+      </c>
       <c r="E19" s="1" t="s">
-        <v>22</v>
+        <v>23</v>
       </c>
       <c r="F19" s="1" t="s">
-        <v>23</v>
+        <v>22</v>
       </c>
       <c r="G19" s="1" t="s">
         <v>22</v>
@@ -2344,10 +2305,10 @@
         <v>22</v>
       </c>
       <c r="L19" s="1" t="s">
-        <v>22</v>
+        <v>30</v>
       </c>
       <c r="M19" s="1" t="s">
-        <v>30</v>
+        <v>22</v>
       </c>
       <c r="N19" s="1" t="s">
         <v>22</v>
@@ -2367,11 +2328,8 @@
       <c r="S19" s="1" t="s">
         <v>22</v>
       </c>
-      <c r="T19" s="1" t="s">
-        <v>22</v>
-      </c>
-    </row>
-    <row r="20" spans="1:20" x14ac:dyDescent="0.25">
+    </row>
+    <row r="20" spans="1:19" x14ac:dyDescent="0.25">
       <c r="A20" s="1" t="s">
         <v>19</v>
       </c>
@@ -2381,12 +2339,14 @@
       <c r="C20" s="1" t="s">
         <v>21</v>
       </c>
-      <c r="D20" s="1"/>
+      <c r="D20" s="1" t="s">
+        <v>22</v>
+      </c>
       <c r="E20" s="1" t="s">
-        <v>22</v>
+        <v>23</v>
       </c>
       <c r="F20" s="1" t="s">
-        <v>23</v>
+        <v>22</v>
       </c>
       <c r="G20" s="1" t="s">
         <v>22</v>
@@ -2404,10 +2364,10 @@
         <v>22</v>
       </c>
       <c r="L20" s="1" t="s">
-        <v>22</v>
+        <v>30</v>
       </c>
       <c r="M20" s="1" t="s">
-        <v>30</v>
+        <v>22</v>
       </c>
       <c r="N20" s="1" t="s">
         <v>22</v>
@@ -2427,11 +2387,8 @@
       <c r="S20" s="1" t="s">
         <v>22</v>
       </c>
-      <c r="T20" s="1" t="s">
-        <v>22</v>
-      </c>
-    </row>
-    <row r="21" spans="1:20" x14ac:dyDescent="0.25">
+    </row>
+    <row r="21" spans="1:19" x14ac:dyDescent="0.25">
       <c r="A21" s="1" t="s">
         <v>19</v>
       </c>
@@ -2441,12 +2398,14 @@
       <c r="C21" s="1" t="s">
         <v>21</v>
       </c>
-      <c r="D21" s="1"/>
+      <c r="D21" s="1" t="s">
+        <v>22</v>
+      </c>
       <c r="E21" s="1" t="s">
-        <v>22</v>
+        <v>23</v>
       </c>
       <c r="F21" s="1" t="s">
-        <v>23</v>
+        <v>22</v>
       </c>
       <c r="G21" s="1" t="s">
         <v>22</v>
@@ -2464,10 +2423,10 @@
         <v>22</v>
       </c>
       <c r="L21" s="1" t="s">
-        <v>22</v>
+        <v>41</v>
       </c>
       <c r="M21" s="1" t="s">
-        <v>41</v>
+        <v>22</v>
       </c>
       <c r="N21" s="1" t="s">
         <v>22</v>
@@ -2487,11 +2446,8 @@
       <c r="S21" s="1" t="s">
         <v>22</v>
       </c>
-      <c r="T21" s="1" t="s">
-        <v>22</v>
-      </c>
-    </row>
-    <row r="22" spans="1:20" x14ac:dyDescent="0.25">
+    </row>
+    <row r="22" spans="1:19" x14ac:dyDescent="0.25">
       <c r="A22" s="1" t="s">
         <v>19</v>
       </c>
@@ -2501,12 +2457,14 @@
       <c r="C22" s="1" t="s">
         <v>21</v>
       </c>
-      <c r="D22" s="1"/>
+      <c r="D22" s="1" t="s">
+        <v>22</v>
+      </c>
       <c r="E22" s="1" t="s">
-        <v>22</v>
+        <v>23</v>
       </c>
       <c r="F22" s="1" t="s">
-        <v>23</v>
+        <v>22</v>
       </c>
       <c r="G22" s="1" t="s">
         <v>22</v>
@@ -2524,10 +2482,10 @@
         <v>22</v>
       </c>
       <c r="L22" s="1" t="s">
-        <v>22</v>
+        <v>30</v>
       </c>
       <c r="M22" s="1" t="s">
-        <v>30</v>
+        <v>22</v>
       </c>
       <c r="N22" s="1" t="s">
         <v>22</v>
@@ -2547,11 +2505,8 @@
       <c r="S22" s="1" t="s">
         <v>22</v>
       </c>
-      <c r="T22" s="1" t="s">
-        <v>22</v>
-      </c>
-    </row>
-    <row r="23" spans="1:20" x14ac:dyDescent="0.25">
+    </row>
+    <row r="23" spans="1:19" x14ac:dyDescent="0.25">
       <c r="A23" s="1" t="s">
         <v>19</v>
       </c>
@@ -2561,12 +2516,14 @@
       <c r="C23" s="1" t="s">
         <v>21</v>
       </c>
-      <c r="D23" s="1"/>
+      <c r="D23" s="1" t="s">
+        <v>22</v>
+      </c>
       <c r="E23" s="1" t="s">
-        <v>22</v>
+        <v>44</v>
       </c>
       <c r="F23" s="1" t="s">
-        <v>44</v>
+        <v>22</v>
       </c>
       <c r="G23" s="1" t="s">
         <v>22</v>
@@ -2584,10 +2541,10 @@
         <v>22</v>
       </c>
       <c r="L23" s="1" t="s">
-        <v>22</v>
+        <v>45</v>
       </c>
       <c r="M23" s="1" t="s">
-        <v>45</v>
+        <v>22</v>
       </c>
       <c r="N23" s="1" t="s">
         <v>22</v>
@@ -2607,11 +2564,8 @@
       <c r="S23" s="1" t="s">
         <v>22</v>
       </c>
-      <c r="T23" s="1" t="s">
-        <v>22</v>
-      </c>
-    </row>
-    <row r="24" spans="1:20" x14ac:dyDescent="0.25">
+    </row>
+    <row r="24" spans="1:19" x14ac:dyDescent="0.25">
       <c r="A24" s="1" t="s">
         <v>19</v>
       </c>
@@ -2621,12 +2575,14 @@
       <c r="C24" s="1" t="s">
         <v>21</v>
       </c>
-      <c r="D24" s="1"/>
+      <c r="D24" s="1" t="s">
+        <v>22</v>
+      </c>
       <c r="E24" s="1" t="s">
-        <v>22</v>
+        <v>23</v>
       </c>
       <c r="F24" s="1" t="s">
-        <v>23</v>
+        <v>22</v>
       </c>
       <c r="G24" s="1" t="s">
         <v>22</v>
@@ -2644,10 +2600,10 @@
         <v>22</v>
       </c>
       <c r="L24" s="1" t="s">
-        <v>22</v>
+        <v>47</v>
       </c>
       <c r="M24" s="1" t="s">
-        <v>47</v>
+        <v>22</v>
       </c>
       <c r="N24" s="1" t="s">
         <v>22</v>
@@ -2667,11 +2623,8 @@
       <c r="S24" s="1" t="s">
         <v>22</v>
       </c>
-      <c r="T24" s="1" t="s">
-        <v>22</v>
-      </c>
-    </row>
-    <row r="25" spans="1:20" x14ac:dyDescent="0.25">
+    </row>
+    <row r="25" spans="1:19" x14ac:dyDescent="0.25">
       <c r="A25" s="1" t="s">
         <v>19</v>
       </c>
@@ -2681,12 +2634,14 @@
       <c r="C25" s="1" t="s">
         <v>21</v>
       </c>
-      <c r="D25" s="1"/>
+      <c r="D25" s="1" t="s">
+        <v>22</v>
+      </c>
       <c r="E25" s="1" t="s">
-        <v>22</v>
+        <v>23</v>
       </c>
       <c r="F25" s="1" t="s">
-        <v>23</v>
+        <v>22</v>
       </c>
       <c r="G25" s="1" t="s">
         <v>22</v>
@@ -2704,10 +2659,10 @@
         <v>22</v>
       </c>
       <c r="L25" s="1" t="s">
-        <v>22</v>
+        <v>30</v>
       </c>
       <c r="M25" s="1" t="s">
-        <v>30</v>
+        <v>22</v>
       </c>
       <c r="N25" s="1" t="s">
         <v>22</v>
@@ -2727,11 +2682,8 @@
       <c r="S25" s="1" t="s">
         <v>22</v>
       </c>
-      <c r="T25" s="1" t="s">
-        <v>22</v>
-      </c>
-    </row>
-    <row r="26" spans="1:20" x14ac:dyDescent="0.25">
+    </row>
+    <row r="26" spans="1:19" x14ac:dyDescent="0.25">
       <c r="A26" s="1" t="s">
         <v>49</v>
       </c>
@@ -2741,39 +2693,41 @@
       <c r="C26" s="1" t="s">
         <v>51</v>
       </c>
-      <c r="D26" s="1"/>
+      <c r="D26" s="1" t="s">
+        <v>52</v>
+      </c>
       <c r="E26" s="1" t="s">
-        <v>52</v>
+        <v>53</v>
       </c>
       <c r="F26" s="1" t="s">
-        <v>53</v>
+        <v>54</v>
       </c>
       <c r="G26" s="1" t="s">
-        <v>54</v>
+        <v>55</v>
       </c>
       <c r="H26" s="1" t="s">
-        <v>55</v>
+        <v>56</v>
       </c>
       <c r="I26" s="1" t="s">
-        <v>56</v>
+        <v>57</v>
       </c>
       <c r="J26" s="1" t="s">
-        <v>57</v>
+        <v>58</v>
       </c>
       <c r="K26" s="1" t="s">
-        <v>58</v>
+        <v>59</v>
       </c>
       <c r="L26" s="1" t="s">
-        <v>59</v>
+        <v>60</v>
       </c>
       <c r="M26" s="1" t="s">
-        <v>60</v>
+        <v>61</v>
       </c>
       <c r="N26" s="1" t="s">
-        <v>61</v>
+        <v>62</v>
       </c>
       <c r="O26" s="1" t="s">
-        <v>62</v>
+        <v>22</v>
       </c>
       <c r="P26" s="1" t="s">
         <v>22</v>
@@ -2782,16 +2736,13 @@
         <v>22</v>
       </c>
       <c r="R26" s="1" t="s">
-        <v>22</v>
+        <v>63</v>
       </c>
       <c r="S26" s="1" t="s">
-        <v>63</v>
-      </c>
-      <c r="T26" s="1" t="s">
         <v>64</v>
       </c>
     </row>
-    <row r="27" spans="1:20" x14ac:dyDescent="0.25">
+    <row r="27" spans="1:19" x14ac:dyDescent="0.25">
       <c r="A27" s="1" t="s">
         <v>65</v>
       </c>
@@ -2801,7 +2752,9 @@
       <c r="C27" s="1" t="s">
         <v>21</v>
       </c>
-      <c r="D27" s="1"/>
+      <c r="D27" s="1" t="s">
+        <v>22</v>
+      </c>
       <c r="E27" s="1" t="s">
         <v>22</v>
       </c>
@@ -2833,25 +2786,22 @@
         <v>22</v>
       </c>
       <c r="O27" s="1" t="s">
-        <v>22</v>
+        <v>67</v>
       </c>
       <c r="P27" s="1" t="s">
-        <v>67</v>
+        <v>68</v>
       </c>
       <c r="Q27" s="1" t="s">
-        <v>68</v>
+        <v>69</v>
       </c>
       <c r="R27" s="1" t="s">
-        <v>69</v>
+        <v>22</v>
       </c>
       <c r="S27" s="1" t="s">
         <v>22</v>
       </c>
-      <c r="T27" s="1" t="s">
-        <v>22</v>
-      </c>
-    </row>
-    <row r="28" spans="1:20" x14ac:dyDescent="0.25">
+    </row>
+    <row r="28" spans="1:19" x14ac:dyDescent="0.25">
       <c r="A28" s="1" t="s">
         <v>65</v>
       </c>
@@ -2861,7 +2811,9 @@
       <c r="C28" s="1" t="s">
         <v>21</v>
       </c>
-      <c r="D28" s="1"/>
+      <c r="D28" s="1" t="s">
+        <v>22</v>
+      </c>
       <c r="E28" s="1" t="s">
         <v>22</v>
       </c>
@@ -2893,25 +2845,22 @@
         <v>22</v>
       </c>
       <c r="O28" s="1" t="s">
-        <v>22</v>
+        <v>71</v>
       </c>
       <c r="P28" s="1" t="s">
-        <v>71</v>
+        <v>72</v>
       </c>
       <c r="Q28" s="1" t="s">
-        <v>72</v>
+        <v>73</v>
       </c>
       <c r="R28" s="1" t="s">
-        <v>73</v>
+        <v>22</v>
       </c>
       <c r="S28" s="1" t="s">
         <v>22</v>
       </c>
-      <c r="T28" s="1" t="s">
-        <v>22</v>
-      </c>
-    </row>
-    <row r="29" spans="1:20" x14ac:dyDescent="0.25">
+    </row>
+    <row r="29" spans="1:19" x14ac:dyDescent="0.25">
       <c r="A29" s="1" t="s">
         <v>65</v>
       </c>
@@ -2921,7 +2870,9 @@
       <c r="C29" s="1" t="s">
         <v>51</v>
       </c>
-      <c r="D29" s="1"/>
+      <c r="D29" s="1" t="s">
+        <v>22</v>
+      </c>
       <c r="E29" s="1" t="s">
         <v>22</v>
       </c>
@@ -2953,25 +2904,22 @@
         <v>22</v>
       </c>
       <c r="O29" s="1" t="s">
-        <v>22</v>
+        <v>74</v>
       </c>
       <c r="P29" s="1" t="s">
-        <v>74</v>
+        <v>75</v>
       </c>
       <c r="Q29" s="1" t="s">
-        <v>75</v>
+        <v>76</v>
       </c>
       <c r="R29" s="1" t="s">
-        <v>76</v>
+        <v>22</v>
       </c>
       <c r="S29" s="1" t="s">
         <v>22</v>
       </c>
-      <c r="T29" s="1" t="s">
-        <v>22</v>
-      </c>
-    </row>
-    <row r="30" spans="1:20" x14ac:dyDescent="0.25">
+    </row>
+    <row r="30" spans="1:19" x14ac:dyDescent="0.25">
       <c r="A30" s="1" t="s">
         <v>65</v>
       </c>
@@ -2981,7 +2929,9 @@
       <c r="C30" s="1" t="s">
         <v>21</v>
       </c>
-      <c r="D30" s="1"/>
+      <c r="D30" s="1" t="s">
+        <v>22</v>
+      </c>
       <c r="E30" s="1" t="s">
         <v>22</v>
       </c>
@@ -3013,25 +2963,22 @@
         <v>22</v>
       </c>
       <c r="O30" s="1" t="s">
-        <v>22</v>
+        <v>78</v>
       </c>
       <c r="P30" s="1" t="s">
-        <v>78</v>
+        <v>79</v>
       </c>
       <c r="Q30" s="1" t="s">
-        <v>79</v>
+        <v>80</v>
       </c>
       <c r="R30" s="1" t="s">
-        <v>80</v>
+        <v>22</v>
       </c>
       <c r="S30" s="1" t="s">
         <v>22</v>
       </c>
-      <c r="T30" s="1" t="s">
-        <v>22</v>
-      </c>
-    </row>
-    <row r="31" spans="1:20" x14ac:dyDescent="0.25">
+    </row>
+    <row r="31" spans="1:19" x14ac:dyDescent="0.25">
       <c r="A31" s="1" t="s">
         <v>65</v>
       </c>
@@ -3041,7 +2988,9 @@
       <c r="C31" s="1" t="s">
         <v>21</v>
       </c>
-      <c r="D31" s="1"/>
+      <c r="D31" s="1" t="s">
+        <v>22</v>
+      </c>
       <c r="E31" s="1" t="s">
         <v>22</v>
       </c>
@@ -3073,25 +3022,22 @@
         <v>22</v>
       </c>
       <c r="O31" s="1" t="s">
-        <v>22</v>
+        <v>71</v>
       </c>
       <c r="P31" s="1" t="s">
-        <v>71</v>
+        <v>82</v>
       </c>
       <c r="Q31" s="1" t="s">
-        <v>82</v>
+        <v>73</v>
       </c>
       <c r="R31" s="1" t="s">
-        <v>73</v>
+        <v>22</v>
       </c>
       <c r="S31" s="1" t="s">
         <v>22</v>
       </c>
-      <c r="T31" s="1" t="s">
-        <v>22</v>
-      </c>
-    </row>
-    <row r="32" spans="1:20" x14ac:dyDescent="0.25">
+    </row>
+    <row r="32" spans="1:19" x14ac:dyDescent="0.25">
       <c r="A32" s="1" t="s">
         <v>65</v>
       </c>
@@ -3101,7 +3047,9 @@
       <c r="C32" s="1" t="s">
         <v>21</v>
       </c>
-      <c r="D32" s="1"/>
+      <c r="D32" s="1" t="s">
+        <v>22</v>
+      </c>
       <c r="E32" s="1" t="s">
         <v>22</v>
       </c>
@@ -3133,25 +3081,22 @@
         <v>22</v>
       </c>
       <c r="O32" s="1" t="s">
-        <v>22</v>
+        <v>71</v>
       </c>
       <c r="P32" s="1" t="s">
-        <v>71</v>
+        <v>84</v>
       </c>
       <c r="Q32" s="1" t="s">
-        <v>84</v>
+        <v>73</v>
       </c>
       <c r="R32" s="1" t="s">
-        <v>73</v>
+        <v>22</v>
       </c>
       <c r="S32" s="1" t="s">
         <v>22</v>
       </c>
-      <c r="T32" s="1" t="s">
-        <v>22</v>
-      </c>
-    </row>
-    <row r="33" spans="1:20" x14ac:dyDescent="0.25">
+    </row>
+    <row r="33" spans="1:19" x14ac:dyDescent="0.25">
       <c r="A33" s="1" t="s">
         <v>85</v>
       </c>
@@ -3161,57 +3106,56 @@
       <c r="C33" s="1" t="s">
         <v>51</v>
       </c>
-      <c r="D33" s="1"/>
+      <c r="D33" s="1" t="s">
+        <v>87</v>
+      </c>
       <c r="E33" s="1" t="s">
+        <v>88</v>
+      </c>
+      <c r="F33" s="1" t="s">
+        <v>89</v>
+      </c>
+      <c r="G33" s="1" t="s">
+        <v>90</v>
+      </c>
+      <c r="H33" s="1" t="s">
+        <v>91</v>
+      </c>
+      <c r="I33" s="1" t="s">
+        <v>92</v>
+      </c>
+      <c r="J33" s="1" t="s">
+        <v>93</v>
+      </c>
+      <c r="K33" s="1" t="s">
+        <v>94</v>
+      </c>
+      <c r="L33" s="1" t="s">
+        <v>95</v>
+      </c>
+      <c r="M33" s="1" t="s">
         <v>87</v>
       </c>
-      <c r="F33" s="1" t="s">
-        <v>88</v>
-      </c>
-      <c r="G33" s="1" t="s">
-        <v>89</v>
-      </c>
-      <c r="H33" s="1" t="s">
-        <v>90</v>
-      </c>
-      <c r="I33" s="1" t="s">
-        <v>91</v>
-      </c>
-      <c r="J33" s="1" t="s">
-        <v>92</v>
-      </c>
-      <c r="K33" s="1" t="s">
+      <c r="N33" s="1" t="s">
+        <v>96</v>
+      </c>
+      <c r="O33" s="1" t="s">
         <v>93</v>
       </c>
-      <c r="L33" s="1" t="s">
-        <v>94</v>
-      </c>
-      <c r="M33" s="1" t="s">
-        <v>95</v>
-      </c>
-      <c r="N33" s="1" t="s">
-        <v>87</v>
-      </c>
-      <c r="O33" s="1" t="s">
-        <v>96</v>
-      </c>
       <c r="P33" s="1" t="s">
-        <v>93</v>
+        <v>97</v>
       </c>
       <c r="Q33" s="1" t="s">
         <v>97</v>
       </c>
       <c r="R33" s="1" t="s">
-        <v>97</v>
+        <v>93</v>
       </c>
       <c r="S33" s="1" t="s">
-        <v>93</v>
-      </c>
-      <c r="T33" s="1" t="s">
-        <v>22</v>
-      </c>
-    </row>
-    <row r="34" spans="1:20" x14ac:dyDescent="0.25">
+        <v>22</v>
+      </c>
+    </row>
+    <row r="34" spans="1:19" x14ac:dyDescent="0.25">
       <c r="A34" s="1" t="s">
         <v>98</v>
       </c>
@@ -3221,57 +3165,56 @@
       <c r="C34" s="1" t="s">
         <v>100</v>
       </c>
-      <c r="D34" s="1"/>
+      <c r="D34" s="1" t="s">
+        <v>101</v>
+      </c>
       <c r="E34" s="1" t="s">
-        <v>101</v>
+        <v>102</v>
       </c>
       <c r="F34" s="1" t="s">
-        <v>102</v>
+        <v>103</v>
       </c>
       <c r="G34" s="1" t="s">
-        <v>103</v>
+        <v>104</v>
       </c>
       <c r="H34" s="1" t="s">
         <v>104</v>
       </c>
       <c r="I34" s="1" t="s">
+        <v>105</v>
+      </c>
+      <c r="J34" s="1" t="s">
+        <v>106</v>
+      </c>
+      <c r="K34" s="1" t="s">
+        <v>107</v>
+      </c>
+      <c r="L34" s="1" t="s">
+        <v>108</v>
+      </c>
+      <c r="M34" s="1" t="s">
+        <v>109</v>
+      </c>
+      <c r="N34" s="1" t="s">
+        <v>110</v>
+      </c>
+      <c r="O34" s="1" t="s">
         <v>104</v>
       </c>
-      <c r="J34" s="1" t="s">
-        <v>105</v>
-      </c>
-      <c r="K34" s="1" t="s">
+      <c r="P34" s="1" t="s">
+        <v>111</v>
+      </c>
+      <c r="Q34" s="1" t="s">
         <v>106</v>
       </c>
-      <c r="L34" s="1" t="s">
-        <v>107</v>
-      </c>
-      <c r="M34" s="1" t="s">
-        <v>108</v>
-      </c>
-      <c r="N34" s="1" t="s">
-        <v>109</v>
-      </c>
-      <c r="O34" s="1" t="s">
-        <v>110</v>
-      </c>
-      <c r="P34" s="1" t="s">
-        <v>104</v>
-      </c>
-      <c r="Q34" s="1" t="s">
-        <v>111</v>
-      </c>
       <c r="R34" s="1" t="s">
-        <v>106</v>
+        <v>112</v>
       </c>
       <c r="S34" s="1" t="s">
-        <v>112</v>
-      </c>
-      <c r="T34" s="1" t="s">
-        <v>22</v>
-      </c>
-    </row>
-    <row r="35" spans="1:20" x14ac:dyDescent="0.25">
+        <v>22</v>
+      </c>
+    </row>
+    <row r="35" spans="1:19" x14ac:dyDescent="0.25">
       <c r="A35" s="1" t="s">
         <v>113</v>
       </c>
@@ -3281,39 +3224,41 @@
       <c r="C35" s="1" t="s">
         <v>21</v>
       </c>
-      <c r="D35" s="1"/>
+      <c r="D35" s="1" t="s">
+        <v>115</v>
+      </c>
       <c r="E35" s="1" t="s">
-        <v>115</v>
+        <v>116</v>
       </c>
       <c r="F35" s="1" t="s">
-        <v>116</v>
+        <v>117</v>
       </c>
       <c r="G35" s="1" t="s">
-        <v>117</v>
+        <v>118</v>
       </c>
       <c r="H35" s="1" t="s">
-        <v>118</v>
+        <v>119</v>
       </c>
       <c r="I35" s="1" t="s">
-        <v>119</v>
+        <v>120</v>
       </c>
       <c r="J35" s="1" t="s">
-        <v>120</v>
+        <v>121</v>
       </c>
       <c r="K35" s="1" t="s">
-        <v>121</v>
+        <v>122</v>
       </c>
       <c r="L35" s="1" t="s">
-        <v>122</v>
+        <v>123</v>
       </c>
       <c r="M35" s="1" t="s">
-        <v>123</v>
+        <v>124</v>
       </c>
       <c r="N35" s="1" t="s">
-        <v>124</v>
+        <v>125</v>
       </c>
       <c r="O35" s="1" t="s">
-        <v>125</v>
+        <v>22</v>
       </c>
       <c r="P35" s="1" t="s">
         <v>22</v>
@@ -3322,16 +3267,13 @@
         <v>22</v>
       </c>
       <c r="R35" s="1" t="s">
-        <v>22</v>
+        <v>126</v>
       </c>
       <c r="S35" s="1" t="s">
-        <v>126</v>
-      </c>
-      <c r="T35" s="1" t="s">
         <v>127</v>
       </c>
     </row>
-    <row r="36" spans="1:20" x14ac:dyDescent="0.25">
+    <row r="36" spans="1:19" x14ac:dyDescent="0.25">
       <c r="A36" s="1" t="s">
         <v>113</v>
       </c>
@@ -3341,39 +3283,41 @@
       <c r="C36" s="1" t="s">
         <v>21</v>
       </c>
-      <c r="D36" s="1"/>
+      <c r="D36" s="1" t="s">
+        <v>129</v>
+      </c>
       <c r="E36" s="1" t="s">
-        <v>129</v>
+        <v>130</v>
       </c>
       <c r="F36" s="1" t="s">
-        <v>130</v>
+        <v>131</v>
       </c>
       <c r="G36" s="1" t="s">
-        <v>131</v>
+        <v>132</v>
       </c>
       <c r="H36" s="1" t="s">
-        <v>132</v>
+        <v>133</v>
       </c>
       <c r="I36" s="1" t="s">
-        <v>133</v>
+        <v>134</v>
       </c>
       <c r="J36" s="1" t="s">
-        <v>134</v>
+        <v>135</v>
       </c>
       <c r="K36" s="1" t="s">
-        <v>135</v>
+        <v>136</v>
       </c>
       <c r="L36" s="1" t="s">
-        <v>136</v>
+        <v>137</v>
       </c>
       <c r="M36" s="1" t="s">
-        <v>137</v>
+        <v>138</v>
       </c>
       <c r="N36" s="1" t="s">
-        <v>138</v>
+        <v>139</v>
       </c>
       <c r="O36" s="1" t="s">
-        <v>139</v>
+        <v>22</v>
       </c>
       <c r="P36" s="1" t="s">
         <v>22</v>
@@ -3382,16 +3326,13 @@
         <v>22</v>
       </c>
       <c r="R36" s="1" t="s">
-        <v>22</v>
+        <v>140</v>
       </c>
       <c r="S36" s="1" t="s">
-        <v>140</v>
-      </c>
-      <c r="T36" s="1" t="s">
         <v>141</v>
       </c>
     </row>
-    <row r="37" spans="1:20" x14ac:dyDescent="0.25">
+    <row r="37" spans="1:19" x14ac:dyDescent="0.25">
       <c r="A37" s="1" t="s">
         <v>113</v>
       </c>
@@ -3401,39 +3342,41 @@
       <c r="C37" s="1" t="s">
         <v>21</v>
       </c>
-      <c r="D37" s="1"/>
+      <c r="D37" s="1" t="s">
+        <v>129</v>
+      </c>
       <c r="E37" s="1" t="s">
-        <v>129</v>
+        <v>130</v>
       </c>
       <c r="F37" s="1" t="s">
-        <v>130</v>
+        <v>131</v>
       </c>
       <c r="G37" s="1" t="s">
-        <v>131</v>
+        <v>132</v>
       </c>
       <c r="H37" s="1" t="s">
-        <v>132</v>
+        <v>133</v>
       </c>
       <c r="I37" s="1" t="s">
-        <v>133</v>
+        <v>134</v>
       </c>
       <c r="J37" s="1" t="s">
-        <v>134</v>
+        <v>135</v>
       </c>
       <c r="K37" s="1" t="s">
-        <v>135</v>
+        <v>136</v>
       </c>
       <c r="L37" s="1" t="s">
-        <v>136</v>
+        <v>137</v>
       </c>
       <c r="M37" s="1" t="s">
-        <v>137</v>
+        <v>138</v>
       </c>
       <c r="N37" s="1" t="s">
-        <v>138</v>
+        <v>143</v>
       </c>
       <c r="O37" s="1" t="s">
-        <v>143</v>
+        <v>22</v>
       </c>
       <c r="P37" s="1" t="s">
         <v>22</v>
@@ -3442,16 +3385,13 @@
         <v>22</v>
       </c>
       <c r="R37" s="1" t="s">
-        <v>22</v>
+        <v>140</v>
       </c>
       <c r="S37" s="1" t="s">
-        <v>140</v>
-      </c>
-      <c r="T37" s="1" t="s">
         <v>141</v>
       </c>
     </row>
-    <row r="38" spans="1:20" x14ac:dyDescent="0.25">
+    <row r="38" spans="1:19" x14ac:dyDescent="0.25">
       <c r="A38" s="1" t="s">
         <v>113</v>
       </c>
@@ -3461,39 +3401,41 @@
       <c r="C38" s="1" t="s">
         <v>21</v>
       </c>
-      <c r="D38" s="1"/>
+      <c r="D38" s="1" t="s">
+        <v>145</v>
+      </c>
       <c r="E38" s="1" t="s">
-        <v>145</v>
+        <v>146</v>
       </c>
       <c r="F38" s="1" t="s">
-        <v>146</v>
+        <v>147</v>
       </c>
       <c r="G38" s="1" t="s">
-        <v>147</v>
+        <v>148</v>
       </c>
       <c r="H38" s="1" t="s">
-        <v>148</v>
+        <v>149</v>
       </c>
       <c r="I38" s="1" t="s">
-        <v>149</v>
+        <v>150</v>
       </c>
       <c r="J38" s="1" t="s">
-        <v>150</v>
+        <v>151</v>
       </c>
       <c r="K38" s="1" t="s">
-        <v>151</v>
+        <v>152</v>
       </c>
       <c r="L38" s="1" t="s">
-        <v>152</v>
+        <v>153</v>
       </c>
       <c r="M38" s="1" t="s">
-        <v>153</v>
+        <v>154</v>
       </c>
       <c r="N38" s="1" t="s">
-        <v>154</v>
+        <v>155</v>
       </c>
       <c r="O38" s="1" t="s">
-        <v>155</v>
+        <v>22</v>
       </c>
       <c r="P38" s="1" t="s">
         <v>22</v>
@@ -3502,16 +3444,13 @@
         <v>22</v>
       </c>
       <c r="R38" s="1" t="s">
-        <v>22</v>
+        <v>156</v>
       </c>
       <c r="S38" s="1" t="s">
-        <v>156</v>
-      </c>
-      <c r="T38" s="1" t="s">
         <v>157</v>
       </c>
     </row>
-    <row r="39" spans="1:20" x14ac:dyDescent="0.25">
+    <row r="39" spans="1:19" x14ac:dyDescent="0.25">
       <c r="A39" s="1" t="s">
         <v>113</v>
       </c>
@@ -3521,39 +3460,41 @@
       <c r="C39" s="1" t="s">
         <v>21</v>
       </c>
-      <c r="D39" s="1"/>
+      <c r="D39" s="1" t="s">
+        <v>158</v>
+      </c>
       <c r="E39" s="1" t="s">
-        <v>158</v>
+        <v>159</v>
       </c>
       <c r="F39" s="1" t="s">
-        <v>159</v>
+        <v>160</v>
       </c>
       <c r="G39" s="1" t="s">
-        <v>160</v>
+        <v>161</v>
       </c>
       <c r="H39" s="1" t="s">
-        <v>161</v>
+        <v>162</v>
       </c>
       <c r="I39" s="1" t="s">
-        <v>162</v>
+        <v>163</v>
       </c>
       <c r="J39" s="1" t="s">
-        <v>163</v>
+        <v>164</v>
       </c>
       <c r="K39" s="1" t="s">
-        <v>164</v>
+        <v>165</v>
       </c>
       <c r="L39" s="1" t="s">
-        <v>165</v>
+        <v>166</v>
       </c>
       <c r="M39" s="1" t="s">
-        <v>166</v>
+        <v>167</v>
       </c>
       <c r="N39" s="1" t="s">
-        <v>167</v>
+        <v>168</v>
       </c>
       <c r="O39" s="1" t="s">
-        <v>168</v>
+        <v>22</v>
       </c>
       <c r="P39" s="1" t="s">
         <v>22</v>
@@ -3562,16 +3503,13 @@
         <v>22</v>
       </c>
       <c r="R39" s="1" t="s">
-        <v>22</v>
+        <v>169</v>
       </c>
       <c r="S39" s="1" t="s">
-        <v>169</v>
-      </c>
-      <c r="T39" s="1" t="s">
         <v>156</v>
       </c>
     </row>
-    <row r="40" spans="1:20" x14ac:dyDescent="0.25">
+    <row r="40" spans="1:19" x14ac:dyDescent="0.25">
       <c r="A40" s="1" t="s">
         <v>113</v>
       </c>
@@ -3581,39 +3519,41 @@
       <c r="C40" s="1" t="s">
         <v>21</v>
       </c>
-      <c r="D40" s="1"/>
+      <c r="D40" s="1" t="s">
+        <v>145</v>
+      </c>
       <c r="E40" s="1" t="s">
-        <v>145</v>
+        <v>170</v>
       </c>
       <c r="F40" s="1" t="s">
-        <v>170</v>
+        <v>147</v>
       </c>
       <c r="G40" s="1" t="s">
-        <v>147</v>
+        <v>171</v>
       </c>
       <c r="H40" s="1" t="s">
-        <v>171</v>
+        <v>149</v>
       </c>
       <c r="I40" s="1" t="s">
-        <v>149</v>
+        <v>150</v>
       </c>
       <c r="J40" s="1" t="s">
-        <v>150</v>
+        <v>151</v>
       </c>
       <c r="K40" s="1" t="s">
-        <v>151</v>
+        <v>172</v>
       </c>
       <c r="L40" s="1" t="s">
-        <v>172</v>
+        <v>173</v>
       </c>
       <c r="M40" s="1" t="s">
-        <v>173</v>
+        <v>174</v>
       </c>
       <c r="N40" s="1" t="s">
-        <v>174</v>
+        <v>175</v>
       </c>
       <c r="O40" s="1" t="s">
-        <v>175</v>
+        <v>22</v>
       </c>
       <c r="P40" s="1" t="s">
         <v>22</v>
@@ -3622,16 +3562,13 @@
         <v>22</v>
       </c>
       <c r="R40" s="1" t="s">
-        <v>22</v>
+        <v>156</v>
       </c>
       <c r="S40" s="1" t="s">
-        <v>156</v>
-      </c>
-      <c r="T40" s="1" t="s">
         <v>157</v>
       </c>
     </row>
-    <row r="41" spans="1:20" x14ac:dyDescent="0.25">
+    <row r="41" spans="1:19" x14ac:dyDescent="0.25">
       <c r="A41" s="1" t="s">
         <v>113</v>
       </c>
@@ -3641,39 +3578,41 @@
       <c r="C41" s="1" t="s">
         <v>21</v>
       </c>
-      <c r="D41" s="1"/>
+      <c r="D41" s="1" t="s">
+        <v>145</v>
+      </c>
       <c r="E41" s="1" t="s">
+        <v>170</v>
+      </c>
+      <c r="F41" s="1" t="s">
+        <v>147</v>
+      </c>
+      <c r="G41" s="1" t="s">
+        <v>171</v>
+      </c>
+      <c r="H41" s="1" t="s">
+        <v>149</v>
+      </c>
+      <c r="I41" s="1" t="s">
+        <v>150</v>
+      </c>
+      <c r="J41" s="1" t="s">
+        <v>151</v>
+      </c>
+      <c r="K41" s="1" t="s">
+        <v>172</v>
+      </c>
+      <c r="L41" s="1" t="s">
+        <v>177</v>
+      </c>
+      <c r="M41" s="1" t="s">
         <v>145</v>
       </c>
-      <c r="F41" s="1" t="s">
-        <v>170</v>
-      </c>
-      <c r="G41" s="1" t="s">
-        <v>147</v>
-      </c>
-      <c r="H41" s="1" t="s">
-        <v>171</v>
-      </c>
-      <c r="I41" s="1" t="s">
-        <v>149</v>
-      </c>
-      <c r="J41" s="1" t="s">
-        <v>150</v>
-      </c>
-      <c r="K41" s="1" t="s">
-        <v>151</v>
-      </c>
-      <c r="L41" s="1" t="s">
-        <v>172</v>
-      </c>
-      <c r="M41" s="1" t="s">
-        <v>177</v>
-      </c>
       <c r="N41" s="1" t="s">
-        <v>145</v>
+        <v>178</v>
       </c>
       <c r="O41" s="1" t="s">
-        <v>178</v>
+        <v>22</v>
       </c>
       <c r="P41" s="1" t="s">
         <v>22</v>
@@ -3682,16 +3621,13 @@
         <v>22</v>
       </c>
       <c r="R41" s="1" t="s">
-        <v>22</v>
+        <v>156</v>
       </c>
       <c r="S41" s="1" t="s">
-        <v>156</v>
-      </c>
-      <c r="T41" s="1" t="s">
         <v>157</v>
       </c>
     </row>
-    <row r="42" spans="1:20" x14ac:dyDescent="0.25">
+    <row r="42" spans="1:19" x14ac:dyDescent="0.25">
       <c r="A42" s="1" t="s">
         <v>113</v>
       </c>
@@ -3701,39 +3637,41 @@
       <c r="C42" s="1" t="s">
         <v>21</v>
       </c>
-      <c r="D42" s="1"/>
+      <c r="D42" s="1" t="s">
+        <v>180</v>
+      </c>
       <c r="E42" s="1" t="s">
-        <v>180</v>
+        <v>181</v>
       </c>
       <c r="F42" s="1" t="s">
-        <v>181</v>
+        <v>182</v>
       </c>
       <c r="G42" s="1" t="s">
-        <v>182</v>
+        <v>183</v>
       </c>
       <c r="H42" s="1" t="s">
-        <v>183</v>
+        <v>137</v>
       </c>
       <c r="I42" s="1" t="s">
-        <v>137</v>
+        <v>184</v>
       </c>
       <c r="J42" s="1" t="s">
-        <v>184</v>
+        <v>185</v>
       </c>
       <c r="K42" s="1" t="s">
-        <v>185</v>
+        <v>186</v>
       </c>
       <c r="L42" s="1" t="s">
-        <v>186</v>
+        <v>187</v>
       </c>
       <c r="M42" s="1" t="s">
-        <v>187</v>
+        <v>188</v>
       </c>
       <c r="N42" s="1" t="s">
-        <v>188</v>
+        <v>189</v>
       </c>
       <c r="O42" s="1" t="s">
-        <v>189</v>
+        <v>22</v>
       </c>
       <c r="P42" s="1" t="s">
         <v>22</v>
@@ -3742,16 +3680,13 @@
         <v>22</v>
       </c>
       <c r="R42" s="1" t="s">
-        <v>22</v>
+        <v>190</v>
       </c>
       <c r="S42" s="1" t="s">
-        <v>190</v>
-      </c>
-      <c r="T42" s="1" t="s">
         <v>191</v>
       </c>
     </row>
-    <row r="43" spans="1:20" x14ac:dyDescent="0.25">
+    <row r="43" spans="1:19" x14ac:dyDescent="0.25">
       <c r="A43" s="1" t="s">
         <v>113</v>
       </c>
@@ -3761,39 +3696,41 @@
       <c r="C43" s="1" t="s">
         <v>21</v>
       </c>
-      <c r="D43" s="1"/>
+      <c r="D43" s="1" t="s">
+        <v>145</v>
+      </c>
       <c r="E43" s="1" t="s">
+        <v>192</v>
+      </c>
+      <c r="F43" s="1" t="s">
+        <v>147</v>
+      </c>
+      <c r="G43" s="1" t="s">
+        <v>193</v>
+      </c>
+      <c r="H43" s="1" t="s">
+        <v>149</v>
+      </c>
+      <c r="I43" s="1" t="s">
+        <v>150</v>
+      </c>
+      <c r="J43" s="1" t="s">
+        <v>151</v>
+      </c>
+      <c r="K43" s="1" t="s">
+        <v>172</v>
+      </c>
+      <c r="L43" s="1" t="s">
+        <v>194</v>
+      </c>
+      <c r="M43" s="1" t="s">
         <v>145</v>
       </c>
-      <c r="F43" s="1" t="s">
-        <v>192</v>
-      </c>
-      <c r="G43" s="1" t="s">
-        <v>147</v>
-      </c>
-      <c r="H43" s="1" t="s">
-        <v>193</v>
-      </c>
-      <c r="I43" s="1" t="s">
-        <v>149</v>
-      </c>
-      <c r="J43" s="1" t="s">
-        <v>150</v>
-      </c>
-      <c r="K43" s="1" t="s">
-        <v>151</v>
-      </c>
-      <c r="L43" s="1" t="s">
-        <v>172</v>
-      </c>
-      <c r="M43" s="1" t="s">
-        <v>194</v>
-      </c>
       <c r="N43" s="1" t="s">
-        <v>145</v>
+        <v>195</v>
       </c>
       <c r="O43" s="1" t="s">
-        <v>195</v>
+        <v>22</v>
       </c>
       <c r="P43" s="1" t="s">
         <v>22</v>
@@ -3802,16 +3739,13 @@
         <v>22</v>
       </c>
       <c r="R43" s="1" t="s">
-        <v>22</v>
+        <v>156</v>
       </c>
       <c r="S43" s="1" t="s">
-        <v>156</v>
-      </c>
-      <c r="T43" s="1" t="s">
         <v>157</v>
       </c>
     </row>
-    <row r="44" spans="1:20" x14ac:dyDescent="0.25">
+    <row r="44" spans="1:19" x14ac:dyDescent="0.25">
       <c r="A44" s="1" t="s">
         <v>113</v>
       </c>
@@ -3821,39 +3755,41 @@
       <c r="C44" s="1" t="s">
         <v>21</v>
       </c>
-      <c r="D44" s="1"/>
+      <c r="D44" s="1" t="s">
+        <v>115</v>
+      </c>
       <c r="E44" s="1" t="s">
-        <v>115</v>
+        <v>196</v>
       </c>
       <c r="F44" s="1" t="s">
-        <v>196</v>
+        <v>117</v>
       </c>
       <c r="G44" s="1" t="s">
-        <v>117</v>
+        <v>197</v>
       </c>
       <c r="H44" s="1" t="s">
-        <v>197</v>
+        <v>119</v>
       </c>
       <c r="I44" s="1" t="s">
-        <v>119</v>
+        <v>120</v>
       </c>
       <c r="J44" s="1" t="s">
-        <v>120</v>
+        <v>121</v>
       </c>
       <c r="K44" s="1" t="s">
-        <v>121</v>
+        <v>198</v>
       </c>
       <c r="L44" s="1" t="s">
-        <v>198</v>
+        <v>199</v>
       </c>
       <c r="M44" s="1" t="s">
-        <v>199</v>
+        <v>200</v>
       </c>
       <c r="N44" s="1" t="s">
-        <v>200</v>
+        <v>201</v>
       </c>
       <c r="O44" s="1" t="s">
-        <v>201</v>
+        <v>22</v>
       </c>
       <c r="P44" s="1" t="s">
         <v>22</v>
@@ -3862,16 +3798,13 @@
         <v>22</v>
       </c>
       <c r="R44" s="1" t="s">
-        <v>22</v>
+        <v>126</v>
       </c>
       <c r="S44" s="1" t="s">
-        <v>126</v>
-      </c>
-      <c r="T44" s="1" t="s">
         <v>127</v>
       </c>
     </row>
-    <row r="45" spans="1:20" x14ac:dyDescent="0.25">
+    <row r="45" spans="1:19" x14ac:dyDescent="0.25">
       <c r="A45" s="1" t="s">
         <v>113</v>
       </c>
@@ -3881,39 +3814,41 @@
       <c r="C45" s="1" t="s">
         <v>21</v>
       </c>
-      <c r="D45" s="1"/>
+      <c r="D45" s="1" t="s">
+        <v>145</v>
+      </c>
       <c r="E45" s="1" t="s">
-        <v>145</v>
+        <v>202</v>
       </c>
       <c r="F45" s="1" t="s">
-        <v>202</v>
+        <v>147</v>
       </c>
       <c r="G45" s="1" t="s">
-        <v>147</v>
+        <v>171</v>
       </c>
       <c r="H45" s="1" t="s">
-        <v>171</v>
+        <v>149</v>
       </c>
       <c r="I45" s="1" t="s">
-        <v>149</v>
+        <v>150</v>
       </c>
       <c r="J45" s="1" t="s">
-        <v>150</v>
+        <v>151</v>
       </c>
       <c r="K45" s="1" t="s">
-        <v>151</v>
+        <v>143</v>
       </c>
       <c r="L45" s="1" t="s">
-        <v>143</v>
+        <v>203</v>
       </c>
       <c r="M45" s="1" t="s">
-        <v>203</v>
+        <v>204</v>
       </c>
       <c r="N45" s="1" t="s">
-        <v>204</v>
+        <v>205</v>
       </c>
       <c r="O45" s="1" t="s">
-        <v>205</v>
+        <v>22</v>
       </c>
       <c r="P45" s="1" t="s">
         <v>22</v>
@@ -3922,16 +3857,13 @@
         <v>22</v>
       </c>
       <c r="R45" s="1" t="s">
-        <v>22</v>
+        <v>156</v>
       </c>
       <c r="S45" s="1" t="s">
-        <v>156</v>
-      </c>
-      <c r="T45" s="1" t="s">
         <v>157</v>
       </c>
     </row>
-    <row r="46" spans="1:20" x14ac:dyDescent="0.25">
+    <row r="46" spans="1:19" x14ac:dyDescent="0.25">
       <c r="A46" s="1" t="s">
         <v>113</v>
       </c>
@@ -3941,39 +3873,41 @@
       <c r="C46" s="1" t="s">
         <v>21</v>
       </c>
-      <c r="D46" s="1"/>
+      <c r="D46" s="1" t="s">
+        <v>145</v>
+      </c>
       <c r="E46" s="1" t="s">
+        <v>170</v>
+      </c>
+      <c r="F46" s="1" t="s">
+        <v>147</v>
+      </c>
+      <c r="G46" s="1" t="s">
+        <v>171</v>
+      </c>
+      <c r="H46" s="1" t="s">
+        <v>149</v>
+      </c>
+      <c r="I46" s="1" t="s">
+        <v>150</v>
+      </c>
+      <c r="J46" s="1" t="s">
+        <v>151</v>
+      </c>
+      <c r="K46" s="1" t="s">
+        <v>172</v>
+      </c>
+      <c r="L46" s="1" t="s">
+        <v>207</v>
+      </c>
+      <c r="M46" s="1" t="s">
         <v>145</v>
       </c>
-      <c r="F46" s="1" t="s">
-        <v>170</v>
-      </c>
-      <c r="G46" s="1" t="s">
-        <v>147</v>
-      </c>
-      <c r="H46" s="1" t="s">
-        <v>171</v>
-      </c>
-      <c r="I46" s="1" t="s">
-        <v>149</v>
-      </c>
-      <c r="J46" s="1" t="s">
-        <v>150</v>
-      </c>
-      <c r="K46" s="1" t="s">
-        <v>151</v>
-      </c>
-      <c r="L46" s="1" t="s">
-        <v>172</v>
-      </c>
-      <c r="M46" s="1" t="s">
-        <v>207</v>
-      </c>
       <c r="N46" s="1" t="s">
-        <v>145</v>
+        <v>208</v>
       </c>
       <c r="O46" s="1" t="s">
-        <v>208</v>
+        <v>22</v>
       </c>
       <c r="P46" s="1" t="s">
         <v>22</v>
@@ -3982,16 +3916,13 @@
         <v>22</v>
       </c>
       <c r="R46" s="1" t="s">
-        <v>22</v>
+        <v>156</v>
       </c>
       <c r="S46" s="1" t="s">
-        <v>156</v>
-      </c>
-      <c r="T46" s="1" t="s">
         <v>157</v>
       </c>
     </row>
-    <row r="47" spans="1:20" x14ac:dyDescent="0.25">
+    <row r="47" spans="1:19" x14ac:dyDescent="0.25">
       <c r="A47" s="1" t="s">
         <v>113</v>
       </c>
@@ -4001,39 +3932,41 @@
       <c r="C47" s="1" t="s">
         <v>21</v>
       </c>
-      <c r="D47" s="1"/>
+      <c r="D47" s="1" t="s">
+        <v>145</v>
+      </c>
       <c r="E47" s="1" t="s">
-        <v>145</v>
+        <v>209</v>
       </c>
       <c r="F47" s="1" t="s">
-        <v>209</v>
+        <v>147</v>
       </c>
       <c r="G47" s="1" t="s">
-        <v>147</v>
+        <v>171</v>
       </c>
       <c r="H47" s="1" t="s">
-        <v>171</v>
+        <v>149</v>
       </c>
       <c r="I47" s="1" t="s">
-        <v>149</v>
+        <v>150</v>
       </c>
       <c r="J47" s="1" t="s">
-        <v>150</v>
+        <v>151</v>
       </c>
       <c r="K47" s="1" t="s">
-        <v>151</v>
+        <v>210</v>
       </c>
       <c r="L47" s="1" t="s">
-        <v>210</v>
+        <v>211</v>
       </c>
       <c r="M47" s="1" t="s">
-        <v>211</v>
+        <v>212</v>
       </c>
       <c r="N47" s="1" t="s">
-        <v>212</v>
+        <v>213</v>
       </c>
       <c r="O47" s="1" t="s">
-        <v>213</v>
+        <v>22</v>
       </c>
       <c r="P47" s="1" t="s">
         <v>22</v>
@@ -4042,16 +3975,13 @@
         <v>22</v>
       </c>
       <c r="R47" s="1" t="s">
-        <v>22</v>
+        <v>156</v>
       </c>
       <c r="S47" s="1" t="s">
-        <v>156</v>
-      </c>
-      <c r="T47" s="1" t="s">
         <v>157</v>
       </c>
     </row>
-    <row r="48" spans="1:20" x14ac:dyDescent="0.25">
+    <row r="48" spans="1:19" x14ac:dyDescent="0.25">
       <c r="A48" s="1" t="s">
         <v>113</v>
       </c>
@@ -4061,39 +3991,41 @@
       <c r="C48" s="1" t="s">
         <v>21</v>
       </c>
-      <c r="D48" s="1"/>
+      <c r="D48" s="1" t="s">
+        <v>145</v>
+      </c>
       <c r="E48" s="1" t="s">
+        <v>170</v>
+      </c>
+      <c r="F48" s="1" t="s">
+        <v>147</v>
+      </c>
+      <c r="G48" s="1" t="s">
+        <v>171</v>
+      </c>
+      <c r="H48" s="1" t="s">
+        <v>149</v>
+      </c>
+      <c r="I48" s="1" t="s">
+        <v>150</v>
+      </c>
+      <c r="J48" s="1" t="s">
+        <v>151</v>
+      </c>
+      <c r="K48" s="1" t="s">
+        <v>172</v>
+      </c>
+      <c r="L48" s="1" t="s">
+        <v>215</v>
+      </c>
+      <c r="M48" s="1" t="s">
         <v>145</v>
       </c>
-      <c r="F48" s="1" t="s">
-        <v>170</v>
-      </c>
-      <c r="G48" s="1" t="s">
-        <v>147</v>
-      </c>
-      <c r="H48" s="1" t="s">
-        <v>171</v>
-      </c>
-      <c r="I48" s="1" t="s">
-        <v>149</v>
-      </c>
-      <c r="J48" s="1" t="s">
-        <v>150</v>
-      </c>
-      <c r="K48" s="1" t="s">
-        <v>151</v>
-      </c>
-      <c r="L48" s="1" t="s">
-        <v>172</v>
-      </c>
-      <c r="M48" s="1" t="s">
-        <v>215</v>
-      </c>
       <c r="N48" s="1" t="s">
-        <v>145</v>
+        <v>208</v>
       </c>
       <c r="O48" s="1" t="s">
-        <v>208</v>
+        <v>22</v>
       </c>
       <c r="P48" s="1" t="s">
         <v>22</v>
@@ -4102,16 +4034,13 @@
         <v>22</v>
       </c>
       <c r="R48" s="1" t="s">
-        <v>22</v>
+        <v>156</v>
       </c>
       <c r="S48" s="1" t="s">
-        <v>156</v>
-      </c>
-      <c r="T48" s="1" t="s">
         <v>157</v>
       </c>
     </row>
-    <row r="49" spans="1:20" x14ac:dyDescent="0.25">
+    <row r="49" spans="1:19" x14ac:dyDescent="0.25">
       <c r="A49" s="1" t="s">
         <v>113</v>
       </c>
@@ -4121,39 +4050,41 @@
       <c r="C49" s="1" t="s">
         <v>21</v>
       </c>
-      <c r="D49" s="1"/>
+      <c r="D49" s="1" t="s">
+        <v>145</v>
+      </c>
       <c r="E49" s="1" t="s">
+        <v>170</v>
+      </c>
+      <c r="F49" s="1" t="s">
+        <v>147</v>
+      </c>
+      <c r="G49" s="1" t="s">
+        <v>171</v>
+      </c>
+      <c r="H49" s="1" t="s">
+        <v>149</v>
+      </c>
+      <c r="I49" s="1" t="s">
+        <v>150</v>
+      </c>
+      <c r="J49" s="1" t="s">
+        <v>151</v>
+      </c>
+      <c r="K49" s="1" t="s">
+        <v>172</v>
+      </c>
+      <c r="L49" s="1" t="s">
+        <v>207</v>
+      </c>
+      <c r="M49" s="1" t="s">
         <v>145</v>
       </c>
-      <c r="F49" s="1" t="s">
-        <v>170</v>
-      </c>
-      <c r="G49" s="1" t="s">
-        <v>147</v>
-      </c>
-      <c r="H49" s="1" t="s">
-        <v>171</v>
-      </c>
-      <c r="I49" s="1" t="s">
-        <v>149</v>
-      </c>
-      <c r="J49" s="1" t="s">
-        <v>150</v>
-      </c>
-      <c r="K49" s="1" t="s">
-        <v>151</v>
-      </c>
-      <c r="L49" s="1" t="s">
-        <v>172</v>
-      </c>
-      <c r="M49" s="1" t="s">
-        <v>207</v>
-      </c>
       <c r="N49" s="1" t="s">
-        <v>145</v>
+        <v>208</v>
       </c>
       <c r="O49" s="1" t="s">
-        <v>208</v>
+        <v>22</v>
       </c>
       <c r="P49" s="1" t="s">
         <v>22</v>
@@ -4162,12 +4093,9 @@
         <v>22</v>
       </c>
       <c r="R49" s="1" t="s">
-        <v>22</v>
+        <v>156</v>
       </c>
       <c r="S49" s="1" t="s">
-        <v>156</v>
-      </c>
-      <c r="T49" s="1" t="s">
         <v>157</v>
       </c>
     </row>
@@ -4176,7 +4104,7 @@
   <mergeCells count="3">
     <mergeCell ref="A2:B2"/>
     <mergeCell ref="A3:B3"/>
-    <mergeCell ref="A1:G1"/>
+    <mergeCell ref="A1:F1"/>
   </mergeCells>
   <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
   <drawing r:id="rId1"/>

</xml_diff>

<commit_message>
Lots of work on Action Level
</commit_message>
<xml_diff>
--- a/Sample Tables/Sample Crosstab.xlsx
+++ b/Sample Tables/Sample Crosstab.xlsx
@@ -942,6 +942,74 @@
   </cellStyles>
   <dxfs count="0"/>
   <tableStyles count="0" defaultTableStyle="TableStyleMedium2" defaultPivotStyle="PivotStyleLight16"/>
+  <colors>
+    <indexedColors>
+      <rgbColor rgb="00000000"/>
+      <rgbColor rgb="00FFFFFF"/>
+      <rgbColor rgb="00FF0000"/>
+      <rgbColor rgb="0000FF00"/>
+      <rgbColor rgb="000000FF"/>
+      <rgbColor rgb="00FFFF00"/>
+      <rgbColor rgb="00FF00FF"/>
+      <rgbColor rgb="0000FFFF"/>
+      <rgbColor rgb="00000000"/>
+      <rgbColor rgb="00FFFFFF"/>
+      <rgbColor rgb="00FF0000"/>
+      <rgbColor rgb="0000FF00"/>
+      <rgbColor rgb="000000FF"/>
+      <rgbColor rgb="00FFFF00"/>
+      <rgbColor rgb="00FF00FF"/>
+      <rgbColor rgb="0000FFFF"/>
+      <rgbColor rgb="00800000"/>
+      <rgbColor rgb="00008000"/>
+      <rgbColor rgb="00000080"/>
+      <rgbColor rgb="00808000"/>
+      <rgbColor rgb="00800080"/>
+      <rgbColor rgb="00008080"/>
+      <rgbColor rgb="00C0C0C0"/>
+      <rgbColor rgb="00808080"/>
+      <rgbColor rgb="009999FF"/>
+      <rgbColor rgb="00993366"/>
+      <rgbColor rgb="00FFFFCC"/>
+      <rgbColor rgb="00CCFFFF"/>
+      <rgbColor rgb="00660066"/>
+      <rgbColor rgb="00FF8080"/>
+      <rgbColor rgb="000066CC"/>
+      <rgbColor rgb="00CCCCFF"/>
+      <rgbColor rgb="00000080"/>
+      <rgbColor rgb="00FF00FF"/>
+      <rgbColor rgb="00FFFF00"/>
+      <rgbColor rgb="0000FFFF"/>
+      <rgbColor rgb="00800080"/>
+      <rgbColor rgb="00800000"/>
+      <rgbColor rgb="00008080"/>
+      <rgbColor rgb="000000FF"/>
+      <rgbColor rgb="0000CCFF"/>
+      <rgbColor rgb="00CCFFFF"/>
+      <rgbColor rgb="00CCFFCC"/>
+      <rgbColor rgb="00FFFF99"/>
+      <rgbColor rgb="0099CCFF"/>
+      <rgbColor rgb="00FF99CC"/>
+      <rgbColor rgb="00CC99FF"/>
+      <rgbColor rgb="00FFCC99"/>
+      <rgbColor rgb="003366FF"/>
+      <rgbColor rgb="0033CCCC"/>
+      <rgbColor rgb="0099CC00"/>
+      <rgbColor rgb="00FFCC00"/>
+      <rgbColor rgb="00FF9900"/>
+      <rgbColor rgb="00FF6600"/>
+      <rgbColor rgb="00666699"/>
+      <rgbColor rgb="00969696"/>
+      <rgbColor rgb="00003366"/>
+      <rgbColor rgb="00339966"/>
+      <rgbColor rgb="00003300"/>
+      <rgbColor rgb="00333300"/>
+      <rgbColor rgb="00993300"/>
+      <rgbColor rgb="00993366"/>
+      <rgbColor rgb="00333399"/>
+      <rgbColor rgb="00CFA4DC"/>
+    </indexedColors>
+  </colors>
   <extLst>
     <ext xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" uri="{EB79DEF2-80B8-43e5-95BD-54CBDDF9020C}">
       <x14:slicerStyles defaultSlicerStyle="SlicerStyleLight1"/>

</xml_diff>

<commit_message>
Lots of account stuff
</commit_message>
<xml_diff>
--- a/Sample Tables/Sample Crosstab.xlsx
+++ b/Sample Tables/Sample Crosstab.xlsx
@@ -17,7 +17,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="896" uniqueCount="260">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="897" uniqueCount="261">
   <si>
     <t>Analysis</t>
   </si>
@@ -797,6 +797,9 @@
   </si>
   <si>
     <t>SGS Engage --- Sample Crosstab</t>
+  </si>
+  <si>
+    <t>Action Level</t>
   </si>
 </sst>
 </file>
@@ -859,7 +862,7 @@
       </patternFill>
     </fill>
   </fills>
-  <borders count="3">
+  <borders count="4">
     <border>
       <left/>
       <right/>
@@ -901,6 +904,21 @@
         <color indexed="0"/>
       </diagonal>
     </border>
+    <border>
+      <left style="thin">
+        <color indexed="64"/>
+      </left>
+      <right style="thin">
+        <color indexed="64"/>
+      </right>
+      <top style="thin">
+        <color indexed="64"/>
+      </top>
+      <bottom style="thin">
+        <color indexed="64"/>
+      </bottom>
+      <diagonal/>
+    </border>
   </borders>
   <cellStyleXfs count="3">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
@@ -911,7 +929,7 @@
       <alignment horizontal="center" vertical="center"/>
     </xf>
   </cellStyleXfs>
-  <cellXfs count="8">
+  <cellXfs count="9">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="1" xfId="1">
       <alignment horizontal="center" vertical="center"/>
@@ -933,6 +951,9 @@
     </xf>
     <xf numFmtId="0" fontId="5" fillId="3" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="2" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
     </xf>
   </cellXfs>
   <cellStyles count="3">
@@ -1350,22 +1371,22 @@
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <sheetPr codeName="Sheet1"/>
-  <dimension ref="A1:S49"/>
+  <dimension ref="A1:T49"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
       <pane ySplit="7" topLeftCell="A8" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="E14" sqref="E14"/>
+      <selection pane="bottomLeft" activeCell="D26" sqref="D26"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="9.140625" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
     <col min="1" max="1" width="17.140625" customWidth="1"/>
     <col min="2" max="2" width="25.85546875" customWidth="1"/>
-    <col min="3" max="3" width="25.7109375" customWidth="1"/>
-    <col min="4" max="19" width="21" customWidth="1"/>
+    <col min="3" max="4" width="25.7109375" customWidth="1"/>
+    <col min="5" max="20" width="21" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:19" ht="38.1" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:20" ht="38.1" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A1" s="7" t="s">
         <v>259</v>
       </c>
@@ -1375,17 +1396,18 @@
       <c r="C1" s="7" t="s">
         <v>259</v>
       </c>
-      <c r="D1" s="7" t="s">
-        <v>259</v>
-      </c>
+      <c r="D1" s="7"/>
       <c r="E1" s="7" t="s">
         <v>259</v>
       </c>
       <c r="F1" s="7" t="s">
         <v>259</v>
       </c>
-    </row>
-    <row r="2" spans="1:19" x14ac:dyDescent="0.25">
+      <c r="G1" s="7" t="s">
+        <v>259</v>
+      </c>
+    </row>
+    <row r="2" spans="1:20" x14ac:dyDescent="0.25">
       <c r="A2" s="6" t="s">
         <v>217</v>
       </c>
@@ -1395,56 +1417,57 @@
       <c r="C2" s="4" t="s">
         <v>219</v>
       </c>
-      <c r="D2" s="5" t="s">
+      <c r="D2" s="4"/>
+      <c r="E2" s="5" t="s">
         <v>224</v>
       </c>
-      <c r="E2" s="5" t="s">
+      <c r="F2" s="5" t="s">
         <v>228</v>
       </c>
-      <c r="F2" s="5" t="s">
+      <c r="G2" s="5" t="s">
         <v>230</v>
       </c>
-      <c r="G2" s="5" t="s">
+      <c r="H2" s="5" t="s">
         <v>232</v>
       </c>
-      <c r="H2" s="5" t="s">
+      <c r="I2" s="5" t="s">
         <v>234</v>
       </c>
-      <c r="I2" s="5" t="s">
+      <c r="J2" s="5" t="s">
         <v>236</v>
       </c>
-      <c r="J2" s="5" t="s">
+      <c r="K2" s="5" t="s">
         <v>238</v>
       </c>
-      <c r="K2" s="5" t="s">
+      <c r="L2" s="5" t="s">
         <v>240</v>
       </c>
-      <c r="L2" s="5" t="s">
+      <c r="M2" s="5" t="s">
         <v>242</v>
       </c>
-      <c r="M2" s="5" t="s">
+      <c r="N2" s="5" t="s">
         <v>244</v>
       </c>
-      <c r="N2" s="5" t="s">
+      <c r="O2" s="5" t="s">
         <v>246</v>
       </c>
-      <c r="O2" s="5" t="s">
+      <c r="P2" s="5" t="s">
         <v>248</v>
       </c>
-      <c r="P2" s="5" t="s">
+      <c r="Q2" s="5" t="s">
         <v>250</v>
       </c>
-      <c r="Q2" s="5" t="s">
+      <c r="R2" s="5" t="s">
         <v>252</v>
       </c>
-      <c r="R2" s="5" t="s">
+      <c r="S2" s="5" t="s">
         <v>254</v>
       </c>
-      <c r="S2" s="5" t="s">
+      <c r="T2" s="5" t="s">
         <v>256</v>
       </c>
     </row>
-    <row r="3" spans="1:19" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:20" x14ac:dyDescent="0.25">
       <c r="A3" s="6" t="s">
         <v>218</v>
       </c>
@@ -1454,62 +1477,61 @@
       <c r="C3" s="4" t="s">
         <v>220</v>
       </c>
-      <c r="D3" s="5" t="s">
+      <c r="D3" s="4"/>
+      <c r="E3" s="5" t="s">
         <v>3</v>
       </c>
-      <c r="E3" s="5" t="s">
+      <c r="F3" s="5" t="s">
         <v>4</v>
       </c>
-      <c r="F3" s="5" t="s">
+      <c r="G3" s="5" t="s">
         <v>5</v>
       </c>
-      <c r="G3" s="5" t="s">
+      <c r="H3" s="5" t="s">
         <v>6</v>
       </c>
-      <c r="H3" s="5" t="s">
+      <c r="I3" s="5" t="s">
         <v>7</v>
       </c>
-      <c r="I3" s="5" t="s">
+      <c r="J3" s="5" t="s">
         <v>8</v>
       </c>
-      <c r="J3" s="5" t="s">
+      <c r="K3" s="5" t="s">
         <v>9</v>
       </c>
-      <c r="K3" s="5" t="s">
+      <c r="L3" s="5" t="s">
         <v>10</v>
       </c>
-      <c r="L3" s="5" t="s">
+      <c r="M3" s="5" t="s">
         <v>11</v>
       </c>
-      <c r="M3" s="5" t="s">
+      <c r="N3" s="5" t="s">
         <v>12</v>
       </c>
-      <c r="N3" s="5" t="s">
+      <c r="O3" s="5" t="s">
         <v>13</v>
       </c>
-      <c r="O3" s="5" t="s">
+      <c r="P3" s="5" t="s">
         <v>14</v>
       </c>
-      <c r="P3" s="5" t="s">
+      <c r="Q3" s="5" t="s">
         <v>15</v>
       </c>
-      <c r="Q3" s="5" t="s">
+      <c r="R3" s="5" t="s">
         <v>16</v>
       </c>
-      <c r="R3" s="5" t="s">
+      <c r="S3" s="5" t="s">
         <v>17</v>
       </c>
-      <c r="S3" s="5" t="s">
+      <c r="T3" s="5" t="s">
         <v>18</v>
       </c>
     </row>
-    <row r="4" spans="1:19" x14ac:dyDescent="0.25">
+    <row r="4" spans="1:20" x14ac:dyDescent="0.25">
       <c r="C4" s="4" t="s">
         <v>221</v>
       </c>
-      <c r="D4" s="5" t="s">
-        <v>225</v>
-      </c>
+      <c r="D4" s="4"/>
       <c r="E4" s="5" t="s">
         <v>225</v>
       </c>
@@ -1555,14 +1577,15 @@
       <c r="S4" s="5" t="s">
         <v>225</v>
       </c>
-    </row>
-    <row r="5" spans="1:19" x14ac:dyDescent="0.25">
+      <c r="T4" s="5" t="s">
+        <v>225</v>
+      </c>
+    </row>
+    <row r="5" spans="1:20" x14ac:dyDescent="0.25">
       <c r="C5" s="4" t="s">
         <v>222</v>
       </c>
-      <c r="D5" s="5" t="s">
-        <v>226</v>
-      </c>
+      <c r="D5" s="4"/>
       <c r="E5" s="5" t="s">
         <v>226</v>
       </c>
@@ -1606,63 +1629,67 @@
         <v>226</v>
       </c>
       <c r="S5" s="5" t="s">
+        <v>226</v>
+      </c>
+      <c r="T5" s="5" t="s">
         <v>257</v>
       </c>
     </row>
-    <row r="6" spans="1:19" x14ac:dyDescent="0.25">
+    <row r="6" spans="1:20" x14ac:dyDescent="0.25">
       <c r="C6" s="4" t="s">
         <v>223</v>
       </c>
-      <c r="D6" s="5" t="s">
+      <c r="D6" s="4"/>
+      <c r="E6" s="5" t="s">
         <v>227</v>
       </c>
-      <c r="E6" s="5" t="s">
+      <c r="F6" s="5" t="s">
         <v>229</v>
       </c>
-      <c r="F6" s="5" t="s">
+      <c r="G6" s="5" t="s">
         <v>231</v>
       </c>
-      <c r="G6" s="5" t="s">
+      <c r="H6" s="5" t="s">
         <v>233</v>
       </c>
-      <c r="H6" s="5" t="s">
+      <c r="I6" s="5" t="s">
         <v>235</v>
       </c>
-      <c r="I6" s="5" t="s">
+      <c r="J6" s="5" t="s">
         <v>237</v>
       </c>
-      <c r="J6" s="5" t="s">
+      <c r="K6" s="5" t="s">
         <v>239</v>
       </c>
-      <c r="K6" s="5" t="s">
+      <c r="L6" s="5" t="s">
         <v>241</v>
       </c>
-      <c r="L6" s="5" t="s">
+      <c r="M6" s="5" t="s">
         <v>243</v>
       </c>
-      <c r="M6" s="5" t="s">
+      <c r="N6" s="5" t="s">
         <v>245</v>
       </c>
-      <c r="N6" s="5" t="s">
+      <c r="O6" s="5" t="s">
         <v>247</v>
       </c>
-      <c r="O6" s="5" t="s">
+      <c r="P6" s="5" t="s">
         <v>249</v>
       </c>
-      <c r="P6" s="5" t="s">
+      <c r="Q6" s="5" t="s">
         <v>251</v>
       </c>
-      <c r="Q6" s="5" t="s">
+      <c r="R6" s="5" t="s">
         <v>253</v>
       </c>
-      <c r="R6" s="5" t="s">
+      <c r="S6" s="5" t="s">
         <v>255</v>
       </c>
-      <c r="S6" s="5" t="s">
+      <c r="T6" s="5" t="s">
         <v>258</v>
       </c>
     </row>
-    <row r="7" spans="1:19" x14ac:dyDescent="0.25">
+    <row r="7" spans="1:20" x14ac:dyDescent="0.25">
       <c r="A7" s="3" t="s">
         <v>0</v>
       </c>
@@ -1672,7 +1699,9 @@
       <c r="C7" s="3" t="s">
         <v>2</v>
       </c>
-      <c r="D7" s="2"/>
+      <c r="D7" s="8" t="s">
+        <v>260</v>
+      </c>
       <c r="E7" s="2"/>
       <c r="F7" s="2"/>
       <c r="G7" s="2"/>
@@ -1688,8 +1717,9 @@
       <c r="Q7" s="2"/>
       <c r="R7" s="2"/>
       <c r="S7" s="2"/>
-    </row>
-    <row r="8" spans="1:19" x14ac:dyDescent="0.25">
+      <c r="T7" s="2"/>
+    </row>
+    <row r="8" spans="1:20" x14ac:dyDescent="0.25">
       <c r="A8" s="1" t="s">
         <v>19</v>
       </c>
@@ -1699,15 +1729,15 @@
       <c r="C8" s="1" t="s">
         <v>21</v>
       </c>
-      <c r="D8" s="1" t="s">
-        <v>22</v>
+      <c r="D8" s="1">
+        <v>410</v>
       </c>
       <c r="E8" s="1" t="s">
+        <v>22</v>
+      </c>
+      <c r="F8" s="1" t="s">
         <v>23</v>
       </c>
-      <c r="F8" s="1" t="s">
-        <v>22</v>
-      </c>
       <c r="G8" s="1" t="s">
         <v>22</v>
       </c>
@@ -1724,11 +1754,11 @@
         <v>22</v>
       </c>
       <c r="L8" s="1" t="s">
+        <v>22</v>
+      </c>
+      <c r="M8" s="1" t="s">
         <v>24</v>
       </c>
-      <c r="M8" s="1" t="s">
-        <v>22</v>
-      </c>
       <c r="N8" s="1" t="s">
         <v>22</v>
       </c>
@@ -1747,8 +1777,11 @@
       <c r="S8" s="1" t="s">
         <v>22</v>
       </c>
-    </row>
-    <row r="9" spans="1:19" x14ac:dyDescent="0.25">
+      <c r="T8" s="1" t="s">
+        <v>22</v>
+      </c>
+    </row>
+    <row r="9" spans="1:20" x14ac:dyDescent="0.25">
       <c r="A9" s="1" t="s">
         <v>19</v>
       </c>
@@ -1758,15 +1791,15 @@
       <c r="C9" s="1" t="s">
         <v>21</v>
       </c>
-      <c r="D9" s="1" t="s">
-        <v>22</v>
+      <c r="D9" s="1">
+        <v>1300</v>
       </c>
       <c r="E9" s="1" t="s">
+        <v>22</v>
+      </c>
+      <c r="F9" s="1" t="s">
         <v>23</v>
       </c>
-      <c r="F9" s="1" t="s">
-        <v>22</v>
-      </c>
       <c r="G9" s="1" t="s">
         <v>22</v>
       </c>
@@ -1783,11 +1816,11 @@
         <v>22</v>
       </c>
       <c r="L9" s="1" t="s">
+        <v>22</v>
+      </c>
+      <c r="M9" s="1" t="s">
         <v>26</v>
       </c>
-      <c r="M9" s="1" t="s">
-        <v>22</v>
-      </c>
       <c r="N9" s="1" t="s">
         <v>22</v>
       </c>
@@ -1806,8 +1839,11 @@
       <c r="S9" s="1" t="s">
         <v>22</v>
       </c>
-    </row>
-    <row r="10" spans="1:19" x14ac:dyDescent="0.25">
+      <c r="T9" s="1" t="s">
+        <v>22</v>
+      </c>
+    </row>
+    <row r="10" spans="1:20" x14ac:dyDescent="0.25">
       <c r="A10" s="1" t="s">
         <v>19</v>
       </c>
@@ -1817,15 +1853,15 @@
       <c r="C10" s="1" t="s">
         <v>21</v>
       </c>
-      <c r="D10" s="1" t="s">
-        <v>22</v>
+      <c r="D10" s="1">
+        <v>37000</v>
       </c>
       <c r="E10" s="1" t="s">
+        <v>22</v>
+      </c>
+      <c r="F10" s="1" t="s">
         <v>23</v>
       </c>
-      <c r="F10" s="1" t="s">
-        <v>22</v>
-      </c>
       <c r="G10" s="1" t="s">
         <v>22</v>
       </c>
@@ -1842,11 +1878,11 @@
         <v>22</v>
       </c>
       <c r="L10" s="1" t="s">
+        <v>22</v>
+      </c>
+      <c r="M10" s="1" t="s">
         <v>28</v>
       </c>
-      <c r="M10" s="1" t="s">
-        <v>22</v>
-      </c>
       <c r="N10" s="1" t="s">
         <v>22</v>
       </c>
@@ -1865,8 +1901,11 @@
       <c r="S10" s="1" t="s">
         <v>22</v>
       </c>
-    </row>
-    <row r="11" spans="1:19" x14ac:dyDescent="0.25">
+      <c r="T10" s="1" t="s">
+        <v>22</v>
+      </c>
+    </row>
+    <row r="11" spans="1:20" x14ac:dyDescent="0.25">
       <c r="A11" s="1" t="s">
         <v>19</v>
       </c>
@@ -1876,15 +1915,15 @@
       <c r="C11" s="1" t="s">
         <v>21</v>
       </c>
-      <c r="D11" s="1" t="s">
-        <v>22</v>
+      <c r="D11" s="1">
+        <v>18000</v>
       </c>
       <c r="E11" s="1" t="s">
+        <v>22</v>
+      </c>
+      <c r="F11" s="1" t="s">
         <v>23</v>
       </c>
-      <c r="F11" s="1" t="s">
-        <v>22</v>
-      </c>
       <c r="G11" s="1" t="s">
         <v>22</v>
       </c>
@@ -1901,11 +1940,11 @@
         <v>22</v>
       </c>
       <c r="L11" s="1" t="s">
+        <v>22</v>
+      </c>
+      <c r="M11" s="1" t="s">
         <v>30</v>
       </c>
-      <c r="M11" s="1" t="s">
-        <v>22</v>
-      </c>
       <c r="N11" s="1" t="s">
         <v>22</v>
       </c>
@@ -1924,8 +1963,11 @@
       <c r="S11" s="1" t="s">
         <v>22</v>
       </c>
-    </row>
-    <row r="12" spans="1:19" x14ac:dyDescent="0.25">
+      <c r="T11" s="1" t="s">
+        <v>22</v>
+      </c>
+    </row>
+    <row r="12" spans="1:20" x14ac:dyDescent="0.25">
       <c r="A12" s="1" t="s">
         <v>19</v>
       </c>
@@ -1935,15 +1977,15 @@
       <c r="C12" s="1" t="s">
         <v>21</v>
       </c>
-      <c r="D12" s="1" t="s">
-        <v>22</v>
+      <c r="D12" s="1">
+        <v>390000</v>
       </c>
       <c r="E12" s="1" t="s">
+        <v>22</v>
+      </c>
+      <c r="F12" s="1" t="s">
         <v>23</v>
       </c>
-      <c r="F12" s="1" t="s">
-        <v>22</v>
-      </c>
       <c r="G12" s="1" t="s">
         <v>22</v>
       </c>
@@ -1960,11 +2002,11 @@
         <v>22</v>
       </c>
       <c r="L12" s="1" t="s">
+        <v>22</v>
+      </c>
+      <c r="M12" s="1" t="s">
         <v>30</v>
       </c>
-      <c r="M12" s="1" t="s">
-        <v>22</v>
-      </c>
       <c r="N12" s="1" t="s">
         <v>22</v>
       </c>
@@ -1983,8 +2025,11 @@
       <c r="S12" s="1" t="s">
         <v>22</v>
       </c>
-    </row>
-    <row r="13" spans="1:19" x14ac:dyDescent="0.25">
+      <c r="T12" s="1" t="s">
+        <v>22</v>
+      </c>
+    </row>
+    <row r="13" spans="1:20" x14ac:dyDescent="0.25">
       <c r="A13" s="1" t="s">
         <v>19</v>
       </c>
@@ -1994,15 +2039,15 @@
       <c r="C13" s="1" t="s">
         <v>21</v>
       </c>
-      <c r="D13" s="1" t="s">
-        <v>22</v>
+      <c r="D13" s="1">
+        <v>280</v>
       </c>
       <c r="E13" s="1" t="s">
+        <v>22</v>
+      </c>
+      <c r="F13" s="1" t="s">
         <v>23</v>
       </c>
-      <c r="F13" s="1" t="s">
-        <v>22</v>
-      </c>
       <c r="G13" s="1" t="s">
         <v>22</v>
       </c>
@@ -2019,11 +2064,11 @@
         <v>22</v>
       </c>
       <c r="L13" s="1" t="s">
+        <v>22</v>
+      </c>
+      <c r="M13" s="1" t="s">
         <v>30</v>
       </c>
-      <c r="M13" s="1" t="s">
-        <v>22</v>
-      </c>
       <c r="N13" s="1" t="s">
         <v>22</v>
       </c>
@@ -2042,8 +2087,11 @@
       <c r="S13" s="1" t="s">
         <v>22</v>
       </c>
-    </row>
-    <row r="14" spans="1:19" x14ac:dyDescent="0.25">
+      <c r="T13" s="1" t="s">
+        <v>22</v>
+      </c>
+    </row>
+    <row r="14" spans="1:20" x14ac:dyDescent="0.25">
       <c r="A14" s="1" t="s">
         <v>19</v>
       </c>
@@ -2053,15 +2101,15 @@
       <c r="C14" s="1" t="s">
         <v>21</v>
       </c>
-      <c r="D14" s="1" t="s">
-        <v>22</v>
+      <c r="D14" s="1">
+        <v>270</v>
       </c>
       <c r="E14" s="1" t="s">
+        <v>22</v>
+      </c>
+      <c r="F14" s="1" t="s">
         <v>23</v>
       </c>
-      <c r="F14" s="1" t="s">
-        <v>22</v>
-      </c>
       <c r="G14" s="1" t="s">
         <v>22</v>
       </c>
@@ -2078,11 +2126,11 @@
         <v>22</v>
       </c>
       <c r="L14" s="1" t="s">
+        <v>22</v>
+      </c>
+      <c r="M14" s="1" t="s">
         <v>30</v>
       </c>
-      <c r="M14" s="1" t="s">
-        <v>22</v>
-      </c>
       <c r="N14" s="1" t="s">
         <v>22</v>
       </c>
@@ -2101,8 +2149,11 @@
       <c r="S14" s="1" t="s">
         <v>22</v>
       </c>
-    </row>
-    <row r="15" spans="1:19" x14ac:dyDescent="0.25">
+      <c r="T14" s="1" t="s">
+        <v>22</v>
+      </c>
+    </row>
+    <row r="15" spans="1:20" x14ac:dyDescent="0.25">
       <c r="A15" s="1" t="s">
         <v>19</v>
       </c>
@@ -2112,15 +2163,15 @@
       <c r="C15" s="1" t="s">
         <v>21</v>
       </c>
-      <c r="D15" s="1" t="s">
-        <v>22</v>
+      <c r="D15" s="1">
+        <v>2700</v>
       </c>
       <c r="E15" s="1" t="s">
+        <v>22</v>
+      </c>
+      <c r="F15" s="1" t="s">
         <v>23</v>
       </c>
-      <c r="F15" s="1" t="s">
-        <v>22</v>
-      </c>
       <c r="G15" s="1" t="s">
         <v>22</v>
       </c>
@@ -2137,11 +2188,11 @@
         <v>22</v>
       </c>
       <c r="L15" s="1" t="s">
+        <v>22</v>
+      </c>
+      <c r="M15" s="1" t="s">
         <v>30</v>
       </c>
-      <c r="M15" s="1" t="s">
-        <v>22</v>
-      </c>
       <c r="N15" s="1" t="s">
         <v>22</v>
       </c>
@@ -2160,8 +2211,11 @@
       <c r="S15" s="1" t="s">
         <v>22</v>
       </c>
-    </row>
-    <row r="16" spans="1:19" x14ac:dyDescent="0.25">
+      <c r="T15" s="1" t="s">
+        <v>22</v>
+      </c>
+    </row>
+    <row r="16" spans="1:20" x14ac:dyDescent="0.25">
       <c r="A16" s="1" t="s">
         <v>19</v>
       </c>
@@ -2171,15 +2225,15 @@
       <c r="C16" s="1" t="s">
         <v>21</v>
       </c>
-      <c r="D16" s="1" t="s">
-        <v>22</v>
+      <c r="D16" s="1">
+        <v>15000000</v>
       </c>
       <c r="E16" s="1" t="s">
+        <v>22</v>
+      </c>
+      <c r="F16" s="1" t="s">
         <v>23</v>
       </c>
-      <c r="F16" s="1" t="s">
-        <v>22</v>
-      </c>
       <c r="G16" s="1" t="s">
         <v>22</v>
       </c>
@@ -2196,11 +2250,11 @@
         <v>22</v>
       </c>
       <c r="L16" s="1" t="s">
+        <v>22</v>
+      </c>
+      <c r="M16" s="1" t="s">
         <v>30</v>
       </c>
-      <c r="M16" s="1" t="s">
-        <v>22</v>
-      </c>
       <c r="N16" s="1" t="s">
         <v>22</v>
       </c>
@@ -2219,8 +2273,11 @@
       <c r="S16" s="1" t="s">
         <v>22</v>
       </c>
-    </row>
-    <row r="17" spans="1:19" x14ac:dyDescent="0.25">
+      <c r="T16" s="1" t="s">
+        <v>22</v>
+      </c>
+    </row>
+    <row r="17" spans="1:20" x14ac:dyDescent="0.25">
       <c r="A17" s="1" t="s">
         <v>19</v>
       </c>
@@ -2230,15 +2287,15 @@
       <c r="C17" s="1" t="s">
         <v>21</v>
       </c>
-      <c r="D17" s="1" t="s">
-        <v>22</v>
+      <c r="D17" s="1">
+        <v>27000</v>
       </c>
       <c r="E17" s="1" t="s">
+        <v>22</v>
+      </c>
+      <c r="F17" s="1" t="s">
         <v>23</v>
       </c>
-      <c r="F17" s="1" t="s">
-        <v>22</v>
-      </c>
       <c r="G17" s="1" t="s">
         <v>22</v>
       </c>
@@ -2255,11 +2312,11 @@
         <v>22</v>
       </c>
       <c r="L17" s="1" t="s">
+        <v>22</v>
+      </c>
+      <c r="M17" s="1" t="s">
         <v>30</v>
       </c>
-      <c r="M17" s="1" t="s">
-        <v>22</v>
-      </c>
       <c r="N17" s="1" t="s">
         <v>22</v>
       </c>
@@ -2278,8 +2335,11 @@
       <c r="S17" s="1" t="s">
         <v>22</v>
       </c>
-    </row>
-    <row r="18" spans="1:19" x14ac:dyDescent="0.25">
+      <c r="T17" s="1" t="s">
+        <v>22</v>
+      </c>
+    </row>
+    <row r="18" spans="1:20" x14ac:dyDescent="0.25">
       <c r="A18" s="1" t="s">
         <v>19</v>
       </c>
@@ -2289,15 +2349,15 @@
       <c r="C18" s="1" t="s">
         <v>21</v>
       </c>
-      <c r="D18" s="1" t="s">
-        <v>22</v>
+      <c r="D18" s="1">
+        <v>82000</v>
       </c>
       <c r="E18" s="1" t="s">
+        <v>22</v>
+      </c>
+      <c r="F18" s="1" t="s">
         <v>23</v>
       </c>
-      <c r="F18" s="1" t="s">
-        <v>22</v>
-      </c>
       <c r="G18" s="1" t="s">
         <v>22</v>
       </c>
@@ -2314,11 +2374,11 @@
         <v>22</v>
       </c>
       <c r="L18" s="1" t="s">
+        <v>22</v>
+      </c>
+      <c r="M18" s="1" t="s">
         <v>30</v>
       </c>
-      <c r="M18" s="1" t="s">
-        <v>22</v>
-      </c>
       <c r="N18" s="1" t="s">
         <v>22</v>
       </c>
@@ -2337,8 +2397,11 @@
       <c r="S18" s="1" t="s">
         <v>22</v>
       </c>
-    </row>
-    <row r="19" spans="1:19" x14ac:dyDescent="0.25">
+      <c r="T18" s="1" t="s">
+        <v>22</v>
+      </c>
+    </row>
+    <row r="19" spans="1:20" x14ac:dyDescent="0.25">
       <c r="A19" s="1" t="s">
         <v>19</v>
       </c>
@@ -2348,15 +2411,15 @@
       <c r="C19" s="1" t="s">
         <v>21</v>
       </c>
-      <c r="D19" s="1" t="s">
-        <v>22</v>
+      <c r="D19" s="1">
+        <v>870</v>
       </c>
       <c r="E19" s="1" t="s">
+        <v>22</v>
+      </c>
+      <c r="F19" s="1" t="s">
         <v>23</v>
       </c>
-      <c r="F19" s="1" t="s">
-        <v>22</v>
-      </c>
       <c r="G19" s="1" t="s">
         <v>22</v>
       </c>
@@ -2373,11 +2436,11 @@
         <v>22</v>
       </c>
       <c r="L19" s="1" t="s">
+        <v>22</v>
+      </c>
+      <c r="M19" s="1" t="s">
         <v>30</v>
       </c>
-      <c r="M19" s="1" t="s">
-        <v>22</v>
-      </c>
       <c r="N19" s="1" t="s">
         <v>22</v>
       </c>
@@ -2396,8 +2459,11 @@
       <c r="S19" s="1" t="s">
         <v>22</v>
       </c>
-    </row>
-    <row r="20" spans="1:19" x14ac:dyDescent="0.25">
+      <c r="T19" s="1" t="s">
+        <v>22</v>
+      </c>
+    </row>
+    <row r="20" spans="1:20" x14ac:dyDescent="0.25">
       <c r="A20" s="1" t="s">
         <v>19</v>
       </c>
@@ -2407,15 +2473,15 @@
       <c r="C20" s="1" t="s">
         <v>21</v>
       </c>
-      <c r="D20" s="1" t="s">
-        <v>22</v>
+      <c r="D20" s="1">
+        <v>590000</v>
       </c>
       <c r="E20" s="1" t="s">
+        <v>22</v>
+      </c>
+      <c r="F20" s="1" t="s">
         <v>23</v>
       </c>
-      <c r="F20" s="1" t="s">
-        <v>22</v>
-      </c>
       <c r="G20" s="1" t="s">
         <v>22</v>
       </c>
@@ -2432,11 +2498,11 @@
         <v>22</v>
       </c>
       <c r="L20" s="1" t="s">
+        <v>22</v>
+      </c>
+      <c r="M20" s="1" t="s">
         <v>30</v>
       </c>
-      <c r="M20" s="1" t="s">
-        <v>22</v>
-      </c>
       <c r="N20" s="1" t="s">
         <v>22</v>
       </c>
@@ -2455,8 +2521,11 @@
       <c r="S20" s="1" t="s">
         <v>22</v>
       </c>
-    </row>
-    <row r="21" spans="1:19" x14ac:dyDescent="0.25">
+      <c r="T20" s="1" t="s">
+        <v>22</v>
+      </c>
+    </row>
+    <row r="21" spans="1:20" x14ac:dyDescent="0.25">
       <c r="A21" s="1" t="s">
         <v>19</v>
       </c>
@@ -2466,15 +2535,15 @@
       <c r="C21" s="1" t="s">
         <v>21</v>
       </c>
-      <c r="D21" s="1" t="s">
-        <v>22</v>
+      <c r="D21" s="1">
+        <v>36000</v>
       </c>
       <c r="E21" s="1" t="s">
+        <v>22</v>
+      </c>
+      <c r="F21" s="1" t="s">
         <v>23</v>
       </c>
-      <c r="F21" s="1" t="s">
-        <v>22</v>
-      </c>
       <c r="G21" s="1" t="s">
         <v>22</v>
       </c>
@@ -2491,11 +2560,11 @@
         <v>22</v>
       </c>
       <c r="L21" s="1" t="s">
+        <v>22</v>
+      </c>
+      <c r="M21" s="1" t="s">
         <v>41</v>
       </c>
-      <c r="M21" s="1" t="s">
-        <v>22</v>
-      </c>
       <c r="N21" s="1" t="s">
         <v>22</v>
       </c>
@@ -2514,8 +2583,11 @@
       <c r="S21" s="1" t="s">
         <v>22</v>
       </c>
-    </row>
-    <row r="22" spans="1:19" x14ac:dyDescent="0.25">
+      <c r="T21" s="1" t="s">
+        <v>22</v>
+      </c>
+    </row>
+    <row r="22" spans="1:20" x14ac:dyDescent="0.25">
       <c r="A22" s="1" t="s">
         <v>19</v>
       </c>
@@ -2525,15 +2597,15 @@
       <c r="C22" s="1" t="s">
         <v>21</v>
       </c>
-      <c r="D22" s="1" t="s">
-        <v>22</v>
+      <c r="D22" s="1">
+        <v>8800</v>
       </c>
       <c r="E22" s="1" t="s">
+        <v>22</v>
+      </c>
+      <c r="F22" s="1" t="s">
         <v>23</v>
       </c>
-      <c r="F22" s="1" t="s">
-        <v>22</v>
-      </c>
       <c r="G22" s="1" t="s">
         <v>22</v>
       </c>
@@ -2550,11 +2622,11 @@
         <v>22</v>
       </c>
       <c r="L22" s="1" t="s">
+        <v>22</v>
+      </c>
+      <c r="M22" s="1" t="s">
         <v>30</v>
       </c>
-      <c r="M22" s="1" t="s">
-        <v>22</v>
-      </c>
       <c r="N22" s="1" t="s">
         <v>22</v>
       </c>
@@ -2573,8 +2645,11 @@
       <c r="S22" s="1" t="s">
         <v>22</v>
       </c>
-    </row>
-    <row r="23" spans="1:19" x14ac:dyDescent="0.25">
+      <c r="T22" s="1" t="s">
+        <v>22</v>
+      </c>
+    </row>
+    <row r="23" spans="1:20" x14ac:dyDescent="0.25">
       <c r="A23" s="1" t="s">
         <v>19</v>
       </c>
@@ -2584,15 +2659,15 @@
       <c r="C23" s="1" t="s">
         <v>21</v>
       </c>
-      <c r="D23" s="1" t="s">
-        <v>22</v>
+      <c r="D23" s="1">
+        <v>38</v>
       </c>
       <c r="E23" s="1" t="s">
+        <v>22</v>
+      </c>
+      <c r="F23" s="1" t="s">
         <v>44</v>
       </c>
-      <c r="F23" s="1" t="s">
-        <v>22</v>
-      </c>
       <c r="G23" s="1" t="s">
         <v>22</v>
       </c>
@@ -2609,11 +2684,11 @@
         <v>22</v>
       </c>
       <c r="L23" s="1" t="s">
+        <v>22</v>
+      </c>
+      <c r="M23" s="1" t="s">
         <v>45</v>
       </c>
-      <c r="M23" s="1" t="s">
-        <v>22</v>
-      </c>
       <c r="N23" s="1" t="s">
         <v>22</v>
       </c>
@@ -2632,8 +2707,11 @@
       <c r="S23" s="1" t="s">
         <v>22</v>
       </c>
-    </row>
-    <row r="24" spans="1:19" x14ac:dyDescent="0.25">
+      <c r="T23" s="1" t="s">
+        <v>22</v>
+      </c>
+    </row>
+    <row r="24" spans="1:20" x14ac:dyDescent="0.25">
       <c r="A24" s="1" t="s">
         <v>19</v>
       </c>
@@ -2643,15 +2721,15 @@
       <c r="C24" s="1" t="s">
         <v>21</v>
       </c>
-      <c r="D24" s="1" t="s">
-        <v>22</v>
+      <c r="D24" s="1">
+        <v>39000</v>
       </c>
       <c r="E24" s="1" t="s">
+        <v>22</v>
+      </c>
+      <c r="F24" s="1" t="s">
         <v>23</v>
       </c>
-      <c r="F24" s="1" t="s">
-        <v>22</v>
-      </c>
       <c r="G24" s="1" t="s">
         <v>22</v>
       </c>
@@ -2668,11 +2746,11 @@
         <v>22</v>
       </c>
       <c r="L24" s="1" t="s">
+        <v>22</v>
+      </c>
+      <c r="M24" s="1" t="s">
         <v>47</v>
       </c>
-      <c r="M24" s="1" t="s">
-        <v>22</v>
-      </c>
       <c r="N24" s="1" t="s">
         <v>22</v>
       </c>
@@ -2691,8 +2769,11 @@
       <c r="S24" s="1" t="s">
         <v>22</v>
       </c>
-    </row>
-    <row r="25" spans="1:19" x14ac:dyDescent="0.25">
+      <c r="T24" s="1" t="s">
+        <v>22</v>
+      </c>
+    </row>
+    <row r="25" spans="1:20" x14ac:dyDescent="0.25">
       <c r="A25" s="1" t="s">
         <v>19</v>
       </c>
@@ -2702,15 +2783,15 @@
       <c r="C25" s="1" t="s">
         <v>21</v>
       </c>
-      <c r="D25" s="1" t="s">
-        <v>22</v>
+      <c r="D25" s="1">
+        <v>87000</v>
       </c>
       <c r="E25" s="1" t="s">
+        <v>22</v>
+      </c>
+      <c r="F25" s="1" t="s">
         <v>23</v>
       </c>
-      <c r="F25" s="1" t="s">
-        <v>22</v>
-      </c>
       <c r="G25" s="1" t="s">
         <v>22</v>
       </c>
@@ -2727,11 +2808,11 @@
         <v>22</v>
       </c>
       <c r="L25" s="1" t="s">
+        <v>22</v>
+      </c>
+      <c r="M25" s="1" t="s">
         <v>30</v>
       </c>
-      <c r="M25" s="1" t="s">
-        <v>22</v>
-      </c>
       <c r="N25" s="1" t="s">
         <v>22</v>
       </c>
@@ -2750,8 +2831,11 @@
       <c r="S25" s="1" t="s">
         <v>22</v>
       </c>
-    </row>
-    <row r="26" spans="1:19" x14ac:dyDescent="0.25">
+      <c r="T25" s="1" t="s">
+        <v>22</v>
+      </c>
+    </row>
+    <row r="26" spans="1:20" x14ac:dyDescent="0.25">
       <c r="A26" s="1" t="s">
         <v>49</v>
       </c>
@@ -2761,42 +2845,42 @@
       <c r="C26" s="1" t="s">
         <v>51</v>
       </c>
-      <c r="D26" s="1" t="s">
+      <c r="D26" s="1">
+        <v>300</v>
+      </c>
+      <c r="E26" s="1" t="s">
         <v>52</v>
       </c>
-      <c r="E26" s="1" t="s">
+      <c r="F26" s="1" t="s">
         <v>53</v>
       </c>
-      <c r="F26" s="1" t="s">
+      <c r="G26" s="1" t="s">
         <v>54</v>
       </c>
-      <c r="G26" s="1" t="s">
+      <c r="H26" s="1" t="s">
         <v>55</v>
       </c>
-      <c r="H26" s="1" t="s">
+      <c r="I26" s="1" t="s">
         <v>56</v>
       </c>
-      <c r="I26" s="1" t="s">
+      <c r="J26" s="1" t="s">
         <v>57</v>
       </c>
-      <c r="J26" s="1" t="s">
+      <c r="K26" s="1" t="s">
         <v>58</v>
       </c>
-      <c r="K26" s="1" t="s">
+      <c r="L26" s="1" t="s">
         <v>59</v>
       </c>
-      <c r="L26" s="1" t="s">
+      <c r="M26" s="1" t="s">
         <v>60</v>
       </c>
-      <c r="M26" s="1" t="s">
+      <c r="N26" s="1" t="s">
         <v>61</v>
       </c>
-      <c r="N26" s="1" t="s">
+      <c r="O26" s="1" t="s">
         <v>62</v>
       </c>
-      <c r="O26" s="1" t="s">
-        <v>22</v>
-      </c>
       <c r="P26" s="1" t="s">
         <v>22</v>
       </c>
@@ -2804,13 +2888,16 @@
         <v>22</v>
       </c>
       <c r="R26" s="1" t="s">
+        <v>22</v>
+      </c>
+      <c r="S26" s="1" t="s">
         <v>63</v>
       </c>
-      <c r="S26" s="1" t="s">
+      <c r="T26" s="1" t="s">
         <v>64</v>
       </c>
     </row>
-    <row r="27" spans="1:19" x14ac:dyDescent="0.25">
+    <row r="27" spans="1:20" x14ac:dyDescent="0.25">
       <c r="A27" s="1" t="s">
         <v>65</v>
       </c>
@@ -2820,7 +2907,7 @@
       <c r="C27" s="1" t="s">
         <v>21</v>
       </c>
-      <c r="D27" s="1" t="s">
+      <c r="D27" s="1">
         <v>22</v>
       </c>
       <c r="E27" s="1" t="s">
@@ -2854,22 +2941,25 @@
         <v>22</v>
       </c>
       <c r="O27" s="1" t="s">
+        <v>22</v>
+      </c>
+      <c r="P27" s="1" t="s">
         <v>67</v>
       </c>
-      <c r="P27" s="1" t="s">
+      <c r="Q27" s="1" t="s">
         <v>68</v>
       </c>
-      <c r="Q27" s="1" t="s">
+      <c r="R27" s="1" t="s">
         <v>69</v>
       </c>
-      <c r="R27" s="1" t="s">
-        <v>22</v>
-      </c>
       <c r="S27" s="1" t="s">
         <v>22</v>
       </c>
-    </row>
-    <row r="28" spans="1:19" x14ac:dyDescent="0.25">
+      <c r="T27" s="1" t="s">
+        <v>22</v>
+      </c>
+    </row>
+    <row r="28" spans="1:20" x14ac:dyDescent="0.25">
       <c r="A28" s="1" t="s">
         <v>65</v>
       </c>
@@ -2879,8 +2969,8 @@
       <c r="C28" s="1" t="s">
         <v>21</v>
       </c>
-      <c r="D28" s="1" t="s">
-        <v>22</v>
+      <c r="D28" s="1">
+        <v>130</v>
       </c>
       <c r="E28" s="1" t="s">
         <v>22</v>
@@ -2913,22 +3003,25 @@
         <v>22</v>
       </c>
       <c r="O28" s="1" t="s">
+        <v>22</v>
+      </c>
+      <c r="P28" s="1" t="s">
         <v>71</v>
       </c>
-      <c r="P28" s="1" t="s">
+      <c r="Q28" s="1" t="s">
         <v>72</v>
       </c>
-      <c r="Q28" s="1" t="s">
+      <c r="R28" s="1" t="s">
         <v>73</v>
       </c>
-      <c r="R28" s="1" t="s">
-        <v>22</v>
-      </c>
       <c r="S28" s="1" t="s">
         <v>22</v>
       </c>
-    </row>
-    <row r="29" spans="1:19" x14ac:dyDescent="0.25">
+      <c r="T28" s="1" t="s">
+        <v>22</v>
+      </c>
+    </row>
+    <row r="29" spans="1:20" x14ac:dyDescent="0.25">
       <c r="A29" s="1" t="s">
         <v>65</v>
       </c>
@@ -2938,8 +3031,8 @@
       <c r="C29" s="1" t="s">
         <v>51</v>
       </c>
-      <c r="D29" s="1" t="s">
-        <v>22</v>
+      <c r="D29" s="1">
+        <v>300</v>
       </c>
       <c r="E29" s="1" t="s">
         <v>22</v>
@@ -2972,22 +3065,25 @@
         <v>22</v>
       </c>
       <c r="O29" s="1" t="s">
+        <v>22</v>
+      </c>
+      <c r="P29" s="1" t="s">
         <v>74</v>
       </c>
-      <c r="P29" s="1" t="s">
+      <c r="Q29" s="1" t="s">
         <v>75</v>
       </c>
-      <c r="Q29" s="1" t="s">
+      <c r="R29" s="1" t="s">
         <v>76</v>
       </c>
-      <c r="R29" s="1" t="s">
-        <v>22</v>
-      </c>
       <c r="S29" s="1" t="s">
         <v>22</v>
       </c>
-    </row>
-    <row r="30" spans="1:19" x14ac:dyDescent="0.25">
+      <c r="T29" s="1" t="s">
+        <v>22</v>
+      </c>
+    </row>
+    <row r="30" spans="1:20" x14ac:dyDescent="0.25">
       <c r="A30" s="1" t="s">
         <v>65</v>
       </c>
@@ -2997,9 +3093,7 @@
       <c r="C30" s="1" t="s">
         <v>21</v>
       </c>
-      <c r="D30" s="1" t="s">
-        <v>22</v>
-      </c>
+      <c r="D30" s="1"/>
       <c r="E30" s="1" t="s">
         <v>22</v>
       </c>
@@ -3031,22 +3125,25 @@
         <v>22</v>
       </c>
       <c r="O30" s="1" t="s">
+        <v>22</v>
+      </c>
+      <c r="P30" s="1" t="s">
         <v>78</v>
       </c>
-      <c r="P30" s="1" t="s">
+      <c r="Q30" s="1" t="s">
         <v>79</v>
       </c>
-      <c r="Q30" s="1" t="s">
+      <c r="R30" s="1" t="s">
         <v>80</v>
       </c>
-      <c r="R30" s="1" t="s">
-        <v>22</v>
-      </c>
       <c r="S30" s="1" t="s">
         <v>22</v>
       </c>
-    </row>
-    <row r="31" spans="1:19" x14ac:dyDescent="0.25">
+      <c r="T30" s="1" t="s">
+        <v>22</v>
+      </c>
+    </row>
+    <row r="31" spans="1:20" x14ac:dyDescent="0.25">
       <c r="A31" s="1" t="s">
         <v>65</v>
       </c>
@@ -3056,8 +3153,8 @@
       <c r="C31" s="1" t="s">
         <v>21</v>
       </c>
-      <c r="D31" s="1" t="s">
-        <v>22</v>
+      <c r="D31" s="1">
+        <v>6700</v>
       </c>
       <c r="E31" s="1" t="s">
         <v>22</v>
@@ -3090,22 +3187,25 @@
         <v>22</v>
       </c>
       <c r="O31" s="1" t="s">
+        <v>22</v>
+      </c>
+      <c r="P31" s="1" t="s">
         <v>71</v>
       </c>
-      <c r="P31" s="1" t="s">
+      <c r="Q31" s="1" t="s">
         <v>82</v>
       </c>
-      <c r="Q31" s="1" t="s">
+      <c r="R31" s="1" t="s">
         <v>73</v>
       </c>
-      <c r="R31" s="1" t="s">
-        <v>22</v>
-      </c>
       <c r="S31" s="1" t="s">
         <v>22</v>
       </c>
-    </row>
-    <row r="32" spans="1:19" x14ac:dyDescent="0.25">
+      <c r="T31" s="1" t="s">
+        <v>22</v>
+      </c>
+    </row>
+    <row r="32" spans="1:20" x14ac:dyDescent="0.25">
       <c r="A32" s="1" t="s">
         <v>65</v>
       </c>
@@ -3115,9 +3215,7 @@
       <c r="C32" s="1" t="s">
         <v>21</v>
       </c>
-      <c r="D32" s="1" t="s">
-        <v>22</v>
-      </c>
+      <c r="D32" s="1"/>
       <c r="E32" s="1" t="s">
         <v>22</v>
       </c>
@@ -3149,22 +3247,25 @@
         <v>22</v>
       </c>
       <c r="O32" s="1" t="s">
+        <v>22</v>
+      </c>
+      <c r="P32" s="1" t="s">
         <v>71</v>
       </c>
-      <c r="P32" s="1" t="s">
+      <c r="Q32" s="1" t="s">
         <v>84</v>
       </c>
-      <c r="Q32" s="1" t="s">
+      <c r="R32" s="1" t="s">
         <v>73</v>
       </c>
-      <c r="R32" s="1" t="s">
-        <v>22</v>
-      </c>
       <c r="S32" s="1" t="s">
         <v>22</v>
       </c>
-    </row>
-    <row r="33" spans="1:19" x14ac:dyDescent="0.25">
+      <c r="T32" s="1" t="s">
+        <v>22</v>
+      </c>
+    </row>
+    <row r="33" spans="1:20" x14ac:dyDescent="0.25">
       <c r="A33" s="1" t="s">
         <v>85</v>
       </c>
@@ -3174,56 +3275,59 @@
       <c r="C33" s="1" t="s">
         <v>51</v>
       </c>
-      <c r="D33" s="1" t="s">
+      <c r="D33" s="1">
+        <v>250</v>
+      </c>
+      <c r="E33" s="1" t="s">
         <v>87</v>
       </c>
-      <c r="E33" s="1" t="s">
+      <c r="F33" s="1" t="s">
         <v>88</v>
       </c>
-      <c r="F33" s="1" t="s">
+      <c r="G33" s="1" t="s">
         <v>89</v>
       </c>
-      <c r="G33" s="1" t="s">
+      <c r="H33" s="1" t="s">
         <v>90</v>
       </c>
-      <c r="H33" s="1" t="s">
+      <c r="I33" s="1" t="s">
         <v>91</v>
       </c>
-      <c r="I33" s="1" t="s">
+      <c r="J33" s="1" t="s">
         <v>92</v>
       </c>
-      <c r="J33" s="1" t="s">
+      <c r="K33" s="1" t="s">
         <v>93</v>
       </c>
-      <c r="K33" s="1" t="s">
+      <c r="L33" s="1" t="s">
         <v>94</v>
       </c>
-      <c r="L33" s="1" t="s">
+      <c r="M33" s="1" t="s">
         <v>95</v>
       </c>
-      <c r="M33" s="1" t="s">
+      <c r="N33" s="1" t="s">
         <v>87</v>
       </c>
-      <c r="N33" s="1" t="s">
+      <c r="O33" s="1" t="s">
         <v>96</v>
       </c>
-      <c r="O33" s="1" t="s">
+      <c r="P33" s="1" t="s">
         <v>93</v>
-      </c>
-      <c r="P33" s="1" t="s">
-        <v>97</v>
       </c>
       <c r="Q33" s="1" t="s">
         <v>97</v>
       </c>
       <c r="R33" s="1" t="s">
+        <v>97</v>
+      </c>
+      <c r="S33" s="1" t="s">
         <v>93</v>
       </c>
-      <c r="S33" s="1" t="s">
-        <v>22</v>
-      </c>
-    </row>
-    <row r="34" spans="1:19" x14ac:dyDescent="0.25">
+      <c r="T33" s="1" t="s">
+        <v>22</v>
+      </c>
+    </row>
+    <row r="34" spans="1:20" x14ac:dyDescent="0.25">
       <c r="A34" s="1" t="s">
         <v>98</v>
       </c>
@@ -3233,56 +3337,57 @@
       <c r="C34" s="1" t="s">
         <v>100</v>
       </c>
-      <c r="D34" s="1" t="s">
+      <c r="D34" s="1"/>
+      <c r="E34" s="1" t="s">
         <v>101</v>
       </c>
-      <c r="E34" s="1" t="s">
+      <c r="F34" s="1" t="s">
         <v>102</v>
       </c>
-      <c r="F34" s="1" t="s">
+      <c r="G34" s="1" t="s">
         <v>103</v>
-      </c>
-      <c r="G34" s="1" t="s">
-        <v>104</v>
       </c>
       <c r="H34" s="1" t="s">
         <v>104</v>
       </c>
       <c r="I34" s="1" t="s">
+        <v>104</v>
+      </c>
+      <c r="J34" s="1" t="s">
         <v>105</v>
       </c>
-      <c r="J34" s="1" t="s">
+      <c r="K34" s="1" t="s">
         <v>106</v>
       </c>
-      <c r="K34" s="1" t="s">
+      <c r="L34" s="1" t="s">
         <v>107</v>
       </c>
-      <c r="L34" s="1" t="s">
+      <c r="M34" s="1" t="s">
         <v>108</v>
       </c>
-      <c r="M34" s="1" t="s">
+      <c r="N34" s="1" t="s">
         <v>109</v>
       </c>
-      <c r="N34" s="1" t="s">
+      <c r="O34" s="1" t="s">
         <v>110</v>
       </c>
-      <c r="O34" s="1" t="s">
+      <c r="P34" s="1" t="s">
         <v>104</v>
       </c>
-      <c r="P34" s="1" t="s">
+      <c r="Q34" s="1" t="s">
         <v>111</v>
       </c>
-      <c r="Q34" s="1" t="s">
+      <c r="R34" s="1" t="s">
         <v>106</v>
       </c>
-      <c r="R34" s="1" t="s">
+      <c r="S34" s="1" t="s">
         <v>112</v>
       </c>
-      <c r="S34" s="1" t="s">
-        <v>22</v>
-      </c>
-    </row>
-    <row r="35" spans="1:19" x14ac:dyDescent="0.25">
+      <c r="T34" s="1" t="s">
+        <v>22</v>
+      </c>
+    </row>
+    <row r="35" spans="1:20" x14ac:dyDescent="0.25">
       <c r="A35" s="1" t="s">
         <v>113</v>
       </c>
@@ -3292,42 +3397,42 @@
       <c r="C35" s="1" t="s">
         <v>21</v>
       </c>
-      <c r="D35" s="1" t="s">
+      <c r="D35" s="1">
+        <v>160</v>
+      </c>
+      <c r="E35" s="1" t="s">
         <v>115</v>
       </c>
-      <c r="E35" s="1" t="s">
+      <c r="F35" s="1" t="s">
         <v>116</v>
       </c>
-      <c r="F35" s="1" t="s">
+      <c r="G35" s="1" t="s">
         <v>117</v>
       </c>
-      <c r="G35" s="1" t="s">
+      <c r="H35" s="1" t="s">
         <v>118</v>
       </c>
-      <c r="H35" s="1" t="s">
+      <c r="I35" s="1" t="s">
         <v>119</v>
       </c>
-      <c r="I35" s="1" t="s">
+      <c r="J35" s="1" t="s">
         <v>120</v>
       </c>
-      <c r="J35" s="1" t="s">
+      <c r="K35" s="1" t="s">
         <v>121</v>
       </c>
-      <c r="K35" s="1" t="s">
+      <c r="L35" s="1" t="s">
         <v>122</v>
       </c>
-      <c r="L35" s="1" t="s">
+      <c r="M35" s="1" t="s">
         <v>123</v>
       </c>
-      <c r="M35" s="1" t="s">
+      <c r="N35" s="1" t="s">
         <v>124</v>
       </c>
-      <c r="N35" s="1" t="s">
+      <c r="O35" s="1" t="s">
         <v>125</v>
       </c>
-      <c r="O35" s="1" t="s">
-        <v>22</v>
-      </c>
       <c r="P35" s="1" t="s">
         <v>22</v>
       </c>
@@ -3335,13 +3440,16 @@
         <v>22</v>
       </c>
       <c r="R35" s="1" t="s">
+        <v>22</v>
+      </c>
+      <c r="S35" s="1" t="s">
         <v>126</v>
       </c>
-      <c r="S35" s="1" t="s">
+      <c r="T35" s="1" t="s">
         <v>127</v>
       </c>
     </row>
-    <row r="36" spans="1:19" x14ac:dyDescent="0.25">
+    <row r="36" spans="1:20" x14ac:dyDescent="0.25">
       <c r="A36" s="1" t="s">
         <v>113</v>
       </c>
@@ -3351,42 +3459,42 @@
       <c r="C36" s="1" t="s">
         <v>21</v>
       </c>
-      <c r="D36" s="1" t="s">
+      <c r="D36" s="1">
+        <v>0.24000000000000002</v>
+      </c>
+      <c r="E36" s="1" t="s">
         <v>129</v>
       </c>
-      <c r="E36" s="1" t="s">
+      <c r="F36" s="1" t="s">
         <v>130</v>
       </c>
-      <c r="F36" s="1" t="s">
+      <c r="G36" s="1" t="s">
         <v>131</v>
       </c>
-      <c r="G36" s="1" t="s">
+      <c r="H36" s="1" t="s">
         <v>132</v>
       </c>
-      <c r="H36" s="1" t="s">
+      <c r="I36" s="1" t="s">
         <v>133</v>
       </c>
-      <c r="I36" s="1" t="s">
+      <c r="J36" s="1" t="s">
         <v>134</v>
       </c>
-      <c r="J36" s="1" t="s">
+      <c r="K36" s="1" t="s">
         <v>135</v>
       </c>
-      <c r="K36" s="1" t="s">
+      <c r="L36" s="1" t="s">
         <v>136</v>
       </c>
-      <c r="L36" s="1" t="s">
+      <c r="M36" s="1" t="s">
         <v>137</v>
       </c>
-      <c r="M36" s="1" t="s">
+      <c r="N36" s="1" t="s">
         <v>138</v>
       </c>
-      <c r="N36" s="1" t="s">
+      <c r="O36" s="1" t="s">
         <v>139</v>
       </c>
-      <c r="O36" s="1" t="s">
-        <v>22</v>
-      </c>
       <c r="P36" s="1" t="s">
         <v>22</v>
       </c>
@@ -3394,13 +3502,16 @@
         <v>22</v>
       </c>
       <c r="R36" s="1" t="s">
+        <v>22</v>
+      </c>
+      <c r="S36" s="1" t="s">
         <v>140</v>
       </c>
-      <c r="S36" s="1" t="s">
+      <c r="T36" s="1" t="s">
         <v>141</v>
       </c>
     </row>
-    <row r="37" spans="1:19" x14ac:dyDescent="0.25">
+    <row r="37" spans="1:20" x14ac:dyDescent="0.25">
       <c r="A37" s="1" t="s">
         <v>113</v>
       </c>
@@ -3410,42 +3521,42 @@
       <c r="C37" s="1" t="s">
         <v>21</v>
       </c>
-      <c r="D37" s="1" t="s">
+      <c r="D37" s="1">
+        <v>5.5</v>
+      </c>
+      <c r="E37" s="1" t="s">
         <v>129</v>
       </c>
-      <c r="E37" s="1" t="s">
+      <c r="F37" s="1" t="s">
         <v>130</v>
       </c>
-      <c r="F37" s="1" t="s">
+      <c r="G37" s="1" t="s">
         <v>131</v>
       </c>
-      <c r="G37" s="1" t="s">
+      <c r="H37" s="1" t="s">
         <v>132</v>
       </c>
-      <c r="H37" s="1" t="s">
+      <c r="I37" s="1" t="s">
         <v>133</v>
       </c>
-      <c r="I37" s="1" t="s">
+      <c r="J37" s="1" t="s">
         <v>134</v>
       </c>
-      <c r="J37" s="1" t="s">
+      <c r="K37" s="1" t="s">
         <v>135</v>
       </c>
-      <c r="K37" s="1" t="s">
+      <c r="L37" s="1" t="s">
         <v>136</v>
       </c>
-      <c r="L37" s="1" t="s">
+      <c r="M37" s="1" t="s">
         <v>137</v>
       </c>
-      <c r="M37" s="1" t="s">
+      <c r="N37" s="1" t="s">
         <v>138</v>
       </c>
-      <c r="N37" s="1" t="s">
+      <c r="O37" s="1" t="s">
         <v>143</v>
       </c>
-      <c r="O37" s="1" t="s">
-        <v>22</v>
-      </c>
       <c r="P37" s="1" t="s">
         <v>22</v>
       </c>
@@ -3453,13 +3564,16 @@
         <v>22</v>
       </c>
       <c r="R37" s="1" t="s">
+        <v>22</v>
+      </c>
+      <c r="S37" s="1" t="s">
         <v>140</v>
       </c>
-      <c r="S37" s="1" t="s">
+      <c r="T37" s="1" t="s">
         <v>141</v>
       </c>
     </row>
-    <row r="38" spans="1:19" x14ac:dyDescent="0.25">
+    <row r="38" spans="1:20" x14ac:dyDescent="0.25">
       <c r="A38" s="1" t="s">
         <v>113</v>
       </c>
@@ -3469,42 +3583,42 @@
       <c r="C38" s="1" t="s">
         <v>21</v>
       </c>
-      <c r="D38" s="1" t="s">
+      <c r="D38" s="1">
+        <v>1300</v>
+      </c>
+      <c r="E38" s="1" t="s">
         <v>145</v>
       </c>
-      <c r="E38" s="1" t="s">
+      <c r="F38" s="1" t="s">
         <v>146</v>
       </c>
-      <c r="F38" s="1" t="s">
+      <c r="G38" s="1" t="s">
         <v>147</v>
       </c>
-      <c r="G38" s="1" t="s">
+      <c r="H38" s="1" t="s">
         <v>148</v>
       </c>
-      <c r="H38" s="1" t="s">
+      <c r="I38" s="1" t="s">
         <v>149</v>
       </c>
-      <c r="I38" s="1" t="s">
+      <c r="J38" s="1" t="s">
         <v>150</v>
       </c>
-      <c r="J38" s="1" t="s">
+      <c r="K38" s="1" t="s">
         <v>151</v>
       </c>
-      <c r="K38" s="1" t="s">
+      <c r="L38" s="1" t="s">
         <v>152</v>
       </c>
-      <c r="L38" s="1" t="s">
+      <c r="M38" s="1" t="s">
         <v>153</v>
       </c>
-      <c r="M38" s="1" t="s">
+      <c r="N38" s="1" t="s">
         <v>154</v>
       </c>
-      <c r="N38" s="1" t="s">
+      <c r="O38" s="1" t="s">
         <v>155</v>
       </c>
-      <c r="O38" s="1" t="s">
-        <v>22</v>
-      </c>
       <c r="P38" s="1" t="s">
         <v>22</v>
       </c>
@@ -3512,13 +3626,16 @@
         <v>22</v>
       </c>
       <c r="R38" s="1" t="s">
+        <v>22</v>
+      </c>
+      <c r="S38" s="1" t="s">
         <v>156</v>
       </c>
-      <c r="S38" s="1" t="s">
+      <c r="T38" s="1" t="s">
         <v>157</v>
       </c>
     </row>
-    <row r="39" spans="1:19" x14ac:dyDescent="0.25">
+    <row r="39" spans="1:20" x14ac:dyDescent="0.25">
       <c r="A39" s="1" t="s">
         <v>113</v>
       </c>
@@ -3528,42 +3645,42 @@
       <c r="C39" s="1" t="s">
         <v>21</v>
       </c>
-      <c r="D39" s="1" t="s">
+      <c r="D39" s="1">
+        <v>22</v>
+      </c>
+      <c r="E39" s="1" t="s">
         <v>158</v>
       </c>
-      <c r="E39" s="1" t="s">
+      <c r="F39" s="1" t="s">
         <v>159</v>
       </c>
-      <c r="F39" s="1" t="s">
+      <c r="G39" s="1" t="s">
         <v>160</v>
       </c>
-      <c r="G39" s="1" t="s">
+      <c r="H39" s="1" t="s">
         <v>161</v>
       </c>
-      <c r="H39" s="1" t="s">
+      <c r="I39" s="1" t="s">
         <v>162</v>
       </c>
-      <c r="I39" s="1" t="s">
+      <c r="J39" s="1" t="s">
         <v>163</v>
       </c>
-      <c r="J39" s="1" t="s">
+      <c r="K39" s="1" t="s">
         <v>164</v>
       </c>
-      <c r="K39" s="1" t="s">
+      <c r="L39" s="1" t="s">
         <v>165</v>
       </c>
-      <c r="L39" s="1" t="s">
+      <c r="M39" s="1" t="s">
         <v>166</v>
       </c>
-      <c r="M39" s="1" t="s">
+      <c r="N39" s="1" t="s">
         <v>167</v>
       </c>
-      <c r="N39" s="1" t="s">
+      <c r="O39" s="1" t="s">
         <v>168</v>
       </c>
-      <c r="O39" s="1" t="s">
-        <v>22</v>
-      </c>
       <c r="P39" s="1" t="s">
         <v>22</v>
       </c>
@@ -3571,13 +3688,16 @@
         <v>22</v>
       </c>
       <c r="R39" s="1" t="s">
+        <v>22</v>
+      </c>
+      <c r="S39" s="1" t="s">
         <v>169</v>
       </c>
-      <c r="S39" s="1" t="s">
+      <c r="T39" s="1" t="s">
         <v>156</v>
       </c>
     </row>
-    <row r="40" spans="1:19" x14ac:dyDescent="0.25">
+    <row r="40" spans="1:20" x14ac:dyDescent="0.25">
       <c r="A40" s="1" t="s">
         <v>113</v>
       </c>
@@ -3587,42 +3707,42 @@
       <c r="C40" s="1" t="s">
         <v>21</v>
       </c>
-      <c r="D40" s="1" t="s">
+      <c r="D40" s="1">
+        <v>130</v>
+      </c>
+      <c r="E40" s="1" t="s">
         <v>145</v>
       </c>
-      <c r="E40" s="1" t="s">
+      <c r="F40" s="1" t="s">
         <v>170</v>
       </c>
-      <c r="F40" s="1" t="s">
+      <c r="G40" s="1" t="s">
         <v>147</v>
       </c>
-      <c r="G40" s="1" t="s">
+      <c r="H40" s="1" t="s">
         <v>171</v>
       </c>
-      <c r="H40" s="1" t="s">
+      <c r="I40" s="1" t="s">
         <v>149</v>
       </c>
-      <c r="I40" s="1" t="s">
+      <c r="J40" s="1" t="s">
         <v>150</v>
       </c>
-      <c r="J40" s="1" t="s">
+      <c r="K40" s="1" t="s">
         <v>151</v>
       </c>
-      <c r="K40" s="1" t="s">
+      <c r="L40" s="1" t="s">
         <v>172</v>
       </c>
-      <c r="L40" s="1" t="s">
+      <c r="M40" s="1" t="s">
         <v>173</v>
       </c>
-      <c r="M40" s="1" t="s">
+      <c r="N40" s="1" t="s">
         <v>174</v>
       </c>
-      <c r="N40" s="1" t="s">
+      <c r="O40" s="1" t="s">
         <v>175</v>
       </c>
-      <c r="O40" s="1" t="s">
-        <v>22</v>
-      </c>
       <c r="P40" s="1" t="s">
         <v>22</v>
       </c>
@@ -3630,13 +3750,16 @@
         <v>22</v>
       </c>
       <c r="R40" s="1" t="s">
+        <v>22</v>
+      </c>
+      <c r="S40" s="1" t="s">
         <v>156</v>
       </c>
-      <c r="S40" s="1" t="s">
+      <c r="T40" s="1" t="s">
         <v>157</v>
       </c>
     </row>
-    <row r="41" spans="1:19" x14ac:dyDescent="0.25">
+    <row r="41" spans="1:20" x14ac:dyDescent="0.25">
       <c r="A41" s="1" t="s">
         <v>113</v>
       </c>
@@ -3646,42 +3769,42 @@
       <c r="C41" s="1" t="s">
         <v>21</v>
       </c>
-      <c r="D41" s="1" t="s">
+      <c r="D41" s="1">
+        <v>5600</v>
+      </c>
+      <c r="E41" s="1" t="s">
         <v>145</v>
       </c>
-      <c r="E41" s="1" t="s">
+      <c r="F41" s="1" t="s">
         <v>170</v>
       </c>
-      <c r="F41" s="1" t="s">
+      <c r="G41" s="1" t="s">
         <v>147</v>
       </c>
-      <c r="G41" s="1" t="s">
+      <c r="H41" s="1" t="s">
         <v>171</v>
       </c>
-      <c r="H41" s="1" t="s">
+      <c r="I41" s="1" t="s">
         <v>149</v>
       </c>
-      <c r="I41" s="1" t="s">
+      <c r="J41" s="1" t="s">
         <v>150</v>
       </c>
-      <c r="J41" s="1" t="s">
+      <c r="K41" s="1" t="s">
         <v>151</v>
       </c>
-      <c r="K41" s="1" t="s">
+      <c r="L41" s="1" t="s">
         <v>172</v>
       </c>
-      <c r="L41" s="1" t="s">
+      <c r="M41" s="1" t="s">
         <v>177</v>
       </c>
-      <c r="M41" s="1" t="s">
+      <c r="N41" s="1" t="s">
         <v>145</v>
       </c>
-      <c r="N41" s="1" t="s">
+      <c r="O41" s="1" t="s">
         <v>178</v>
       </c>
-      <c r="O41" s="1" t="s">
-        <v>22</v>
-      </c>
       <c r="P41" s="1" t="s">
         <v>22</v>
       </c>
@@ -3689,13 +3812,16 @@
         <v>22</v>
       </c>
       <c r="R41" s="1" t="s">
+        <v>22</v>
+      </c>
+      <c r="S41" s="1" t="s">
         <v>156</v>
       </c>
-      <c r="S41" s="1" t="s">
+      <c r="T41" s="1" t="s">
         <v>157</v>
       </c>
     </row>
-    <row r="42" spans="1:19" x14ac:dyDescent="0.25">
+    <row r="42" spans="1:20" x14ac:dyDescent="0.25">
       <c r="A42" s="1" t="s">
         <v>113</v>
       </c>
@@ -3705,42 +3831,42 @@
       <c r="C42" s="1" t="s">
         <v>21</v>
       </c>
-      <c r="D42" s="1" t="s">
+      <c r="D42" s="1">
+        <v>400</v>
+      </c>
+      <c r="E42" s="1" t="s">
         <v>180</v>
       </c>
-      <c r="E42" s="1" t="s">
+      <c r="F42" s="1" t="s">
         <v>181</v>
       </c>
-      <c r="F42" s="1" t="s">
+      <c r="G42" s="1" t="s">
         <v>182</v>
       </c>
-      <c r="G42" s="1" t="s">
+      <c r="H42" s="1" t="s">
         <v>183</v>
       </c>
-      <c r="H42" s="1" t="s">
+      <c r="I42" s="1" t="s">
         <v>137</v>
       </c>
-      <c r="I42" s="1" t="s">
+      <c r="J42" s="1" t="s">
         <v>184</v>
       </c>
-      <c r="J42" s="1" t="s">
+      <c r="K42" s="1" t="s">
         <v>185</v>
       </c>
-      <c r="K42" s="1" t="s">
+      <c r="L42" s="1" t="s">
         <v>186</v>
       </c>
-      <c r="L42" s="1" t="s">
+      <c r="M42" s="1" t="s">
         <v>187</v>
       </c>
-      <c r="M42" s="1" t="s">
+      <c r="N42" s="1" t="s">
         <v>188</v>
       </c>
-      <c r="N42" s="1" t="s">
+      <c r="O42" s="1" t="s">
         <v>189</v>
       </c>
-      <c r="O42" s="1" t="s">
-        <v>22</v>
-      </c>
       <c r="P42" s="1" t="s">
         <v>22</v>
       </c>
@@ -3748,13 +3874,16 @@
         <v>22</v>
       </c>
       <c r="R42" s="1" t="s">
+        <v>22</v>
+      </c>
+      <c r="S42" s="1" t="s">
         <v>190</v>
       </c>
-      <c r="S42" s="1" t="s">
+      <c r="T42" s="1" t="s">
         <v>191</v>
       </c>
     </row>
-    <row r="43" spans="1:19" x14ac:dyDescent="0.25">
+    <row r="43" spans="1:20" x14ac:dyDescent="0.25">
       <c r="A43" s="1" t="s">
         <v>113</v>
       </c>
@@ -3764,42 +3893,42 @@
       <c r="C43" s="1" t="s">
         <v>21</v>
       </c>
-      <c r="D43" s="1" t="s">
+      <c r="D43" s="1">
+        <v>38</v>
+      </c>
+      <c r="E43" s="1" t="s">
         <v>145</v>
       </c>
-      <c r="E43" s="1" t="s">
+      <c r="F43" s="1" t="s">
         <v>192</v>
       </c>
-      <c r="F43" s="1" t="s">
+      <c r="G43" s="1" t="s">
         <v>147</v>
       </c>
-      <c r="G43" s="1" t="s">
+      <c r="H43" s="1" t="s">
         <v>193</v>
       </c>
-      <c r="H43" s="1" t="s">
+      <c r="I43" s="1" t="s">
         <v>149</v>
       </c>
-      <c r="I43" s="1" t="s">
+      <c r="J43" s="1" t="s">
         <v>150</v>
       </c>
-      <c r="J43" s="1" t="s">
+      <c r="K43" s="1" t="s">
         <v>151</v>
       </c>
-      <c r="K43" s="1" t="s">
+      <c r="L43" s="1" t="s">
         <v>172</v>
       </c>
-      <c r="L43" s="1" t="s">
+      <c r="M43" s="1" t="s">
         <v>194</v>
       </c>
-      <c r="M43" s="1" t="s">
+      <c r="N43" s="1" t="s">
         <v>145</v>
       </c>
-      <c r="N43" s="1" t="s">
+      <c r="O43" s="1" t="s">
         <v>195</v>
       </c>
-      <c r="O43" s="1" t="s">
-        <v>22</v>
-      </c>
       <c r="P43" s="1" t="s">
         <v>22</v>
       </c>
@@ -3807,13 +3936,16 @@
         <v>22</v>
       </c>
       <c r="R43" s="1" t="s">
+        <v>22</v>
+      </c>
+      <c r="S43" s="1" t="s">
         <v>156</v>
       </c>
-      <c r="S43" s="1" t="s">
+      <c r="T43" s="1" t="s">
         <v>157</v>
       </c>
     </row>
-    <row r="44" spans="1:19" x14ac:dyDescent="0.25">
+    <row r="44" spans="1:20" x14ac:dyDescent="0.25">
       <c r="A44" s="1" t="s">
         <v>113</v>
       </c>
@@ -3823,42 +3955,40 @@
       <c r="C44" s="1" t="s">
         <v>21</v>
       </c>
-      <c r="D44" s="1" t="s">
+      <c r="D44" s="1"/>
+      <c r="E44" s="1" t="s">
         <v>115</v>
       </c>
-      <c r="E44" s="1" t="s">
+      <c r="F44" s="1" t="s">
         <v>196</v>
       </c>
-      <c r="F44" s="1" t="s">
+      <c r="G44" s="1" t="s">
         <v>117</v>
       </c>
-      <c r="G44" s="1" t="s">
+      <c r="H44" s="1" t="s">
         <v>197</v>
       </c>
-      <c r="H44" s="1" t="s">
+      <c r="I44" s="1" t="s">
         <v>119</v>
       </c>
-      <c r="I44" s="1" t="s">
+      <c r="J44" s="1" t="s">
         <v>120</v>
       </c>
-      <c r="J44" s="1" t="s">
+      <c r="K44" s="1" t="s">
         <v>121</v>
       </c>
-      <c r="K44" s="1" t="s">
+      <c r="L44" s="1" t="s">
         <v>198</v>
       </c>
-      <c r="L44" s="1" t="s">
+      <c r="M44" s="1" t="s">
         <v>199</v>
       </c>
-      <c r="M44" s="1" t="s">
+      <c r="N44" s="1" t="s">
         <v>200</v>
       </c>
-      <c r="N44" s="1" t="s">
+      <c r="O44" s="1" t="s">
         <v>201</v>
       </c>
-      <c r="O44" s="1" t="s">
-        <v>22</v>
-      </c>
       <c r="P44" s="1" t="s">
         <v>22</v>
       </c>
@@ -3866,13 +3996,16 @@
         <v>22</v>
       </c>
       <c r="R44" s="1" t="s">
+        <v>22</v>
+      </c>
+      <c r="S44" s="1" t="s">
         <v>126</v>
       </c>
-      <c r="S44" s="1" t="s">
+      <c r="T44" s="1" t="s">
         <v>127</v>
       </c>
     </row>
-    <row r="45" spans="1:19" x14ac:dyDescent="0.25">
+    <row r="45" spans="1:20" x14ac:dyDescent="0.25">
       <c r="A45" s="1" t="s">
         <v>113</v>
       </c>
@@ -3882,42 +4015,42 @@
       <c r="C45" s="1" t="s">
         <v>21</v>
       </c>
-      <c r="D45" s="1" t="s">
+      <c r="D45" s="1">
+        <v>6700</v>
+      </c>
+      <c r="E45" s="1" t="s">
         <v>145</v>
       </c>
-      <c r="E45" s="1" t="s">
+      <c r="F45" s="1" t="s">
         <v>202</v>
       </c>
-      <c r="F45" s="1" t="s">
+      <c r="G45" s="1" t="s">
         <v>147</v>
       </c>
-      <c r="G45" s="1" t="s">
+      <c r="H45" s="1" t="s">
         <v>171</v>
       </c>
-      <c r="H45" s="1" t="s">
+      <c r="I45" s="1" t="s">
         <v>149</v>
       </c>
-      <c r="I45" s="1" t="s">
+      <c r="J45" s="1" t="s">
         <v>150</v>
       </c>
-      <c r="J45" s="1" t="s">
+      <c r="K45" s="1" t="s">
         <v>151</v>
       </c>
-      <c r="K45" s="1" t="s">
+      <c r="L45" s="1" t="s">
         <v>143</v>
       </c>
-      <c r="L45" s="1" t="s">
+      <c r="M45" s="1" t="s">
         <v>203</v>
       </c>
-      <c r="M45" s="1" t="s">
+      <c r="N45" s="1" t="s">
         <v>204</v>
       </c>
-      <c r="N45" s="1" t="s">
+      <c r="O45" s="1" t="s">
         <v>205</v>
       </c>
-      <c r="O45" s="1" t="s">
-        <v>22</v>
-      </c>
       <c r="P45" s="1" t="s">
         <v>22</v>
       </c>
@@ -3925,13 +4058,16 @@
         <v>22</v>
       </c>
       <c r="R45" s="1" t="s">
+        <v>22</v>
+      </c>
+      <c r="S45" s="1" t="s">
         <v>156</v>
       </c>
-      <c r="S45" s="1" t="s">
+      <c r="T45" s="1" t="s">
         <v>157</v>
       </c>
     </row>
-    <row r="46" spans="1:19" x14ac:dyDescent="0.25">
+    <row r="46" spans="1:20" x14ac:dyDescent="0.25">
       <c r="A46" s="1" t="s">
         <v>113</v>
       </c>
@@ -3941,42 +4077,42 @@
       <c r="C46" s="1" t="s">
         <v>21</v>
       </c>
-      <c r="D46" s="1" t="s">
+      <c r="D46" s="1">
+        <v>23000</v>
+      </c>
+      <c r="E46" s="1" t="s">
         <v>145</v>
       </c>
-      <c r="E46" s="1" t="s">
+      <c r="F46" s="1" t="s">
         <v>170</v>
       </c>
-      <c r="F46" s="1" t="s">
+      <c r="G46" s="1" t="s">
         <v>147</v>
       </c>
-      <c r="G46" s="1" t="s">
+      <c r="H46" s="1" t="s">
         <v>171</v>
       </c>
-      <c r="H46" s="1" t="s">
+      <c r="I46" s="1" t="s">
         <v>149</v>
       </c>
-      <c r="I46" s="1" t="s">
+      <c r="J46" s="1" t="s">
         <v>150</v>
       </c>
-      <c r="J46" s="1" t="s">
+      <c r="K46" s="1" t="s">
         <v>151</v>
       </c>
-      <c r="K46" s="1" t="s">
+      <c r="L46" s="1" t="s">
         <v>172</v>
       </c>
-      <c r="L46" s="1" t="s">
+      <c r="M46" s="1" t="s">
         <v>207</v>
       </c>
-      <c r="M46" s="1" t="s">
+      <c r="N46" s="1" t="s">
         <v>145</v>
       </c>
-      <c r="N46" s="1" t="s">
+      <c r="O46" s="1" t="s">
         <v>208</v>
       </c>
-      <c r="O46" s="1" t="s">
-        <v>22</v>
-      </c>
       <c r="P46" s="1" t="s">
         <v>22</v>
       </c>
@@ -3984,13 +4120,16 @@
         <v>22</v>
       </c>
       <c r="R46" s="1" t="s">
+        <v>22</v>
+      </c>
+      <c r="S46" s="1" t="s">
         <v>156</v>
       </c>
-      <c r="S46" s="1" t="s">
+      <c r="T46" s="1" t="s">
         <v>157</v>
       </c>
     </row>
-    <row r="47" spans="1:19" x14ac:dyDescent="0.25">
+    <row r="47" spans="1:20" x14ac:dyDescent="0.25">
       <c r="A47" s="1" t="s">
         <v>113</v>
       </c>
@@ -4000,42 +4139,40 @@
       <c r="C47" s="1" t="s">
         <v>21</v>
       </c>
-      <c r="D47" s="1" t="s">
+      <c r="D47" s="1"/>
+      <c r="E47" s="1" t="s">
         <v>145</v>
       </c>
-      <c r="E47" s="1" t="s">
+      <c r="F47" s="1" t="s">
         <v>209</v>
       </c>
-      <c r="F47" s="1" t="s">
+      <c r="G47" s="1" t="s">
         <v>147</v>
       </c>
-      <c r="G47" s="1" t="s">
+      <c r="H47" s="1" t="s">
         <v>171</v>
       </c>
-      <c r="H47" s="1" t="s">
+      <c r="I47" s="1" t="s">
         <v>149</v>
       </c>
-      <c r="I47" s="1" t="s">
+      <c r="J47" s="1" t="s">
         <v>150</v>
       </c>
-      <c r="J47" s="1" t="s">
+      <c r="K47" s="1" t="s">
         <v>151</v>
       </c>
-      <c r="K47" s="1" t="s">
+      <c r="L47" s="1" t="s">
         <v>210</v>
       </c>
-      <c r="L47" s="1" t="s">
+      <c r="M47" s="1" t="s">
         <v>211</v>
       </c>
-      <c r="M47" s="1" t="s">
+      <c r="N47" s="1" t="s">
         <v>212</v>
       </c>
-      <c r="N47" s="1" t="s">
+      <c r="O47" s="1" t="s">
         <v>213</v>
       </c>
-      <c r="O47" s="1" t="s">
-        <v>22</v>
-      </c>
       <c r="P47" s="1" t="s">
         <v>22</v>
       </c>
@@ -4043,13 +4180,16 @@
         <v>22</v>
       </c>
       <c r="R47" s="1" t="s">
+        <v>22</v>
+      </c>
+      <c r="S47" s="1" t="s">
         <v>156</v>
       </c>
-      <c r="S47" s="1" t="s">
+      <c r="T47" s="1" t="s">
         <v>157</v>
       </c>
     </row>
-    <row r="48" spans="1:19" x14ac:dyDescent="0.25">
+    <row r="48" spans="1:20" x14ac:dyDescent="0.25">
       <c r="A48" s="1" t="s">
         <v>113</v>
       </c>
@@ -4059,42 +4199,42 @@
       <c r="C48" s="1" t="s">
         <v>21</v>
       </c>
-      <c r="D48" s="1" t="s">
+      <c r="D48" s="1">
+        <v>42000</v>
+      </c>
+      <c r="E48" s="1" t="s">
         <v>145</v>
       </c>
-      <c r="E48" s="1" t="s">
+      <c r="F48" s="1" t="s">
         <v>170</v>
       </c>
-      <c r="F48" s="1" t="s">
+      <c r="G48" s="1" t="s">
         <v>147</v>
       </c>
-      <c r="G48" s="1" t="s">
+      <c r="H48" s="1" t="s">
         <v>171</v>
       </c>
-      <c r="H48" s="1" t="s">
+      <c r="I48" s="1" t="s">
         <v>149</v>
       </c>
-      <c r="I48" s="1" t="s">
+      <c r="J48" s="1" t="s">
         <v>150</v>
       </c>
-      <c r="J48" s="1" t="s">
+      <c r="K48" s="1" t="s">
         <v>151</v>
       </c>
-      <c r="K48" s="1" t="s">
+      <c r="L48" s="1" t="s">
         <v>172</v>
       </c>
-      <c r="L48" s="1" t="s">
+      <c r="M48" s="1" t="s">
         <v>215</v>
       </c>
-      <c r="M48" s="1" t="s">
+      <c r="N48" s="1" t="s">
         <v>145</v>
       </c>
-      <c r="N48" s="1" t="s">
+      <c r="O48" s="1" t="s">
         <v>208</v>
       </c>
-      <c r="O48" s="1" t="s">
-        <v>22</v>
-      </c>
       <c r="P48" s="1" t="s">
         <v>22</v>
       </c>
@@ -4102,13 +4242,16 @@
         <v>22</v>
       </c>
       <c r="R48" s="1" t="s">
+        <v>22</v>
+      </c>
+      <c r="S48" s="1" t="s">
         <v>156</v>
       </c>
-      <c r="S48" s="1" t="s">
+      <c r="T48" s="1" t="s">
         <v>157</v>
       </c>
     </row>
-    <row r="49" spans="1:19" x14ac:dyDescent="0.25">
+    <row r="49" spans="1:20" x14ac:dyDescent="0.25">
       <c r="A49" s="1" t="s">
         <v>113</v>
       </c>
@@ -4118,42 +4261,42 @@
       <c r="C49" s="1" t="s">
         <v>21</v>
       </c>
-      <c r="D49" s="1" t="s">
+      <c r="D49" s="1">
+        <v>11000</v>
+      </c>
+      <c r="E49" s="1" t="s">
         <v>145</v>
       </c>
-      <c r="E49" s="1" t="s">
+      <c r="F49" s="1" t="s">
         <v>170</v>
       </c>
-      <c r="F49" s="1" t="s">
+      <c r="G49" s="1" t="s">
         <v>147</v>
       </c>
-      <c r="G49" s="1" t="s">
+      <c r="H49" s="1" t="s">
         <v>171</v>
       </c>
-      <c r="H49" s="1" t="s">
+      <c r="I49" s="1" t="s">
         <v>149</v>
       </c>
-      <c r="I49" s="1" t="s">
+      <c r="J49" s="1" t="s">
         <v>150</v>
       </c>
-      <c r="J49" s="1" t="s">
+      <c r="K49" s="1" t="s">
         <v>151</v>
       </c>
-      <c r="K49" s="1" t="s">
+      <c r="L49" s="1" t="s">
         <v>172</v>
       </c>
-      <c r="L49" s="1" t="s">
+      <c r="M49" s="1" t="s">
         <v>207</v>
       </c>
-      <c r="M49" s="1" t="s">
+      <c r="N49" s="1" t="s">
         <v>145</v>
       </c>
-      <c r="N49" s="1" t="s">
+      <c r="O49" s="1" t="s">
         <v>208</v>
       </c>
-      <c r="O49" s="1" t="s">
-        <v>22</v>
-      </c>
       <c r="P49" s="1" t="s">
         <v>22</v>
       </c>
@@ -4161,9 +4304,12 @@
         <v>22</v>
       </c>
       <c r="R49" s="1" t="s">
+        <v>22</v>
+      </c>
+      <c r="S49" s="1" t="s">
         <v>156</v>
       </c>
-      <c r="S49" s="1" t="s">
+      <c r="T49" s="1" t="s">
         <v>157</v>
       </c>
     </row>
@@ -4172,7 +4318,7 @@
   <mergeCells count="3">
     <mergeCell ref="A2:B2"/>
     <mergeCell ref="A3:B3"/>
-    <mergeCell ref="A1:F1"/>
+    <mergeCell ref="A1:G1"/>
   </mergeCells>
   <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
   <drawing r:id="rId1"/>

</xml_diff>